<commit_message>
🔄 Actualización automática del mapa (2025-07-18 14:01:51)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P93"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2318,7 +2318,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>803608455</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2328,17 +2328,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>VALDENEGRO /ALT/ 4037</t>
+          <t>COCHABAMBA /ALT/ 1790</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>803608455</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambiar poste podrido apoyado en tanque de agua. Es sobre parque junto a medianera.  Dar prioridad .</t>
+          <t>SIN RIEGO</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2366,55 +2366,55 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.493679</v>
+        <v>-58.391153</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.557149</v>
+        <v>-34.624022</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>-281</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>COCHABAMBA /ALT/ 1790</t>
+          <t>SOLER /ALT/ 4517</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>803651203</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>SIN RIEGO</t>
+          <t>columna de 114 con nodo y redes nuestra.</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2451,14 +2451,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.391153</v>
+        <v>-58.423405</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.624022</v>
+        <v>-34.588075</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2470,17 +2470,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-281</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>SOLER /ALT/ 4517</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2490,7 +2490,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803651203</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>columna de 114 con nodo y redes nuestra.</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2518,19 +2518,19 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.423405</v>
+        <v>-58.42486</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.588075</v>
+        <v>-34.577318</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2546,27 +2546,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>-316</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>4/3/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>ALBERTI /ALT/ 621</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804468365</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2599,18 +2599,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.42486</v>
+        <v>-58.401202</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.577318</v>
+        <v>-34.61683</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2622,27 +2622,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-316</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/3/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ALBERTI /ALT/ 621</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804468365</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2657,7 +2657,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2670,7 +2670,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2679,26 +2679,26 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.401202</v>
+        <v>-58.491074</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.61683</v>
+        <v>-34.575623</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-326</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2708,17 +2708,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GARCIA DEL RIO /ALT/ 3354</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804634199</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2733,7 +2733,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Retirar poste de vereda. Reparar la vereda donde estaba colocado el poste.</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2751,18 +2751,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.478106</v>
+        <v>-58.525125</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.551523</v>
+        <v>-34.604668</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2774,27 +2774,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>-336</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>BAUNESS /ALT/ 1419</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804838856</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>"Aplomar columna 114 con rienda a pique o colocar terminal"</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2831,10 +2831,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.491074</v>
+        <v>-58.479168</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.575623</v>
+        <v>-34.584482</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2850,27 +2850,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2907,26 +2907,26 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.525125</v>
+        <v>-58.421964</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.604668</v>
+        <v>-34.586342</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-336</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2936,17 +2936,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>BAUNESS /ALT/ 1419</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804838856</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>"Aplomar columna 114 con rienda a pique o colocar terminal"</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2983,10 +2983,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.479168</v>
+        <v>-58.498493</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.584482</v>
+        <v>-34.581262</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3002,7 +3002,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-340</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3012,17 +3012,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>SUPERI /ALT/ 1445</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804838869</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3059,36 +3059,36 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.421964</v>
+        <v>-58.460666</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.586342</v>
+        <v>-34.573823</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3113,15 +3113,15 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3135,10 +3135,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.498493</v>
+        <v>-58.502447</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.581262</v>
+        <v>-34.561008</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3154,27 +3154,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-340</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SUPERI /ALT/ 1445</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804838869</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3189,15 +3189,15 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3211,14 +3211,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.460666</v>
+        <v>-58.483947</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.573823</v>
+        <v>-34.583207</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3230,27 +3230,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-341</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO /ALT/ 4835</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804838980</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3265,15 +3265,15 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>"Retirar poste teco cobre en desuso entrada Edificio reclamo municipal "</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3287,14 +3287,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.469157</v>
+        <v>-58.503673</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.536783</v>
+        <v>-34.586925</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3306,7 +3306,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-347</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3316,17 +3316,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>AVALOS /ALT/ 1610</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804839214</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t>Cambiar columna de 168 - VIRARDI</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente TLC</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3363,10 +3363,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.502447</v>
+        <v>-58.480099</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.561008</v>
+        <v>-34.582085</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3382,7 +3382,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-353</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3392,17 +3392,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>CAAGUAZU /ALT/ 5703</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839589</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar columna de 114. Fuera de plomo empotrada en árbol colocar rienda. ( se pasa tareas a contratista tratista de limpieza tensado y elevación del tendido).  - VIRARDI</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3439,14 +3439,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.483947</v>
+        <v>-58.511462</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.583207</v>
+        <v>-34.640542</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3458,7 +3458,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3468,7 +3468,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3478,7 +3478,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3511,14 +3511,14 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.503673</v>
+        <v>-58.504455</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.586925</v>
+        <v>-34.579941</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3534,7 +3534,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-347</t>
+          <t>-355</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3544,17 +3544,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>AVALOS /ALT/ 1610</t>
+          <t>CUENCA /ALT/ 4480</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804839214</t>
+          <t>804839675</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Cambiar columna de 168 - VIRARDI</t>
+          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3591,10 +3591,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.480099</v>
+        <v>-58.504568</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.582085</v>
+        <v>-34.590534</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3610,7 +3610,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-353</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3620,17 +3620,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CAAGUAZU /ALT/ 5703</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804839589</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. Fuera de plomo empotrada en árbol colocar rienda. ( se pasa tareas a contratista tratista de limpieza tensado y elevación del tendido).  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3667,14 +3667,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.511462</v>
+        <v>-58.503195</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.640542</v>
+        <v>-34.581735</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3686,7 +3686,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-363</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3696,17 +3696,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>OSLO /ALT/ 1255</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839962</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Cambiar columna de 168 podrida en su base.  - VIRARDI</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3743,10 +3743,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.504455</v>
+        <v>-58.481767</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.579941</v>
+        <v>-34.589507</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-355</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 4480</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3782,7 +3782,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804839675</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3810,7 +3810,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3819,14 +3819,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.504568</v>
+        <v>-58.493164</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.590534</v>
+        <v>-34.55732</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3838,7 +3838,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3895,10 +3895,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.503195</v>
+        <v>-58.491934</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.581735</v>
+        <v>-34.569348</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3914,7 +3914,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-363</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3924,17 +3924,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>OSLO /ALT/ 1255</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804839962</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar columna de 168 podrida en su base.  - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3971,10 +3971,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.481767</v>
+        <v>-58.501418</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.589507</v>
+        <v>-34.574363</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3990,7 +3990,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4010,7 +4010,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4025,7 +4025,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4047,10 +4047,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.493164</v>
+        <v>-58.494584</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.55732</v>
+        <v>-34.554981</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4066,27 +4066,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4101,15 +4101,15 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4119,18 +4119,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.491934</v>
+        <v>-58.465608</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.569348</v>
+        <v>-34.538489</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4142,27 +4142,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4177,15 +4177,15 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4199,10 +4199,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.501418</v>
+        <v>-58.436788</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.574363</v>
+        <v>-34.604014</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4218,27 +4218,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4253,11 +4253,11 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -4275,46 +4275,46 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.494584</v>
+        <v>-58.439461</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.554981</v>
+        <v>-34.605744</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-375</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>PAVON /ALT/ 3335</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903824</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Colocar columna nueva donde estaba la anterior cortada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4347,30 +4347,30 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.465608</v>
+        <v>-58.412418</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.538489</v>
+        <v>-34.629288</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4380,17 +4380,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4405,7 +4405,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4427,26 +4427,26 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.436788</v>
+        <v>-58.418424</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.604014</v>
+        <v>-34.604463</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-377</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4456,17 +4456,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>HUMAHUACA /ALT/ 3918</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903788</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4503,10 +4503,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.439461</v>
+        <v>-58.419694</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.605744</v>
+        <v>-34.602062</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4522,27 +4522,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-375</t>
+          <t>-383</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>PAVON /ALT/ 3335</t>
+          <t>VALDERRAMA /ALT/ 4187</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>804903824</t>
+          <t>805507401</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Colocar columna nueva donde estaba la anterior cortada</t>
+          <t xml:space="preserve">Aplomar columna 114 </t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4579,46 +4579,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.412418</v>
+        <v>-58.481834</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.629288</v>
+        <v>-34.560796</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4655,46 +4655,46 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.418424</v>
+        <v>-58.473936</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.604463</v>
+        <v>-34.577346</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-377</t>
+          <t>-385</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>HUMAHUACA /ALT/ 3918</t>
+          <t>MOLDES /ALT/ 1913</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>804903788</t>
+          <t>805507415</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4731,26 +4731,26 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.419694</v>
+        <v>-58.45789</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.602062</v>
+        <v>-34.565423</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-383</t>
+          <t>-386</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4760,17 +4760,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>VALDERRAMA /ALT/ 4187</t>
+          <t>MOLDES /ALT/ 1943</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>805507401</t>
+          <t>805507419</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114 </t>
+          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4798,7 +4798,7 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
@@ -4807,14 +4807,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.481834</v>
+        <v>-58.458217</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.560796</v>
+        <v>-34.565043</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4826,27 +4826,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-391</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>IBERA /ALT/ 5074</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805676610</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4883,14 +4883,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.473936</v>
+        <v>-58.49045</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.577346</v>
+        <v>-34.566894</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4902,27 +4902,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-385</t>
+          <t>-392</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1913</t>
+          <t>GARCIA TEODORO /ALT/ 1775</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>805507415</t>
+          <t>805676615</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4959,10 +4959,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.45789</v>
+        <v>-58.440367</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.565423</v>
+        <v>-34.563551</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4978,27 +4978,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-386</t>
+          <t>-393</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1943</t>
+          <t>3 DE FEBRERO /ALT/ 1272</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>805507419</t>
+          <t>805676618</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5021,12 +5021,12 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -5035,10 +5035,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.458217</v>
+        <v>-58.445186</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.565043</v>
+        <v>-34.567417</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5054,27 +5054,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-391</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>IBERA /ALT/ 5074</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>805676610</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5089,7 +5089,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5111,46 +5111,46 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.49045</v>
+        <v>-58.387847</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.566894</v>
+        <v>-34.587043</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-392</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>GARCIA TEODORO /ALT/ 1775</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>805676615</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5165,7 +5165,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5187,14 +5187,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.440367</v>
+        <v>-58.46579</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.563551</v>
+        <v>-34.555012</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5206,27 +5206,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-393</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO /ALT/ 1272</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>805676618</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5241,7 +5241,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5263,10 +5263,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.445186</v>
+        <v>-58.451835</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.567417</v>
+        <v>-34.562646</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5282,27 +5282,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5317,7 +5317,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5325,7 +5325,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5335,50 +5335,50 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.387847</v>
+        <v>-58.488252</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.587043</v>
+        <v>-34.553391</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-403</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SUCRE MRCAL A J DE /ALT/ 3515</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>805722878</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t xml:space="preserve">Retirar poste teco cobre tirado y reparar vereda </t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5411,18 +5411,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.466241</v>
+        <v>-58.470837</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.57047</v>
+        <v>-34.545751</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5434,7 +5434,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5444,17 +5444,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5482,7 +5482,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -5491,10 +5491,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.46579</v>
+        <v>-58.472267</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.555012</v>
+        <v>-34.551163</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5510,17 +5510,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5567,14 +5567,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.451835</v>
+        <v>-58.464144</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.562646</v>
+        <v>-34.541832</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5586,27 +5586,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5629,7 +5629,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5639,50 +5639,50 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.488252</v>
+        <v>-58.434761</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.553391</v>
+        <v>-34.598381</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5697,7 +5697,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5705,7 +5705,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5715,14 +5715,14 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.470837</v>
+        <v>-58.464177</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.545751</v>
+        <v>-34.558239</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5738,27 +5738,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5773,7 +5773,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5781,12 +5781,12 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5795,46 +5795,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.472267</v>
+        <v>-58.412302</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.551163</v>
+        <v>-34.59301</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5849,11 +5849,11 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -5871,10 +5871,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.464144</v>
+        <v>-58.485056</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.541832</v>
+        <v>-34.555059</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5890,27 +5890,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-425</t>
+          <t>-450</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Av. Eva Peron 7437</t>
+          <t>Moldes 2325</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>806926621</t>
+          <t>807044059</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5925,7 +5925,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar columna de 114</t>
+          <t xml:space="preserve">Corroida en base para cambiar contiene CDO/NAP propio </t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5947,14 +5947,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.501029</v>
+        <v>-58.461167</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.673558</v>
+        <v>-34.561613</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5966,27 +5966,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-426</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Av. Eva Peron 7471</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>806926647</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6001,7 +6001,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 con rienda</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6009,7 +6009,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6019,18 +6019,18 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.501565</v>
+        <v>-58.49147</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.673845</v>
+        <v>-34.55031</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6042,27 +6042,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6075,11 +6075,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
-        </is>
-      </c>
+      <c r="H75" t="inlineStr"/>
       <c r="I75" t="n">
         <v>1</v>
       </c>
@@ -6099,14 +6095,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.434761</v>
+        <v>-58.405761</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.598381</v>
+        <v>-34.582476</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6118,27 +6114,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-432</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ALVAREZ JULIAN 618</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>806926759</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6153,7 +6149,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Columna con base corroida sin riesgo de caida al 14/05/2025</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6175,10 +6171,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.433867</v>
+        <v>-58.432241</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.599149</v>
+        <v>-34.56642</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6194,27 +6190,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6229,7 +6225,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6247,50 +6243,50 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.464177</v>
+        <v>-58.417348</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.558239</v>
+        <v>-34.595467</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6305,7 +6301,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6323,18 +6319,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.412302</v>
+        <v>-58.472311</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.59301</v>
+        <v>-34.654867</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6346,27 +6342,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6381,11 +6377,11 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -6403,14 +6399,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.485056</v>
+        <v>-58.450113</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.555059</v>
+        <v>-34.574534</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6422,27 +6418,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-450</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Moldes 2325</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>807044059</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6457,7 +6453,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Corroida en base para cambiar contiene CDO/NAP propio </t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6475,18 +6471,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.461167</v>
+        <v>-58.484729</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.561613</v>
+        <v>-34.574614</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6498,27 +6494,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-491</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>3 de Febrero 2171</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6533,7 +6529,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Columna 114 propia picada en base con NAP</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6555,10 +6551,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.49147</v>
+        <v>-58.452636</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.55031</v>
+        <v>-34.558607</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6574,27 +6570,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6607,13 +6603,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H82" t="inlineStr"/>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Poste inclinado</t>
+        </is>
+      </c>
       <c r="I82" t="n">
         <v>1</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -6623,50 +6623,50 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.405761</v>
+        <v>-58.510247</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.582476</v>
+        <v>-34.645038</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>6410</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>BEAUCHEF 421</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>808373658</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6703,14 +6703,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.432241</v>
+        <v>-58.433724</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.56642</v>
+        <v>-34.621643</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6722,27 +6722,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-518</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6757,7 +6757,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6779,46 +6779,46 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.417348</v>
+        <v>-58.483145</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.595467</v>
+        <v>-34.557043</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6454</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/18/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>HABANA 3382</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>808413466</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6833,7 +6833,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6851,50 +6851,50 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.472311</v>
+        <v>-58.505747</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.654867</v>
+        <v>-34.593173</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>6457</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/18/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>BATLLE Y ORDOÑEZ, JOSE P.T. 4659</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>808413477</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6931,551 +6931,19 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.450113</v>
+        <v>-58.464657</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.574534</v>
+        <v>-34.670556</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>-488</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Blanco Encalada 4896</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>807763099</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M87" t="n">
-        <v>-58.484729</v>
-      </c>
-      <c r="N87" t="n">
-        <v>-34.574614</v>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>-491</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>6/26/2025</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>3 de Febrero 2171</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>807789702</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Columna 114 propia picada en base con NAP</t>
-        </is>
-      </c>
-      <c r="I88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M88" t="n">
-        <v>-58.452636</v>
-      </c>
-      <c r="N88" t="n">
-        <v>-34.558607</v>
-      </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P88" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>6399</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>7/14/2025</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>ESCALADA AV. 966</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>808258198</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M89" t="n">
-        <v>-58.493069</v>
-      </c>
-      <c r="N89" t="n">
-        <v>-34.646557</v>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>-515</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Rivadavia 7470</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>808263485</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I90" t="n">
-        <v>1</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M90" t="n">
-        <v>-58.470715</v>
-      </c>
-      <c r="N90" t="n">
-        <v>-34.631107</v>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P90" t="inlineStr">
-        <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>6398</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>LARRAZABAL AV. 579</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>808373655</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Poste inclinado</t>
-        </is>
-      </c>
-      <c r="I91" t="n">
-        <v>1</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M91" t="n">
-        <v>-58.510247</v>
-      </c>
-      <c r="N91" t="n">
-        <v>-34.645038</v>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P91" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>6410</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>BEAUCHEF 421</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>808373658</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M92" t="n">
-        <v>-58.433724</v>
-      </c>
-      <c r="N92" t="n">
-        <v>-34.621643</v>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P92" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>-518</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>7/16/2025</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Crisologo Larralde 4073</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>808373627</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>Cambiar columna corroída en base</t>
-        </is>
-      </c>
-      <c r="I93" t="n">
-        <v>1</v>
-      </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M93" t="n">
-        <v>-58.483145</v>
-      </c>
-      <c r="N93" t="n">
-        <v>-34.557043</v>
-      </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P93" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-21 07:30:51)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6947,6 +6947,78 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>-521</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>7/21/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Gregario Laferrere 6572</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>808430950</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 12:17:08)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -3458,7 +3458,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-347</t>
+          <t>-353</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3468,17 +3468,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>AVALOS /ALT/ 1610</t>
+          <t>CAAGUAZU /ALT/ 5703</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804839214</t>
+          <t>804839589</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Cambiar columna de 168 - VIRARDI</t>
+          <t>Cambiar columna de 114. Fuera de plomo empotrada en árbol colocar rienda. ( se pasa tareas a contratista tratista de limpieza tensado y elevación del tendido).  - VIRARDI</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3515,14 +3515,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.480099</v>
+        <v>-58.511462</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.582085</v>
+        <v>-34.640542</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3534,7 +3534,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-353</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3544,17 +3544,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CAAGUAZU /ALT/ 5703</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804839589</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. Fuera de plomo empotrada en árbol colocar rienda. ( se pasa tareas a contratista tratista de limpieza tensado y elevación del tendido).  - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3591,14 +3591,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.511462</v>
+        <v>-58.504455</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.640542</v>
+        <v>-34.579941</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3610,7 +3610,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-355</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3620,7 +3620,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>CUENCA /ALT/ 4480</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3630,7 +3630,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839675</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente TLC</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3667,10 +3667,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.504455</v>
+        <v>-58.504568</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.579941</v>
+        <v>-34.590534</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3686,7 +3686,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-355</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3696,7 +3696,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 4480</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3706,7 +3706,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804839675</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3743,10 +3743,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.504568</v>
+        <v>-58.503195</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.590534</v>
+        <v>-34.581735</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-363</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3772,17 +3772,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>OSLO /ALT/ 1255</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839962</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Cambiar columna de 168 podrida en su base.  - VIRARDI</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3819,10 +3819,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.503195</v>
+        <v>-58.481767</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.581735</v>
+        <v>-34.589507</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-363</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3848,17 +3848,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>OSLO /ALT/ 1255</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804839962</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna de 168 podrida en su base.  - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3895,14 +3895,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.481767</v>
+        <v>-58.493164</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.589507</v>
+        <v>-34.55732</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3914,7 +3914,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3934,7 +3934,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3971,14 +3971,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.493164</v>
+        <v>-58.491934</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.55732</v>
+        <v>-34.569348</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3990,7 +3990,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4010,7 +4010,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4025,7 +4025,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4047,10 +4047,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.491934</v>
+        <v>-58.501418</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.569348</v>
+        <v>-34.574363</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4066,7 +4066,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4076,7 +4076,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4123,14 +4123,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.501418</v>
+        <v>-58.494584</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.574363</v>
+        <v>-34.554981</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4142,27 +4142,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4177,11 +4177,11 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4195,14 +4195,14 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.494584</v>
+        <v>-58.465608</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.554981</v>
+        <v>-34.538489</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4218,27 +4218,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4271,18 +4271,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.465608</v>
+        <v>-58.436788</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.538489</v>
+        <v>-34.604014</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4294,7 +4294,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4304,17 +4304,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4351,26 +4351,26 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.436788</v>
+        <v>-58.439461</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.604014</v>
+        <v>-34.605744</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-375</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4380,17 +4380,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>PAVON /ALT/ 3335</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903824</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4405,7 +4405,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Colocar columna nueva donde estaba la anterior cortada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4427,14 +4427,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.439461</v>
+        <v>-58.412418</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.605744</v>
+        <v>-34.629288</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4446,7 +4446,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-375</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4456,7 +4456,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>PAVON /ALT/ 3335</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4466,7 +4466,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>804903824</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Colocar columna nueva donde estaba la anterior cortada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4503,14 +4503,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.412418</v>
+        <v>-58.418424</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.629288</v>
+        <v>-34.604463</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>-377</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4532,7 +4532,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>HUMAHUACA /ALT/ 3918</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4542,7 +4542,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>804903788</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4579,10 +4579,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.418424</v>
+        <v>-58.419694</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.604463</v>
+        <v>-34.602062</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4598,27 +4598,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-377</t>
+          <t>-383</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>HUMAHUACA /ALT/ 3918</t>
+          <t>VALDERRAMA /ALT/ 4187</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>804903788</t>
+          <t>805507401</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t xml:space="preserve">Aplomar columna 114 </t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4655,26 +4655,26 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.419694</v>
+        <v>-58.481834</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.602062</v>
+        <v>-34.560796</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-383</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4684,17 +4684,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>VALDERRAMA /ALT/ 4187</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>805507401</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114 </t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4731,14 +4731,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.481834</v>
+        <v>-58.473936</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.560796</v>
+        <v>-34.577346</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4750,7 +4750,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-385</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4760,17 +4760,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>MOLDES /ALT/ 1913</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805507415</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4807,10 +4807,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.473936</v>
+        <v>-58.45789</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.577346</v>
+        <v>-34.565423</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4826,7 +4826,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-385</t>
+          <t>-386</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1913</t>
+          <t>MOLDES /ALT/ 1943</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4846,7 +4846,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>805507415</t>
+          <t>805507419</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4874,7 +4874,7 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
@@ -4883,10 +4883,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.45789</v>
+        <v>-58.458217</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.565423</v>
+        <v>-34.565043</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4902,27 +4902,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-386</t>
+          <t>-391</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1943</t>
+          <t>IBERA /ALT/ 5074</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>805507419</t>
+          <t>805676610</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4945,12 +4945,12 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
@@ -4959,14 +4959,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.458217</v>
+        <v>-58.49045</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.565043</v>
+        <v>-34.566894</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4978,7 +4978,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-391</t>
+          <t>-392</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4988,17 +4988,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>IBERA /ALT/ 5074</t>
+          <t>GARCIA TEODORO /ALT/ 1775</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>805676610</t>
+          <t>805676615</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5035,14 +5035,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.49045</v>
+        <v>-58.440367</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.566894</v>
+        <v>-34.563551</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5054,7 +5054,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-392</t>
+          <t>-393</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5064,7 +5064,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>GARCIA TEODORO /ALT/ 1775</t>
+          <t>3 DE FEBRERO /ALT/ 1272</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5074,7 +5074,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>805676615</t>
+          <t>805676618</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5111,10 +5111,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.440367</v>
+        <v>-58.445186</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.563551</v>
+        <v>-34.567417</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5130,27 +5130,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-393</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO /ALT/ 1272</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>805676618</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5165,7 +5165,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5187,46 +5187,46 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.445186</v>
+        <v>-58.387847</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.567417</v>
+        <v>-34.587043</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5241,7 +5241,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5263,26 +5263,26 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.387847</v>
+        <v>-58.46579</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.587043</v>
+        <v>-34.555012</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5292,7 +5292,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5302,7 +5302,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5317,7 +5317,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5325,7 +5325,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5339,14 +5339,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.46579</v>
+        <v>-58.451835</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.555012</v>
+        <v>-34.562646</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5358,7 +5358,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5368,17 +5368,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5411,18 +5411,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.451835</v>
+        <v>-58.488252</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.562646</v>
+        <v>-34.553391</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5434,7 +5434,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5454,7 +5454,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5469,7 +5469,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5477,7 +5477,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5491,10 +5491,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.488252</v>
+        <v>-58.470837</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.553391</v>
+        <v>-34.545751</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5510,7 +5510,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5520,7 +5520,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5558,19 +5558,19 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5586,27 +5586,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5629,12 +5629,12 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5643,10 +5643,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -5662,7 +5662,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5672,17 +5672,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5697,7 +5697,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5719,26 +5719,26 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5748,17 +5748,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5773,7 +5773,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5791,30 +5791,30 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5824,17 +5824,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5867,50 +5867,50 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5925,11 +5925,11 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -5947,46 +5947,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.412302</v>
+        <v>-58.485056</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.59301</v>
+        <v>-34.555059</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>-450</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Moldes 2325</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807044059</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6001,11 +6001,11 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t xml:space="preserve">Corroida en base para cambiar contiene CDO/NAP propio </t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -6023,10 +6023,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.485056</v>
+        <v>-58.461167</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.555059</v>
+        <v>-34.561613</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6042,27 +6042,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-450</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Moldes 2325</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807044059</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Corroida en base para cambiar contiene CDO/NAP propio </t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6099,10 +6099,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.461167</v>
+        <v>-58.49147</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.561613</v>
+        <v>-34.55031</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6118,27 +6118,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6151,11 +6151,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H76" t="inlineStr"/>
       <c r="I76" t="n">
         <v>1</v>
       </c>
@@ -6175,36 +6171,36 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.49147</v>
+        <v>-58.405761</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.55031</v>
+        <v>-34.582476</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6214,7 +6210,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6227,7 +6223,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr"/>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I77" t="n">
         <v>1</v>
       </c>
@@ -6247,14 +6247,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6266,7 +6266,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6276,7 +6276,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6286,7 +6286,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6323,10 +6323,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6342,27 +6342,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6377,7 +6377,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6395,18 +6395,18 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6418,7 +6418,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6428,17 +6428,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6453,7 +6453,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6471,30 +6471,30 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.472311</v>
+        <v>-58.450113</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.654867</v>
+        <v>-34.574534</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6504,17 +6504,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6547,18 +6547,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.450113</v>
+        <v>-58.484729</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.574534</v>
+        <v>-34.574614</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6570,27 +6570,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>-491</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>3 de Febrero 2171</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Columna 114 propia picada en base con NAP</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6623,18 +6623,18 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.484729</v>
+        <v>-58.452636</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.574614</v>
+        <v>-34.558607</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6646,27 +6646,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-491</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>3 de Febrero 2171</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6681,7 +6681,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Columna 114 propia picada en base con NAP</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6699,18 +6699,18 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.452636</v>
+        <v>-58.510247</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.558607</v>
+        <v>-34.645038</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6722,7 +6722,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6410</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6732,17 +6732,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>BEAUCHEF 421</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373658</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6757,7 +6757,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6775,50 +6775,50 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.510247</v>
+        <v>-58.433724</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.645038</v>
+        <v>-34.621643</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>6410</t>
+          <t>-518</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>BEAUCHEF 421</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808373658</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6833,7 +6833,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6855,46 +6855,46 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.433724</v>
+        <v>-58.483145</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.621643</v>
+        <v>-34.557043</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>-518</t>
+          <t>6454</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/18/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>HABANA 3382</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808413466</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6931,14 +6931,14 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.483145</v>
+        <v>-58.505747</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.557043</v>
+        <v>-34.593173</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6950,7 +6950,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>6454</t>
+          <t>6457</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -6960,17 +6960,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>HABANA 3382</t>
+          <t>BATLLE Y ORDOÑEZ, JOSE P.T. 4659</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>808413466</t>
+          <t>808413477</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6985,7 +6985,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -7007,46 +7007,46 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.505747</v>
+        <v>-58.464657</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.593173</v>
+        <v>-34.670556</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>6457</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7/18/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>BATLLE Y ORDOÑEZ, JOSE P.T. 4659</t>
+          <t>Gregario Laferrere 6572</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>808413477</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7061,7 +7061,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7069,7 +7069,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -7082,47 +7082,43 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M88" t="n">
-        <v>-58.464657</v>
-      </c>
-      <c r="N88" t="n">
-        <v>-34.670556</v>
-      </c>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>No ubicado</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6472</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Gregario Laferrere 6572</t>
+          <t>DUMONT, SANTOS 3744</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808509381</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7137,7 +7133,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7155,19 +7151,23 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.448576</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.585794</v>
+      </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-25 07:05:22)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5130,7 +5130,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>805707158</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5140,17 +5140,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Cañada de Gómez 4433</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805707158</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5187,14 +5187,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.387847</v>
+        <v>-58.479486</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.587043</v>
+        <v>-34.681953</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5206,27 +5206,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5241,7 +5241,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5263,26 +5263,26 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.46579</v>
+        <v>-58.387847</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.555012</v>
+        <v>-34.587043</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5292,7 +5292,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5302,7 +5302,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5317,7 +5317,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5325,7 +5325,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5339,14 +5339,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.451835</v>
+        <v>-58.46579</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.562646</v>
+        <v>-34.555012</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5358,7 +5358,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5368,17 +5368,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5411,18 +5411,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.488252</v>
+        <v>-58.451835</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.553391</v>
+        <v>-34.562646</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5434,7 +5434,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5454,7 +5454,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5469,7 +5469,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5477,7 +5477,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5491,10 +5491,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.470837</v>
+        <v>-58.488252</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.545751</v>
+        <v>-34.553391</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5510,7 +5510,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5520,7 +5520,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5558,19 +5558,19 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.472267</v>
+        <v>-58.470837</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.551163</v>
+        <v>-34.545751</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5586,27 +5586,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5629,12 +5629,12 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5643,10 +5643,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.464144</v>
+        <v>-58.472267</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.541832</v>
+        <v>-34.551163</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -5662,7 +5662,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5672,17 +5672,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5697,7 +5697,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5719,26 +5719,26 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.434761</v>
+        <v>-58.464144</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.598381</v>
+        <v>-34.541832</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5748,17 +5748,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5773,7 +5773,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5791,30 +5791,30 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.464177</v>
+        <v>-58.434761</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.558239</v>
+        <v>-34.598381</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5824,17 +5824,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5867,50 +5867,50 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.412302</v>
+        <v>-58.464177</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.59301</v>
+        <v>-34.558239</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5925,11 +5925,11 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -5947,46 +5947,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.485056</v>
+        <v>-58.412302</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.555059</v>
+        <v>-34.59301</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-450</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Moldes 2325</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>807044059</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6001,11 +6001,11 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Corroida en base para cambiar contiene CDO/NAP propio </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -6023,10 +6023,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.461167</v>
+        <v>-58.485056</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.561613</v>
+        <v>-34.555059</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6042,27 +6042,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6099,46 +6099,46 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.49147</v>
+        <v>-58.487144</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.55031</v>
+        <v>-34.669078</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>807044286</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Echeandía 5779</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807044286</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6151,7 +6151,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I76" t="n">
         <v>1</v>
       </c>
@@ -6171,14 +6175,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.405761</v>
+        <v>-58.487136</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.582476</v>
+        <v>-34.667828</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6190,17 +6194,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>6496</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Moldes 2327</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6210,7 +6214,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807044059</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6247,46 +6251,46 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.432241</v>
+        <v>-58.461172</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.56642</v>
+        <v>-34.561608</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6301,7 +6305,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6323,46 +6327,46 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.417348</v>
+        <v>-58.49147</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.595467</v>
+        <v>-34.55031</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6375,11 +6379,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Columna inclinada con base  corroida</t>
-        </is>
-      </c>
+      <c r="H79" t="inlineStr"/>
       <c r="I79" t="n">
         <v>1</v>
       </c>
@@ -6395,18 +6395,18 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.472311</v>
+        <v>-58.405761</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.654867</v>
+        <v>-34.582476</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6418,27 +6418,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6475,46 +6475,46 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.450113</v>
+        <v>-58.432241</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.574534</v>
+        <v>-34.56642</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6547,50 +6547,50 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.484729</v>
+        <v>-58.417348</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.574614</v>
+        <v>-34.595467</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>-491</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>3 de Febrero 2171</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Columna 114 propia picada en base con NAP</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6623,50 +6623,50 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.452636</v>
+        <v>-58.472311</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.558607</v>
+        <v>-34.654867</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6681,7 +6681,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6699,18 +6699,18 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.510247</v>
+        <v>-58.450113</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.645038</v>
+        <v>-34.574534</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6722,27 +6722,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6410</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>BEAUCHEF 421</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808373658</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6757,7 +6757,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6775,50 +6775,50 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.433724</v>
+        <v>-58.484729</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.621643</v>
+        <v>-34.574614</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-518</t>
+          <t>-491</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>3 de Febrero 2171</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6833,7 +6833,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Columna 114 propia picada en base con NAP</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6855,10 +6855,10 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.483145</v>
+        <v>-58.452636</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.557043</v>
+        <v>-34.558607</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -6874,27 +6874,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6454</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/18/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>HABANA 3382</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808413466</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6927,18 +6927,18 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.505747</v>
+        <v>-58.510247</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.593173</v>
+        <v>-34.645038</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6950,27 +6950,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>6457</t>
+          <t>6410</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7/18/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>BATLLE Y ORDOÑEZ, JOSE P.T. 4659</t>
+          <t>BEAUCHEF 421</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>808413477</t>
+          <t>808373658</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6985,7 +6985,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -7007,10 +7007,10 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.464657</v>
+        <v>-58.433724</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.670556</v>
+        <v>-34.621643</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7026,27 +7026,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>-518</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Gregario Laferrere 6572</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7061,7 +7061,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7082,43 +7082,47 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
+      <c r="M88" t="n">
+        <v>-58.483145</v>
+      </c>
+      <c r="N88" t="n">
+        <v>-34.557043</v>
+      </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>6472</t>
+          <t>6454</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/18/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>DUMONT, SANTOS 3744</t>
+          <t>HABANA 3382</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>808509381</t>
+          <t>808413466</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7133,7 +7137,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7151,21 +7155,245 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.505747</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.593173</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>6457</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>7/18/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>BATLLE Y ORDOÑEZ, JOSE P.T. 4659</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>808413477</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Inclinada</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>-58.464657</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.670556</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>-521</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>7/21/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Gregario Laferrere 6572</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>808430950</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>6472</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>7/24/2025</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>DUMONT, SANTOS 3744</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>808509381</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
           <t>Poste</t>
         </is>
       </c>
-      <c r="M89" t="n">
+      <c r="M92" t="n">
         <v>-58.448576</v>
       </c>
-      <c r="N89" t="n">
+      <c r="N92" t="n">
         <v>-34.585794</v>
       </c>
-      <c r="O89" t="inlineStr">
+      <c r="O92" t="inlineStr">
         <is>
           <t>Colegiales</t>
         </is>
       </c>
-      <c r="P89" t="inlineStr">
+      <c r="P92" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-25 11:59:28)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6042,27 +6042,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6099,26 +6099,26 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.487144</v>
+        <v>-58.469783</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.669078</v>
+        <v>-34.599214</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>807044286</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6128,7 +6128,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Echeandía 5779</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807044286</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6175,10 +6175,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.487136</v>
+        <v>-58.487144</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.667828</v>
+        <v>-34.669078</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6194,7 +6194,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6496</t>
+          <t>807044286</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6204,17 +6204,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Moldes 2327</t>
+          <t>Echeandía 5779</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807044059</t>
+          <t>807044286</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6251,46 +6251,46 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.461172</v>
+        <v>-58.487136</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.561608</v>
+        <v>-34.667828</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>6496</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Moldes 2327</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807044059</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6305,7 +6305,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6327,10 +6327,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.49147</v>
+        <v>-58.461172</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.55031</v>
+        <v>-34.561608</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6346,27 +6346,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6379,7 +6379,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr"/>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Inclinada</t>
+        </is>
+      </c>
       <c r="I79" t="n">
         <v>1</v>
       </c>
@@ -6399,36 +6403,36 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.405761</v>
+        <v>-58.49147</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.582476</v>
+        <v>-34.55031</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6438,7 +6442,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6451,11 +6455,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H80" t="inlineStr"/>
       <c r="I80" t="n">
         <v>1</v>
       </c>
@@ -6475,14 +6475,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.432241</v>
+        <v>-58.405761</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.56642</v>
+        <v>-34.582476</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6494,7 +6494,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6504,7 +6504,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -6514,7 +6514,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6551,10 +6551,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.417348</v>
+        <v>-58.432241</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.595467</v>
+        <v>-34.56642</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6570,27 +6570,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6623,18 +6623,18 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.472311</v>
+        <v>-58.417348</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.654867</v>
+        <v>-34.595467</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6646,7 +6646,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6656,17 +6656,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6681,7 +6681,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6699,30 +6699,30 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.450113</v>
+        <v>-58.472311</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.574534</v>
+        <v>-34.654867</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6732,17 +6732,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6757,7 +6757,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6775,18 +6775,18 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.484729</v>
+        <v>-58.450113</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.574614</v>
+        <v>-34.574534</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6798,27 +6798,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-491</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>3 de Febrero 2171</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6833,7 +6833,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Columna 114 propia picada en base con NAP</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6851,18 +6851,18 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.452636</v>
+        <v>-58.484729</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.558607</v>
+        <v>-34.574614</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6874,27 +6874,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>-491</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>3 de Febrero 2171</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna 114 propia picada en base con NAP</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6927,18 +6927,18 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.510247</v>
+        <v>-58.452636</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.645038</v>
+        <v>-34.558607</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6950,7 +6950,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>6410</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -6960,17 +6960,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>BEAUCHEF 421</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>808373658</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6985,7 +6985,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -7003,50 +7003,50 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.433724</v>
+        <v>-58.510247</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.621643</v>
+        <v>-34.645038</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-518</t>
+          <t>6410</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>BEAUCHEF 421</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808373658</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7061,7 +7061,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7083,46 +7083,46 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.483145</v>
+        <v>-58.433724</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.557043</v>
+        <v>-34.621643</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>6454</t>
+          <t>-518</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>7/18/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>HABANA 3382</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>808413466</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7137,7 +7137,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7159,14 +7159,14 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.505747</v>
+        <v>-58.483145</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.593173</v>
+        <v>-34.557043</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
@@ -7178,7 +7178,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>6457</t>
+          <t>6454</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -7188,17 +7188,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>BATLLE Y ORDOÑEZ, JOSE P.T. 4659</t>
+          <t>HABANA 3382</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>808413477</t>
+          <t>808413466</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -7213,7 +7213,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -7221,7 +7221,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -7235,46 +7235,46 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.464657</v>
+        <v>-58.505747</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.670556</v>
+        <v>-34.593173</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6457</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/18/2025</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Gregario Laferrere 6572</t>
+          <t>BATLLE Y ORDOÑEZ, JOSE P.T. 4659</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808413477</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -7289,7 +7289,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -7297,7 +7297,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
@@ -7310,43 +7310,47 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M91" t="inlineStr"/>
-      <c r="N91" t="inlineStr"/>
+      <c r="M91" t="n">
+        <v>-58.464657</v>
+      </c>
+      <c r="N91" t="n">
+        <v>-34.670556</v>
+      </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>No ubicado</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>6472</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>DUMONT, SANTOS 3744</t>
+          <t>Gregario Laferrere 6572</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>808509381</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -7361,7 +7365,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -7379,21 +7383,93 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>No ubicado</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>No clasificado, consultar con mantenimiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>6472</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>7/24/2025</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>DUMONT, SANTOS 3744</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>808509381</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>1</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
           <t>Poste</t>
         </is>
       </c>
-      <c r="M92" t="n">
+      <c r="M93" t="n">
         <v>-58.448576</v>
       </c>
-      <c r="N92" t="n">
+      <c r="N93" t="n">
         <v>-34.585794</v>
       </c>
-      <c r="O92" t="inlineStr">
+      <c r="O93" t="inlineStr">
         <is>
           <t>Colegiales</t>
         </is>
       </c>
-      <c r="P92" t="inlineStr">
+      <c r="P93" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-25 14:21:51)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P93"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7475,6 +7475,82 @@
         </is>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>6497</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>7/25/2025</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>808533127</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Inclinada</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>1</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
+        <v>-58.422229</v>
+      </c>
+      <c r="N94" t="n">
+        <v>-34.573148</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-30 06:58:14)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P94"/>
+  <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7551,6 +7551,78 @@
         </is>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>-536</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>7/29/2025</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Olof palme 4142</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Aplomar o desmontar poste</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>1</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>-58.488239</v>
+      </c>
+      <c r="N95" t="n">
+        <v>-34.55341</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-31 13:31:39)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -5764,11 +5764,7 @@
           <t>8</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>807044233</t>
-        </is>
-      </c>
+      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
           <t>AYKO</t>
@@ -5781,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I71" t="n">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-31 14:41:34)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -5764,7 +5764,11 @@
           <t>8</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ICD30261461 </t>
+        </is>
+      </c>
       <c r="F71" t="inlineStr">
         <is>
           <t>AYKO</t>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-02 07:27:04)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5062,7 +5062,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5072,7 +5072,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5097,7 +5097,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5119,10 +5119,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.488252</v>
+        <v>-58.470837</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.553391</v>
+        <v>-34.545751</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5138,7 +5138,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5158,7 +5158,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5186,19 +5186,19 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5214,27 +5214,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5257,12 +5257,12 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
@@ -5271,10 +5271,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5290,7 +5290,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5300,17 +5300,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5347,26 +5347,26 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5376,17 +5376,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5419,30 +5419,30 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5452,17 +5452,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5477,7 +5477,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5495,50 +5495,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5553,11 +5553,11 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -5575,46 +5575,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.412302</v>
+        <v>-58.485056</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.59301</v>
+        <v>-34.555059</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5629,15 +5629,15 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5651,14 +5651,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.485056</v>
+        <v>-58.469783</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.555059</v>
+        <v>-34.599214</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5670,27 +5670,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5705,7 +5705,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5723,30 +5723,30 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.469783</v>
+        <v>-58.487144</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.599214</v>
+        <v>-34.669078</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>6496</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5756,17 +5756,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Moldes 2327</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807044059</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5799,50 +5799,50 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.487144</v>
+        <v>-58.461172</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.669078</v>
+        <v>-34.561608</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6496</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Moldes 2327</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807044059</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5857,7 +5857,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5879,10 +5879,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.461172</v>
+        <v>-58.49147</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.561608</v>
+        <v>-34.55031</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5898,27 +5898,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5931,11 +5931,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H73" t="inlineStr"/>
       <c r="I73" t="n">
         <v>1</v>
       </c>
@@ -5955,36 +5951,36 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.49147</v>
+        <v>-58.405761</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.55031</v>
+        <v>-34.582476</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -5994,7 +5990,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6007,7 +6003,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I74" t="n">
         <v>1</v>
       </c>
@@ -6027,14 +6027,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6046,7 +6046,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6056,7 +6056,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6066,7 +6066,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6103,10 +6103,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6122,27 +6122,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6157,7 +6157,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6175,18 +6175,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6198,7 +6198,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6208,17 +6208,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6251,30 +6251,30 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.472311</v>
+        <v>-58.450113</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.654867</v>
+        <v>-34.574534</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6284,17 +6284,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6327,18 +6327,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.450113</v>
+        <v>-58.484729</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.574534</v>
+        <v>-34.574614</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6350,27 +6350,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>-491</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>3 de Febrero 2171</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6385,7 +6385,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Columna 114 propia picada en base con NAP</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6403,18 +6403,18 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.484729</v>
+        <v>-58.452636</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.574614</v>
+        <v>-34.558607</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6426,27 +6426,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-491</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>3 de Febrero 2171</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Columna 114 propia picada en base con NAP</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6479,18 +6479,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.452636</v>
+        <v>-58.510247</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.558607</v>
+        <v>-34.645038</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6502,7 +6502,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6410</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6512,17 +6512,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>BEAUCHEF 421</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373658</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6545,7 +6545,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6555,50 +6555,50 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.510247</v>
+        <v>-58.433724</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.645038</v>
+        <v>-34.621643</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6410</t>
+          <t>-518</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>BEAUCHEF 421</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808373658</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6635,46 +6635,46 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.433724</v>
+        <v>-58.483145</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.621643</v>
+        <v>-34.557043</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-518</t>
+          <t>6454</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/18/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>HABANA 3382</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808413466</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6711,14 +6711,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.483145</v>
+        <v>-58.505747</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.557043</v>
+        <v>-34.593173</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6730,27 +6730,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6454</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7/18/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>HABANA 3382</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808413466</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6787,14 +6787,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.505747</v>
+        <v>-58.496608</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.593173</v>
+        <v>-34.666371</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6806,27 +6806,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6472</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>DUMONT, SANTOS 3744</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808509381</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6859,18 +6859,18 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.496608</v>
+        <v>-58.448576</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.666371</v>
+        <v>-34.585794</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6882,27 +6882,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6472</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>DUMONT, SANTOS 3744</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808509381</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6925,7 +6925,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6935,175 +6935,23 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.448576</v>
+        <v>-58.422229</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.585794</v>
+        <v>-34.573148</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>6497</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>7/25/2025</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>808533127</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M87" t="n">
-        <v>-58.422229</v>
-      </c>
-      <c r="N87" t="n">
-        <v>-34.573148</v>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
-        <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>-536</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>7/29/2025</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Olof palme 4142</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ICD30249764 </t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Aplomar o desmontar poste</t>
-        </is>
-      </c>
-      <c r="I88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M88" t="n">
-        <v>-58.488239</v>
-      </c>
-      <c r="N88" t="n">
-        <v>-34.55341</v>
-      </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P88" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-05 08:03:53)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6347,6 +6347,154 @@
         </is>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>6481</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>8/4/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>DIAZ, CESAR, GRAL. 3520</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>808703875</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.486002</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.61821</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>6556</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>8/4/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>2 DE ABRIL DE 1982 6982</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.494864</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.678826</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-06 07:05:49)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6495,6 +6495,234 @@
         </is>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>6193</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>8/5/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>POLA 591</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>808720861</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.507385</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.644479</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>6277</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>8/5/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>SENILLOSA 323</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>808720859</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.429726</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.619969</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>6274</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>8/5/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>808720858</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>chocada</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>-58.473089</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.625478</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-07 07:22:31)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6444,7 +6444,11 @@
           <t>8</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
       <c r="F80" t="inlineStr">
         <is>
           <t>AYKO</t>
@@ -6720,6 +6724,234 @@
       <c r="P83" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>6469</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>USPALLATA 3626</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>808733910</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Aplomar</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.414389</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.641308</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>808733912</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.468841</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.686635</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>6567</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>SAN ANTONIO 1221</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>808733914</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Aplomar</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>-58.375684</v>
+      </c>
+      <c r="N86" t="n">
+        <v>-34.656092</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-07 14:26:16)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6046,7 +6046,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-518</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6952,6 +6952,82 @@
       <c r="P86" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>-549</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>8/7/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>14 de Julio 65</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>808749189</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>picada</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>-58.468496</v>
+      </c>
+      <c r="N87" t="n">
+        <v>-34.591282</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-11 11:26:58)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6502,7 +6502,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6193</t>
+          <t>6277</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6512,17 +6512,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>POLA 591</t>
+          <t>SENILLOSA 323</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808720861</t>
+          <t>808720859</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6541,7 +6541,7 @@
         </is>
       </c>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -6559,26 +6559,26 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.507385</v>
+        <v>-58.429726</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.644479</v>
+        <v>-34.619969</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6277</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6588,17 +6588,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SENILLOSA 323</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808720859</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6635,46 +6635,46 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.429726</v>
+        <v>-58.473089</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.619969</v>
+        <v>-34.625478</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6469</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>USPALLATA 3626</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733910</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6711,26 +6711,26 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.473089</v>
+        <v>-58.414389</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.625478</v>
+        <v>-34.641308</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6469</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6740,17 +6740,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>USPALLATA 3626</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808733910</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6787,10 +6787,10 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.414389</v>
+        <v>-58.468841</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.641308</v>
+        <v>-34.686635</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -6806,7 +6806,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6816,17 +6816,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6849,7 +6849,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -6863,14 +6863,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.468841</v>
+        <v>-58.375684</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.686635</v>
+        <v>-34.656092</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6882,27 +6882,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>-549</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>14 de Julio 65</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808749189</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6925,7 +6925,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6939,93 +6939,17 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.375684</v>
+        <v>-58.468496</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.656092</v>
+        <v>-34.591282</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>-549</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>8/7/2025</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>14 de Julio 65</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>808749189</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>picada</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M87" t="n">
-        <v>-58.468496</v>
-      </c>
-      <c r="N87" t="n">
-        <v>-34.591282</v>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-13 08:41:12)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2022,29 +2022,29 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>6901</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2/24/2025</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>PINO, Virrey del 2644</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>803608215</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>2/24/2025</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>DEL PINO VIRREY /ALT/ 2646</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>803608215</t>
-        </is>
-      </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>AYKO</t>
@@ -2057,11 +2057,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Columna 114 quebrada en base dar prioridad.</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2079,10 +2079,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.45524</v>
+        <v>-58.455073</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.567858</v>
+        <v>-34.56776</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -6350,27 +6350,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6481</t>
+          <t>6411</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>DIAZ, CESAR, GRAL. 3520</t>
+          <t>CRAIG 720</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808703875</t>
+          <t>808609241</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6407,26 +6407,26 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.486002</v>
+        <v>-58.434949</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.61821</v>
+        <v>-34.627171</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6481</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6436,17 +6436,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>DIAZ, CESAR, GRAL. 3520</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808703875</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6479,50 +6479,50 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.494864</v>
+        <v>-58.486002</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.678826</v>
+        <v>-34.61821</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6277</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>SENILLOSA 323</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808720859</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6545,7 +6545,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6555,14 +6555,14 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.429726</v>
+        <v>-58.494864</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.619969</v>
+        <v>-34.678826</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6578,7 +6578,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6277</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6588,17 +6588,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>SENILLOSA 323</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808720859</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6635,46 +6635,46 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.473089</v>
+        <v>-58.429726</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.625478</v>
+        <v>-34.619969</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6469</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>USPALLATA 3626</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808733910</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6711,26 +6711,26 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.414389</v>
+        <v>-58.473089</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.641308</v>
+        <v>-34.625478</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6469</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6740,17 +6740,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>USPALLATA 3626</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733910</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6787,10 +6787,10 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.468841</v>
+        <v>-58.414389</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.686635</v>
+        <v>-34.641308</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -6806,7 +6806,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6816,17 +6816,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6849,7 +6849,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -6863,14 +6863,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.375684</v>
+        <v>-58.468841</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.656092</v>
+        <v>-34.686635</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6882,27 +6882,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6925,31 +6925,107 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>-58.375684</v>
+      </c>
+      <c r="N86" t="n">
+        <v>-34.656092</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>-549</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>8/7/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>14 de Julio 65</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>808749189</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>picada</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M86" t="n">
+      <c r="M87" t="n">
         <v>-58.468496</v>
       </c>
-      <c r="N86" t="n">
+      <c r="N87" t="n">
         <v>-34.591282</v>
       </c>
-      <c r="O86" t="inlineStr">
+      <c r="O87" t="inlineStr">
         <is>
           <t>Paternal</t>
         </is>
       </c>
-      <c r="P86" t="inlineStr">
+      <c r="P87" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-15 11:42:08)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -746,7 +746,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-9</t>
+          <t>6968</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SANTA FE ,AV. /ALT/ 5154</t>
+          <t>SANTA FE AV. 5154</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -781,11 +781,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>cambio de columna la misma NO presenta riesgo de caída</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -802,22 +802,10 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M5" t="n">
-        <v>-58.432658</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-34.576446</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5818,7 +5806,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-491</t>
+          <t>6942</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5828,7 +5816,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>3 de Febrero 2171</t>
+          <t>3 DE FEBRERO 2169</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5853,7 +5841,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Columna 114 propia picada en base con NAP</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5874,22 +5862,10 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M72" t="n">
-        <v>-58.452636</v>
-      </c>
-      <c r="N72" t="n">
-        <v>-34.558607</v>
-      </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P72" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -7030,6 +7006,198 @@
           <t>Capital Norte</t>
         </is>
       </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>6947</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>ALMAFUERTE AV. 682</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>808972978</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>6951</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>MEXICO 2751</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>808972984</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>6960</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>8/14/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>VALLESE, FELIPE 1940</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>808972988</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-15 11:45:48)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -802,10 +802,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>-58.432658</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-34.576446</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5862,10 +5874,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
-      <c r="O72" t="inlineStr"/>
-      <c r="P72" t="inlineStr"/>
+      <c r="M72" t="n">
+        <v>-58.452583</v>
+      </c>
+      <c r="N72" t="n">
+        <v>-34.558668</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -7066,10 +7090,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
-      <c r="O88" t="inlineStr"/>
-      <c r="P88" t="inlineStr"/>
+      <c r="M88" t="n">
+        <v>-58.414185</v>
+      </c>
+      <c r="N88" t="n">
+        <v>-34.64524</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -7130,10 +7166,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
-      <c r="O89" t="inlineStr"/>
-      <c r="P89" t="inlineStr"/>
+      <c r="M89" t="n">
+        <v>-58.404946</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.617251</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -7194,10 +7242,22 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr"/>
-      <c r="P90" t="inlineStr"/>
+      <c r="M90" t="n">
+        <v>-58.460818</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.618934</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-20 07:39:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1946,27 +1946,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-263</t>
+          <t>6901</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Fraga 93</t>
+          <t>PINO, Virrey del 2644</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>802848838</t>
+          <t>803608215</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1999,14 +1999,14 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.446721</v>
+        <v>-58.455073</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.587175</v>
+        <v>-34.56776</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2022,7 +2022,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6901</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2032,17 +2032,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PINO, Virrey del 2644</t>
+          <t>COCHABAMBA /ALT/ 1790</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803608215</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2057,11 +2057,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>SIN RIEGO</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2079,46 +2079,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.455073</v>
+        <v>-58.391153</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.56776</v>
+        <v>-34.624022</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>-281</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>COCHABAMBA /ALT/ 1790</t>
+          <t>SOLER /ALT/ 4517</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>803651203</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>SIN RIEGO</t>
+          <t>columna de 114 con nodo y redes nuestra.</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2155,14 +2155,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.391153</v>
+        <v>-58.423405</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.624022</v>
+        <v>-34.588075</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,17 +2174,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-281</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SOLER /ALT/ 4517</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>803651203</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,11 +2209,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>columna de 114 con nodo y redes nuestra.</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2222,19 +2222,19 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.423405</v>
+        <v>-58.42486</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.588075</v>
+        <v>-34.577318</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2250,27 +2250,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2298,35 +2298,35 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.42486</v>
+        <v>-58.491074</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.577318</v>
+        <v>-34.575623</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2336,17 +2336,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,12 +2369,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2383,14 +2383,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.491074</v>
+        <v>-58.525125</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.575623</v>
+        <v>-34.604668</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2402,27 +2402,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2459,26 +2459,26 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.525125</v>
+        <v>-58.421964</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.604668</v>
+        <v>-34.586342</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,17 +2488,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2535,26 +2535,26 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.421964</v>
+        <v>-58.498493</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.586342</v>
+        <v>-34.581262</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-340</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2564,17 +2564,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>SUPERI /ALT/ 1445</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804838869</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2611,14 +2611,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.498493</v>
+        <v>-58.460666</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.581262</v>
+        <v>-34.573823</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2630,27 +2630,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-340</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SUPERI /ALT/ 1445</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804838869</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,11 +2665,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2687,14 +2687,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.460666</v>
+        <v>-58.502447</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.573823</v>
+        <v>-34.561008</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2706,7 +2706,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2716,17 +2716,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2763,10 +2763,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.502447</v>
+        <v>-58.483947</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.561008</v>
+        <v>-34.583207</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,17 +2792,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,14 +2835,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.483947</v>
+        <v>-58.503673</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.583207</v>
+        <v>-34.586925</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2858,7 +2858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2911,14 +2911,14 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.503673</v>
+        <v>-58.504455</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.586925</v>
+        <v>-34.579941</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2934,7 +2934,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-355</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>CUENCA /ALT/ 4480</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839675</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2982,7 +2982,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente TLC</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2991,10 +2991,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.504455</v>
+        <v>-58.504568</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579941</v>
+        <v>-34.590534</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3010,7 +3010,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-355</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 4480</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804839675</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3067,10 +3067,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.504568</v>
+        <v>-58.503195</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.590534</v>
+        <v>-34.581735</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3086,7 +3086,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3106,7 +3106,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3143,14 +3143,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.503195</v>
+        <v>-58.493164</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.581735</v>
+        <v>-34.55732</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3162,7 +3162,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3172,7 +3172,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3219,14 +3219,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.493164</v>
+        <v>-58.491934</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.55732</v>
+        <v>-34.569348</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3238,7 +3238,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3295,10 +3295,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.491934</v>
+        <v>-58.501418</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.569348</v>
+        <v>-34.574363</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3314,7 +3314,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3334,7 +3334,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3371,14 +3371,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.501418</v>
+        <v>-58.494584</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.574363</v>
+        <v>-34.554981</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3390,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,11 +3425,11 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3443,14 +3443,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.494584</v>
+        <v>-58.465608</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.554981</v>
+        <v>-34.538489</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3466,27 +3466,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3519,18 +3519,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.465608</v>
+        <v>-58.436788</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.538489</v>
+        <v>-34.604014</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3542,7 +3542,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3552,17 +3552,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3599,26 +3599,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.436788</v>
+        <v>-58.439461</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.604014</v>
+        <v>-34.605744</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,17 +3628,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3675,10 +3675,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.439461</v>
+        <v>-58.418424</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.605744</v>
+        <v>-34.604463</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,7 +3694,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>-377</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>HUMAHUACA /ALT/ 3918</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>804903788</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3751,10 +3751,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.418424</v>
+        <v>-58.419694</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.604463</v>
+        <v>-34.602062</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-377</t>
+          <t>-383</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HUMAHUACA /ALT/ 3918</t>
+          <t>VALDERRAMA /ALT/ 4187</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804903788</t>
+          <t>805507401</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t xml:space="preserve">Aplomar columna 114 </t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3827,26 +3827,26 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.419694</v>
+        <v>-58.481834</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.602062</v>
+        <v>-34.560796</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-383</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,17 +3856,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>VALDERRAMA /ALT/ 4187</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805507401</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114 </t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3903,14 +3903,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.481834</v>
+        <v>-58.473936</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.560796</v>
+        <v>-34.577346</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-385</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>MOLDES /ALT/ 1913</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805507415</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3979,10 +3979,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.473936</v>
+        <v>-58.45789</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.577346</v>
+        <v>-34.565423</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,7 +3998,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-385</t>
+          <t>-386</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,7 +4008,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1913</t>
+          <t>MOLDES /ALT/ 1943</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4018,7 +4018,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805507415</t>
+          <t>805507419</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4055,10 +4055,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.45789</v>
+        <v>-58.458217</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.565423</v>
+        <v>-34.565043</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,27 +4074,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-386</t>
+          <t>-392</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1943</t>
+          <t>GARCIA TEODORO /ALT/ 1775</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805507419</t>
+          <t>805676615</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4117,12 +4117,12 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4131,10 +4131,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.458217</v>
+        <v>-58.440367</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.565043</v>
+        <v>-34.563551</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4150,7 +4150,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-392</t>
+          <t>-393</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>GARCIA TEODORO /ALT/ 1775</t>
+          <t>3 DE FEBRERO /ALT/ 1272</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805676615</t>
+          <t>805676618</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4207,10 +4207,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.440367</v>
+        <v>-58.445186</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.563551</v>
+        <v>-34.567417</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4226,27 +4226,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-393</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO /ALT/ 1272</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805676618</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4283,46 +4283,46 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.445186</v>
+        <v>-58.387847</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.567417</v>
+        <v>-34.587043</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4359,26 +4359,26 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.387847</v>
+        <v>-58.46579</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.587043</v>
+        <v>-34.555012</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4435,14 +4435,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.46579</v>
+        <v>-58.451835</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.555012</v>
+        <v>-34.562646</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4454,7 +4454,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,17 +4464,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4507,18 +4507,18 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.451835</v>
+        <v>-58.470837</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.562646</v>
+        <v>-34.545751</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4530,7 +4530,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4550,7 +4550,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4578,19 +4578,19 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4606,27 +4606,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4649,12 +4649,12 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -4663,10 +4663,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4682,7 +4682,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4692,17 +4692,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,26 +4739,26 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4768,17 +4768,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4811,30 +4811,30 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4844,17 +4844,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4887,50 +4887,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,11 +4945,11 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -4967,46 +4967,46 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.412302</v>
+        <v>-58.485056</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.59301</v>
+        <v>-34.555059</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5021,15 +5021,15 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5043,14 +5043,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.485056</v>
+        <v>-58.469783</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.555059</v>
+        <v>-34.599214</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5062,27 +5062,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5097,7 +5097,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5115,30 +5115,30 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.469783</v>
+        <v>-58.487144</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.599214</v>
+        <v>-34.669078</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>6496</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5148,17 +5148,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Moldes 2327</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807044059</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5191,50 +5191,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.487144</v>
+        <v>-58.461172</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.669078</v>
+        <v>-34.561608</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6496</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Moldes 2327</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807044059</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5271,10 +5271,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.461172</v>
+        <v>-58.49147</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.561608</v>
+        <v>-34.55031</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5290,27 +5290,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5323,11 +5323,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H65" t="inlineStr"/>
       <c r="I65" t="n">
         <v>1</v>
       </c>
@@ -5347,36 +5343,36 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.49147</v>
+        <v>-58.405761</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.55031</v>
+        <v>-34.582476</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5386,7 +5382,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5399,7 +5395,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H66" t="inlineStr"/>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I66" t="n">
         <v>1</v>
       </c>
@@ -5419,14 +5419,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5438,7 +5438,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5448,7 +5448,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5458,7 +5458,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5495,10 +5495,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5514,27 +5514,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5567,18 +5567,18 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5600,17 +5600,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5643,30 +5643,30 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.472311</v>
+        <v>-58.450113</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.654867</v>
+        <v>-34.574534</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5676,17 +5676,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5719,18 +5719,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.450113</v>
+        <v>-58.484729</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.574534</v>
+        <v>-34.574614</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5742,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6942</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>3 DE FEBRERO 2169</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5795,18 +5795,18 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.484729</v>
+        <v>-58.452583</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.574614</v>
+        <v>-34.558668</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5818,27 +5818,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6942</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 2169</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5871,18 +5871,18 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.452583</v>
+        <v>-58.510247</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.558668</v>
+        <v>-34.645038</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5894,7 +5894,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6410</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5904,17 +5904,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>BEAUCHEF 421</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373658</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5929,7 +5929,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5947,50 +5947,50 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.510247</v>
+        <v>-58.433724</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.645038</v>
+        <v>-34.621643</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6410</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BEAUCHEF 421</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808373658</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6027,46 +6027,46 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.433724</v>
+        <v>-58.483145</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.621643</v>
+        <v>-34.557043</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6103,14 +6103,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.483145</v>
+        <v>-58.496608</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.557043</v>
+        <v>-34.666371</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6122,27 +6122,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6157,7 +6157,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6165,7 +6165,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -6179,46 +6179,46 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.496608</v>
+        <v>-58.422229</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.666371</v>
+        <v>-34.573148</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6472</t>
+          <t>6411</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/31/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>DUMONT, SANTOS 3744</t>
+          <t>CRAIG 720</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808509381</t>
+          <t>808609241</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6251,50 +6251,50 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.448576</v>
+        <v>-58.434949</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.585794</v>
+        <v>-34.627171</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6481</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>DIAZ, CESAR, GRAL. 3520</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808703875</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6331,46 +6331,46 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.422229</v>
+        <v>-58.486002</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.573148</v>
+        <v>-34.61821</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6411</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>CRAIG 720</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808609241</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6385,7 +6385,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6393,7 +6393,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6403,14 +6403,14 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.434949</v>
+        <v>-58.494864</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.627171</v>
+        <v>-34.678826</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -6426,27 +6426,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6481</t>
+          <t>6277</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>DIAZ, CESAR, GRAL. 3520</t>
+          <t>SENILLOSA 323</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808703875</t>
+          <t>808720859</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6483,46 +6483,46 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.486002</v>
+        <v>-58.429726</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.61821</v>
+        <v>-34.619969</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6545,7 +6545,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6555,50 +6555,50 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.494864</v>
+        <v>-58.473089</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.678826</v>
+        <v>-34.625478</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6277</t>
+          <t>6469</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SENILLOSA 323</t>
+          <t>USPALLATA 3626</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808720859</t>
+          <t>808733910</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6621,7 +6621,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -6635,10 +6635,10 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.429726</v>
+        <v>-58.414389</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.619969</v>
+        <v>-34.641308</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6654,27 +6654,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6711,26 +6711,26 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.473089</v>
+        <v>-58.468841</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.625478</v>
+        <v>-34.686635</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6469</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6740,7 +6740,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>USPALLATA 3626</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6750,7 +6750,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808733910</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6787,14 +6787,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.414389</v>
+        <v>-58.375684</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.641308</v>
+        <v>-34.656092</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6806,27 +6806,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>-549</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>14 de Julio 65</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808749189</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6863,36 +6863,36 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.468841</v>
+        <v>-58.468496</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.686635</v>
+        <v>-34.591282</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6947</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>ALMAFUERTE AV. 682</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -6902,7 +6902,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808972978</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6925,7 +6925,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6939,10 +6939,10 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.375684</v>
+        <v>-58.414185</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.656092</v>
+        <v>-34.64524</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6958,27 +6958,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>6951</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>MEXICO 2751</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>808972984</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7015,26 +7015,26 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.468496</v>
+        <v>-58.404946</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.591282</v>
+        <v>-34.617251</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>6947</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7044,17 +7044,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>ALMAFUERTE AV. 682</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>808972978</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7069,7 +7069,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7091,14 +7091,14 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.414185</v>
+        <v>-58.460818</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.64524</v>
+        <v>-34.618934</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
@@ -7110,27 +7110,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>6951</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>MEXICO 2751</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>808972984</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7145,7 +7145,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7153,7 +7153,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -7167,93 +7167,17 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.404946</v>
+        <v>-58.460441</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.617251</v>
+        <v>-34.628243</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>6960</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>VALLESE, FELIPE 1940</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>808972988</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I90" t="n">
-        <v>1</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M90" t="n">
-        <v>-58.460818</v>
-      </c>
-      <c r="N90" t="n">
-        <v>-34.618934</v>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P90" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-21 08:06:48)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -5818,27 +5818,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6409</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>CASTAÑARES AV. 5656</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Faltan cargar las fotos del cierre</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5871,30 +5871,30 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.510247</v>
+        <v>-58.479921</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.645038</v>
+        <v>-34.673021</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6410</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5904,17 +5904,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BEAUCHEF 421</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808373658</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5929,7 +5929,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5947,23 +5947,23 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.433724</v>
+        <v>-58.510247</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.621643</v>
+        <v>-34.645038</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-22 08:55:08)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7183,6 +7183,82 @@
         </is>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>-557</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>8/21/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Av Castañares 4621</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Colocar columna para pedir traspaso de nodo telecom</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>-58.470977</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.665358</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 08:01:21)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6198,27 +6198,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6411</t>
+          <t>6481</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7/31/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>CRAIG 720</t>
+          <t>DIAZ, CESAR, GRAL. 3520</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808609241</t>
+          <t>808703875</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6255,26 +6255,26 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.434949</v>
+        <v>-58.486002</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.627171</v>
+        <v>-34.61821</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6481</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6284,17 +6284,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>DIAZ, CESAR, GRAL. 3520</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808703875</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6327,50 +6327,50 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.486002</v>
+        <v>-58.494864</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.61821</v>
+        <v>-34.678826</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6385,7 +6385,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6393,7 +6393,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6403,50 +6403,50 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.494864</v>
+        <v>-58.473089</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.678826</v>
+        <v>-34.625478</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6277</t>
+          <t>6469</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SENILLOSA 323</t>
+          <t>USPALLATA 3626</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808720859</t>
+          <t>808733910</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6483,10 +6483,10 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.429726</v>
+        <v>-58.414389</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.619969</v>
+        <v>-34.641308</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -6502,27 +6502,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6559,26 +6559,26 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.473089</v>
+        <v>-58.468841</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.625478</v>
+        <v>-34.686635</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6469</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6588,7 +6588,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>USPALLATA 3626</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6598,7 +6598,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808733910</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6635,14 +6635,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.414389</v>
+        <v>-58.375684</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.641308</v>
+        <v>-34.656092</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6654,27 +6654,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>-549</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>14 de Julio 65</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808749189</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6711,36 +6711,36 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.468841</v>
+        <v>-58.468496</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.686635</v>
+        <v>-34.591282</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6947</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>ALMAFUERTE AV. 682</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6750,7 +6750,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808972978</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6787,10 +6787,10 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.375684</v>
+        <v>-58.414185</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.656092</v>
+        <v>-34.64524</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -6806,27 +6806,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>6951</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>MEXICO 2751</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>808972984</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6863,26 +6863,26 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.468496</v>
+        <v>-58.404946</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.591282</v>
+        <v>-34.617251</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6947</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -6892,17 +6892,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>ALMAFUERTE AV. 682</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808972978</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6939,14 +6939,14 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.414185</v>
+        <v>-58.460818</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.64524</v>
+        <v>-34.618934</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6958,27 +6958,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>6951</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>MEXICO 2751</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>808972984</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -7015,14 +7015,14 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.404946</v>
+        <v>-58.460441</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.617251</v>
+        <v>-34.628243</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -7034,27 +7034,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>-557</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>Av Castañares 4621</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>ICD30462144</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7069,7 +7069,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de nodo telecom</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7082,7 +7082,7 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L88" t="inlineStr">
@@ -7091,10 +7091,10 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.460818</v>
+        <v>-58.470977</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.618934</v>
+        <v>-34.665358</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -7102,158 +7102,6 @@
         </is>
       </c>
       <c r="P88" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>6979</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>8/18/2025</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>RIVADAVIA AV. 6740</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>809006419</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M89" t="n">
-        <v>-58.460441</v>
-      </c>
-      <c r="N89" t="n">
-        <v>-34.628243</v>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>-557</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>8/21/2025</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Av Castañares 4621</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>Pendiente ADM</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Colocar columna para pedir traspaso de nodo telecom</t>
-        </is>
-      </c>
-      <c r="I90" t="n">
-        <v>1</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M90" t="n">
-        <v>-58.470977</v>
-      </c>
-      <c r="N90" t="n">
-        <v>-34.665358</v>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P90" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 13:59:21)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7107,6 +7107,82 @@
         </is>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>-563</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Av Castañares 4520</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>809157022</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Cambiar pasante</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.470249</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.664835</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 15:13:04)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -3694,7 +3694,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-377</t>
+          <t>7054</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HUMAHUACA /ALT/ 3918</t>
+          <t>HUMAHUACA 3918</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -6806,7 +6806,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>6951</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6816,17 +6816,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>MEXICO 2751</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808972984</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6863,14 +6863,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.404946</v>
+        <v>-58.460818</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.617251</v>
+        <v>-34.618934</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6882,17 +6882,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -6902,7 +6902,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6925,7 +6925,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6939,10 +6939,10 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.460818</v>
+        <v>-58.460441</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.618934</v>
+        <v>-34.628243</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6958,27 +6958,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>-557</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>Av Castañares 4621</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>ICD30462144</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Colocar columna para pedir traspaso de nodo telecom</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7001,12 +7001,12 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L87" t="inlineStr">
@@ -7015,10 +7015,10 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.460441</v>
+        <v>-58.470977</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.628243</v>
+        <v>-34.665358</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7034,27 +7034,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-557</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Av Castañares 4621</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>ICD30462144</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7069,7 +7069,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo telecom</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7082,19 +7082,19 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.470977</v>
+        <v>-58.435017</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.665358</v>
+        <v>-34.622044</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -7110,27 +7110,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>-563</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Av Castañares 4520</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>809157022</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7145,7 +7145,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Cambiar pasante</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7167,14 +7167,14 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.470249</v>
+        <v>-58.373428</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.664835</v>
+        <v>-34.63705</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-27 15:04:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6426,7 +6426,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6469</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6436,17 +6436,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>USPALLATA 3626</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808733910</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6483,10 +6483,10 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.414389</v>
+        <v>-58.468841</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.641308</v>
+        <v>-34.686635</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -6502,7 +6502,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6512,17 +6512,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6545,7 +6545,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6559,14 +6559,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.468841</v>
+        <v>-58.375684</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.686635</v>
+        <v>-34.656092</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6578,27 +6578,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>-549</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>14 de Julio 65</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808749189</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6621,7 +6621,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -6635,46 +6635,46 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.375684</v>
+        <v>-58.468496</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.656092</v>
+        <v>-34.591282</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6711,46 +6711,46 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.468496</v>
+        <v>-58.460818</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.591282</v>
+        <v>-34.618934</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6947</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>ALMAFUERTE AV. 682</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808972978</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6787,14 +6787,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.414185</v>
+        <v>-58.460441</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.64524</v>
+        <v>-34.628243</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6806,27 +6806,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>-557</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>Av Castañares 4621</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>ICD30462144</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de nodo telecom</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6854,7 +6854,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
@@ -6863,10 +6863,10 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.460818</v>
+        <v>-58.470977</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.618934</v>
+        <v>-34.665358</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -6882,27 +6882,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6925,24 +6925,24 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.460441</v>
+        <v>-58.435017</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.628243</v>
+        <v>-34.622044</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6958,27 +6958,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-557</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Av Castañares 4621</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>ICD30462144</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo telecom</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7006,7 +7006,7 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L87" t="inlineStr">
@@ -7015,14 +7015,14 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.470977</v>
+        <v>-58.373428</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.665358</v>
+        <v>-34.63705</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -7034,7 +7034,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7044,17 +7044,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7069,7 +7069,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7082,104 +7082,28 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.435017</v>
+        <v>-58.488424</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.622044</v>
+        <v>-34.642002</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>7060</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>8/26/2025</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>PINZON 1578</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>809195671</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M89" t="n">
-        <v>-58.373428</v>
-      </c>
-      <c r="N89" t="n">
-        <v>-34.63705</v>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-28 07:05:58)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -6806,7 +6806,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-557</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6816,7 +6816,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Av Castañares 4621</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -6826,7 +6826,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>ICD30462144</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6836,12 +6836,12 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo telecom</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6857,16 +6857,12 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L85" t="inlineStr"/>
       <c r="M85" t="n">
-        <v>-58.470977</v>
+        <v>-58.470919</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.665358</v>
+        <v>-34.665309</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-29 08:11:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7103,6 +7103,158 @@
         </is>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>7091</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>SUAREZ AV. 1966</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>809279022</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.377974</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.641024</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>7096</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>VEDIA, AGUSTIN DE 2185</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>809279069</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>-58.435511</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.644702</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-30 08:22:16)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4150,7 +4150,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4207,14 +4207,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.46579</v>
+        <v>-58.451835</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.555012</v>
+        <v>-34.562646</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4226,7 +4226,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4236,17 +4236,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4279,18 +4279,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.451835</v>
+        <v>-58.470837</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.562646</v>
+        <v>-34.545751</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,7 +4302,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4312,7 +4312,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4322,7 +4322,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4350,19 +4350,19 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4378,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4421,12 +4421,12 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4435,10 +4435,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4454,7 +4454,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,17 +4464,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,26 +4511,26 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,17 +4540,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4583,30 +4583,30 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4616,17 +4616,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4659,50 +4659,50 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,11 +4717,11 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -4739,46 +4739,46 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.412302</v>
+        <v>-58.485056</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.59301</v>
+        <v>-34.555059</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,15 +4793,15 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4815,14 +4815,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.485056</v>
+        <v>-58.469783</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.555059</v>
+        <v>-34.599214</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4834,27 +4834,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4887,50 +4887,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.469783</v>
+        <v>-58.487144</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.599214</v>
+        <v>-34.669078</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4963,50 +4963,50 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.487144</v>
+        <v>-58.49147</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.669078</v>
+        <v>-34.55031</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5019,11 +5019,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H61" t="inlineStr"/>
       <c r="I61" t="n">
         <v>1</v>
       </c>
@@ -5043,36 +5039,36 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.49147</v>
+        <v>-58.405761</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.55031</v>
+        <v>-34.582476</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5082,7 +5078,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5095,7 +5091,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr"/>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I62" t="n">
         <v>1</v>
       </c>
@@ -5115,14 +5115,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5134,7 +5134,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5144,7 +5144,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5154,7 +5154,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5191,10 +5191,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5210,27 +5210,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5263,18 +5263,18 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,7 +5286,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5296,17 +5296,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5339,30 +5339,30 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.472311</v>
+        <v>-58.450113</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.654867</v>
+        <v>-34.574534</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5372,17 +5372,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5415,18 +5415,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.450113</v>
+        <v>-58.484729</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.574534</v>
+        <v>-34.574614</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6942</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>3 DE FEBRERO 2169</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5491,18 +5491,18 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.484729</v>
+        <v>-58.452583</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.574614</v>
+        <v>-34.558668</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5514,27 +5514,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6942</t>
+          <t>6409</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 2169</t>
+          <t>CASTAÑARES AV. 5656</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Faltan cargar las fotos del cierre</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5567,50 +5567,50 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.452583</v>
+        <v>-58.479921</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.558668</v>
+        <v>-34.673021</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6409</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 5656</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Faltan cargar las fotos del cierre</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5643,50 +5643,50 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.479921</v>
+        <v>-58.510247</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.673021</v>
+        <v>-34.645038</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5719,18 +5719,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.510247</v>
+        <v>-58.483145</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.645038</v>
+        <v>-34.557043</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5742,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5799,14 +5799,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.483145</v>
+        <v>-58.496608</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.557043</v>
+        <v>-34.666371</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5818,27 +5818,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5875,46 +5875,46 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.496608</v>
+        <v>-58.422229</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.666371</v>
+        <v>-34.573148</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6481</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>DIAZ, CESAR, GRAL. 3520</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808703875</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5929,7 +5929,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5951,26 +5951,26 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.422229</v>
+        <v>-58.486002</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.573148</v>
+        <v>-34.61821</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6481</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5980,17 +5980,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>DIAZ, CESAR, GRAL. 3520</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808703875</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6023,50 +6023,50 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.486002</v>
+        <v>-58.494864</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.61821</v>
+        <v>-34.678826</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6099,50 +6099,50 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.494864</v>
+        <v>-58.473089</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.678826</v>
+        <v>-34.625478</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6157,7 +6157,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6179,26 +6179,26 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.473089</v>
+        <v>-58.468841</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.625478</v>
+        <v>-34.686635</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6208,17 +6208,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6255,14 +6255,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.468841</v>
+        <v>-58.375684</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.686635</v>
+        <v>-34.656092</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6274,27 +6274,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>-549</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>14 de Julio 65</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808749189</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6331,46 +6331,46 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.375684</v>
+        <v>-58.468496</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.656092</v>
+        <v>-34.591282</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6385,7 +6385,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6407,36 +6407,36 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.468496</v>
+        <v>-58.460818</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.591282</v>
+        <v>-34.618934</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6483,10 +6483,10 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.460818</v>
+        <v>-58.460441</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.618934</v>
+        <v>-34.628243</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -6502,27 +6502,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6532,12 +6532,12 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6545,24 +6545,20 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr"/>
       <c r="M81" t="n">
-        <v>-58.460441</v>
+        <v>-58.470919</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.628243</v>
+        <v>-34.665309</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6578,27 +6574,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6608,12 +6604,12 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6626,15 +6622,19 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr"/>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M82" t="n">
-        <v>-58.470919</v>
+        <v>-58.435017</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.665309</v>
+        <v>-34.622044</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6650,7 +6650,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6660,17 +6660,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6698,23 +6698,23 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.435017</v>
+        <v>-58.373428</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.622044</v>
+        <v>-34.63705</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6726,7 +6726,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6736,17 +6736,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6783,46 +6783,46 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.373428</v>
+        <v>-58.488424</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.63705</v>
+        <v>-34.642002</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6837,7 +6837,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6855,40 +6855,40 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.488424</v>
+        <v>-58.37456</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.642002</v>
+        <v>-34.649779</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -6898,7 +6898,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6931,14 +6931,14 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.37456</v>
+        <v>-58.37805</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.649779</v>
+        <v>-34.649722</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6954,17 +6954,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -6974,7 +6974,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7011,10 +7011,10 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.37805</v>
+        <v>-58.378104</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.649722</v>
+        <v>-34.649578</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7030,7 +7030,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7040,7 +7040,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -7050,7 +7050,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7087,10 +7087,10 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.378104</v>
+        <v>-58.377974</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.649578</v>
+        <v>-34.641024</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -7106,7 +7106,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -7116,17 +7116,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7163,93 +7163,17 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.377974</v>
+        <v>-58.435511</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.641024</v>
+        <v>-34.644702</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>7096</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>8/28/2025</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>809279069</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I90" t="n">
-        <v>1</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M90" t="n">
-        <v>-58.435511</v>
-      </c>
-      <c r="N90" t="n">
-        <v>-34.644702</v>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P90" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-30 11:05:38)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1946,7 +1946,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>6901</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1956,17 +1956,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PINO, Virrey del 2644</t>
+          <t>COCHABAMBA /ALT/ 1790</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>803608215</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,11 +1981,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>SIN RIEGO</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2003,46 +2003,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.455073</v>
+        <v>-58.391153</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.56776</v>
+        <v>-34.624022</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>-281</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>COCHABAMBA /ALT/ 1790</t>
+          <t>SOLER /ALT/ 4517</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>803651203</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>SIN RIEGO</t>
+          <t>columna de 114 con nodo y redes nuestra.</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2079,14 +2079,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.391153</v>
+        <v>-58.423405</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.624022</v>
+        <v>-34.588075</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2098,17 +2098,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-281</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SOLER /ALT/ 4517</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2118,7 +2118,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803651203</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,11 +2133,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>columna de 114 con nodo y redes nuestra.</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2146,19 +2146,19 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.423405</v>
+        <v>-58.42486</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.588075</v>
+        <v>-34.577318</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2174,27 +2174,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2222,35 +2222,35 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.42486</v>
+        <v>-58.491074</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.577318</v>
+        <v>-34.575623</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2260,17 +2260,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,12 +2293,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2307,14 +2307,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.491074</v>
+        <v>-58.525125</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.575623</v>
+        <v>-34.604668</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2326,27 +2326,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2383,26 +2383,26 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.525125</v>
+        <v>-58.421964</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.604668</v>
+        <v>-34.586342</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2412,17 +2412,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2459,26 +2459,26 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.421964</v>
+        <v>-58.498493</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.586342</v>
+        <v>-34.581262</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-340</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,17 +2488,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>SUPERI /ALT/ 1445</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804838869</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2535,14 +2535,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.498493</v>
+        <v>-58.460666</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.581262</v>
+        <v>-34.573823</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2554,27 +2554,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-340</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>SUPERI /ALT/ 1445</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804838869</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,11 +2589,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2611,14 +2611,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.460666</v>
+        <v>-58.502447</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.573823</v>
+        <v>-34.561008</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2630,7 +2630,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2640,17 +2640,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2687,10 +2687,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.502447</v>
+        <v>-58.483947</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.561008</v>
+        <v>-34.583207</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2706,7 +2706,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2716,17 +2716,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2759,14 +2759,14 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.483947</v>
+        <v>-58.503673</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.583207</v>
+        <v>-34.586925</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,14 +2835,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.503673</v>
+        <v>-58.504455</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.586925</v>
+        <v>-34.579941</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2858,7 +2858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-355</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>CUENCA /ALT/ 4480</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839675</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente TLC</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2915,10 +2915,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.504455</v>
+        <v>-58.504568</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.579941</v>
+        <v>-34.590534</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2934,7 +2934,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-355</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 4480</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804839675</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2982,7 +2982,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2991,10 +2991,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.504568</v>
+        <v>-58.503195</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.590534</v>
+        <v>-34.581735</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3010,7 +3010,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3067,14 +3067,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.503195</v>
+        <v>-58.493164</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.581735</v>
+        <v>-34.55732</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,7 +3086,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3106,7 +3106,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3143,14 +3143,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.493164</v>
+        <v>-58.491934</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.55732</v>
+        <v>-34.569348</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3162,7 +3162,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3172,7 +3172,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3219,10 +3219,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.491934</v>
+        <v>-58.501418</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.569348</v>
+        <v>-34.574363</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3238,7 +3238,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3295,14 +3295,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.501418</v>
+        <v>-58.494584</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.574363</v>
+        <v>-34.554981</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3314,27 +3314,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,11 +3349,11 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3367,14 +3367,14 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.494584</v>
+        <v>-58.465608</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.554981</v>
+        <v>-34.538489</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3443,18 +3443,18 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.465608</v>
+        <v>-58.436788</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.538489</v>
+        <v>-34.604014</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3466,7 +3466,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3476,17 +3476,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3523,26 +3523,26 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.436788</v>
+        <v>-58.439461</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.604014</v>
+        <v>-34.605744</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3552,17 +3552,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3599,10 +3599,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.439461</v>
+        <v>-58.418424</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.605744</v>
+        <v>-34.604463</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>7054</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,7 +3628,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>HUMAHUACA 3918</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>804903788</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3675,10 +3675,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.418424</v>
+        <v>-58.419694</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.604463</v>
+        <v>-34.602062</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,27 +3694,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>7054</t>
+          <t>-383</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HUMAHUACA 3918</t>
+          <t>VALDERRAMA /ALT/ 4187</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804903788</t>
+          <t>805507401</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t xml:space="preserve">Aplomar columna 114 </t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3751,26 +3751,26 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.419694</v>
+        <v>-58.481834</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.602062</v>
+        <v>-34.560796</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-383</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3780,17 +3780,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>VALDERRAMA /ALT/ 4187</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805507401</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114 </t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3827,14 +3827,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.481834</v>
+        <v>-58.473936</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.560796</v>
+        <v>-34.577346</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3846,7 +3846,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-385</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,17 +3856,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>MOLDES /ALT/ 1913</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805507415</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.473936</v>
+        <v>-58.45789</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.577346</v>
+        <v>-34.565423</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-385</t>
+          <t>-386</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,7 +3932,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1913</t>
+          <t>MOLDES /ALT/ 1943</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805507415</t>
+          <t>805507419</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3970,7 +3970,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3979,10 +3979,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.45789</v>
+        <v>-58.458217</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.565423</v>
+        <v>-34.565043</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3998,27 +3998,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-386</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1943</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805507419</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4041,12 +4041,12 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4055,46 +4055,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.458217</v>
+        <v>-58.387847</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.565043</v>
+        <v>-34.587043</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4131,26 +4131,26 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.387847</v>
+        <v>-58.451835</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.587043</v>
+        <v>-34.562646</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4160,17 +4160,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4203,18 +4203,18 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.451835</v>
+        <v>-58.470837</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.562646</v>
+        <v>-34.545751</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4226,7 +4226,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4246,7 +4246,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4274,19 +4274,19 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4345,12 +4345,12 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4359,10 +4359,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4388,17 +4388,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4435,26 +4435,26 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,17 +4464,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4507,30 +4507,30 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4540,17 +4540,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4583,50 +4583,50 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,11 +4641,11 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -4663,46 +4663,46 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.412302</v>
+        <v>-58.485056</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.59301</v>
+        <v>-34.555059</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,15 +4717,15 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4739,14 +4739,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.485056</v>
+        <v>-58.469783</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.555059</v>
+        <v>-34.599214</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4758,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4811,50 +4811,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.469783</v>
+        <v>-58.487144</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.599214</v>
+        <v>-34.669078</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4887,50 +4887,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.487144</v>
+        <v>-58.49147</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.669078</v>
+        <v>-34.55031</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4943,11 +4943,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H60" t="inlineStr"/>
       <c r="I60" t="n">
         <v>1</v>
       </c>
@@ -4967,36 +4963,36 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.49147</v>
+        <v>-58.405761</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.55031</v>
+        <v>-34.582476</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5006,7 +5002,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5019,7 +5015,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr"/>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I61" t="n">
         <v>1</v>
       </c>
@@ -5039,14 +5039,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5058,7 +5058,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5068,7 +5068,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5078,7 +5078,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5115,10 +5115,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5134,27 +5134,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5187,18 +5187,18 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5210,7 +5210,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5220,17 +5220,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5263,30 +5263,30 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.472311</v>
+        <v>-58.450113</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.654867</v>
+        <v>-34.574534</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5296,17 +5296,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5339,18 +5339,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.450113</v>
+        <v>-58.484729</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.574534</v>
+        <v>-34.574614</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5362,27 +5362,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6942</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>3 DE FEBRERO 2169</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5415,18 +5415,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.484729</v>
+        <v>-58.452583</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.574614</v>
+        <v>-34.558668</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6942</t>
+          <t>6409</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 2169</t>
+          <t>CASTAÑARES AV. 5656</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Faltan cargar las fotos del cierre</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5491,50 +5491,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.452583</v>
+        <v>-58.479921</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.558668</v>
+        <v>-34.673021</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6409</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 5656</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Faltan cargar las fotos del cierre</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5567,50 +5567,50 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.479921</v>
+        <v>-58.510247</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.673021</v>
+        <v>-34.645038</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5643,18 +5643,18 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.510247</v>
+        <v>-58.483145</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.645038</v>
+        <v>-34.557043</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5666,27 +5666,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5723,14 +5723,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.483145</v>
+        <v>-58.496608</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.557043</v>
+        <v>-34.666371</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5742,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5799,46 +5799,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.496608</v>
+        <v>-58.422229</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.666371</v>
+        <v>-34.573148</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6481</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>DIAZ, CESAR, GRAL. 3520</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808703875</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5875,26 +5875,26 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.422229</v>
+        <v>-58.486002</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.573148</v>
+        <v>-34.61821</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6481</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5904,17 +5904,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>DIAZ, CESAR, GRAL. 3520</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808703875</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5929,7 +5929,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5947,50 +5947,50 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.486002</v>
+        <v>-58.494864</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.61821</v>
+        <v>-34.678826</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6023,50 +6023,50 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.494864</v>
+        <v>-58.473089</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.678826</v>
+        <v>-34.625478</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6103,26 +6103,26 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.473089</v>
+        <v>-58.468841</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.625478</v>
+        <v>-34.686635</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6132,17 +6132,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6157,7 +6157,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6165,7 +6165,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -6179,14 +6179,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.468841</v>
+        <v>-58.375684</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.686635</v>
+        <v>-34.656092</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6198,27 +6198,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>-549</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>14 de Julio 65</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808749189</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6255,46 +6255,46 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.375684</v>
+        <v>-58.468496</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.656092</v>
+        <v>-34.591282</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6331,36 +6331,36 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.468496</v>
+        <v>-58.460818</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.591282</v>
+        <v>-34.618934</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6370,7 +6370,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6385,7 +6385,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6393,7 +6393,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6407,10 +6407,10 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.460818</v>
+        <v>-58.460441</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.618934</v>
+        <v>-34.628243</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -6426,27 +6426,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6456,12 +6456,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6469,24 +6469,20 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr"/>
       <c r="M80" t="n">
-        <v>-58.460441</v>
+        <v>-58.470919</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.628243</v>
+        <v>-34.665309</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -6502,27 +6498,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6532,12 +6528,12 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6550,15 +6546,19 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr"/>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M81" t="n">
-        <v>-58.470919</v>
+        <v>-58.435017</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.665309</v>
+        <v>-34.622044</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6574,7 +6574,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6584,17 +6584,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6622,23 +6622,23 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.435017</v>
+        <v>-58.373428</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.622044</v>
+        <v>-34.63705</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6650,7 +6650,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6660,17 +6660,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6707,46 +6707,46 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.373428</v>
+        <v>-58.488424</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.63705</v>
+        <v>-34.642002</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6779,40 +6779,40 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.488424</v>
+        <v>-58.37456</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.642002</v>
+        <v>-34.649779</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -6822,7 +6822,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6855,14 +6855,14 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.37456</v>
+        <v>-58.37805</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.649779</v>
+        <v>-34.649722</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -6878,17 +6878,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -6898,7 +6898,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6935,10 +6935,10 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.37805</v>
+        <v>-58.378104</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.649722</v>
+        <v>-34.649578</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6954,7 +6954,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -6964,7 +6964,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -6974,7 +6974,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7011,10 +7011,10 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.378104</v>
+        <v>-58.377974</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.649578</v>
+        <v>-34.641024</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7030,7 +7030,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7040,17 +7040,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7087,93 +7087,17 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.377974</v>
+        <v>-58.435511</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.641024</v>
+        <v>-34.644702</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>7096</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>8/28/2025</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>809279069</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M89" t="n">
-        <v>-58.435511</v>
-      </c>
-      <c r="N89" t="n">
-        <v>-34.644702</v>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-01 14:41:04)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3846,7 +3846,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-385</t>
+          <t>-386</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,7 +3856,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1913</t>
+          <t>MOLDES /ALT/ 1943</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805507415</t>
+          <t>805507419</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3894,7 +3894,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.45789</v>
+        <v>-58.458217</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.565423</v>
+        <v>-34.565043</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,27 +3922,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-386</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1943</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805507419</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3965,12 +3965,12 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3979,46 +3979,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.458217</v>
+        <v>-58.387847</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.565043</v>
+        <v>-34.587043</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4055,26 +4055,26 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.387847</v>
+        <v>-58.451835</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.587043</v>
+        <v>-34.562646</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4084,17 +4084,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4127,18 +4127,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.451835</v>
+        <v>-58.470837</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.562646</v>
+        <v>-34.545751</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4150,7 +4150,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4198,19 +4198,19 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4226,27 +4226,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4269,12 +4269,12 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4283,10 +4283,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4302,7 +4302,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4312,17 +4312,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,26 +4359,26 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4388,17 +4388,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4431,30 +4431,30 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4464,17 +4464,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4507,50 +4507,50 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,11 +4565,11 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -4587,46 +4587,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.412302</v>
+        <v>-58.485056</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.59301</v>
+        <v>-34.555059</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,15 +4641,15 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4663,14 +4663,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.485056</v>
+        <v>-58.469783</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.555059</v>
+        <v>-34.599214</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4682,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4735,50 +4735,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.469783</v>
+        <v>-58.487144</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.599214</v>
+        <v>-34.669078</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4811,50 +4811,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.487144</v>
+        <v>-58.49147</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.669078</v>
+        <v>-34.55031</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4867,11 +4867,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Inclinada</t>
-        </is>
-      </c>
+      <c r="H59" t="inlineStr"/>
       <c r="I59" t="n">
         <v>1</v>
       </c>
@@ -4891,36 +4887,36 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.49147</v>
+        <v>-58.405761</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.55031</v>
+        <v>-34.582476</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4930,7 +4926,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4943,7 +4939,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I60" t="n">
         <v>1</v>
       </c>
@@ -4963,14 +4963,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4982,7 +4982,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4992,7 +4992,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5002,7 +5002,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5039,10 +5039,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5058,27 +5058,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5111,18 +5111,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5134,7 +5134,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5144,17 +5144,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5187,30 +5187,30 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.472311</v>
+        <v>-58.450113</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.654867</v>
+        <v>-34.574534</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5220,17 +5220,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5263,18 +5263,18 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.450113</v>
+        <v>-58.484729</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.574534</v>
+        <v>-34.574614</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6942</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>3 DE FEBRERO 2169</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5339,18 +5339,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.484729</v>
+        <v>-58.452583</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.574614</v>
+        <v>-34.558668</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5362,27 +5362,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6942</t>
+          <t>6409</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 2169</t>
+          <t>CASTAÑARES AV. 5656</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Faltan cargar las fotos del cierre</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5415,50 +5415,50 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.452583</v>
+        <v>-58.479921</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.558668</v>
+        <v>-34.673021</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6409</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 5656</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Faltan cargar las fotos del cierre</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5491,50 +5491,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.479921</v>
+        <v>-58.510247</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.673021</v>
+        <v>-34.645038</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5567,18 +5567,18 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.510247</v>
+        <v>-58.483145</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.645038</v>
+        <v>-34.557043</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5590,27 +5590,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5647,14 +5647,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.483145</v>
+        <v>-58.496608</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.557043</v>
+        <v>-34.666371</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5666,27 +5666,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5723,46 +5723,46 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.496608</v>
+        <v>-58.422229</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.666371</v>
+        <v>-34.573148</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5795,18 +5795,18 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.422229</v>
+        <v>-58.494864</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.573148</v>
+        <v>-34.678826</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5818,27 +5818,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6481</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>DIAZ, CESAR, GRAL. 3520</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808703875</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5875,10 +5875,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.486002</v>
+        <v>-58.473089</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.61821</v>
+        <v>-34.625478</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5894,17 +5894,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -5914,7 +5914,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5929,7 +5929,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5947,14 +5947,14 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.494864</v>
+        <v>-58.468841</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.678826</v>
+        <v>-34.686635</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -5970,27 +5970,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6027,46 +6027,46 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.473089</v>
+        <v>-58.375684</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.625478</v>
+        <v>-34.656092</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>-549</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>14 de Julio 65</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808749189</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6103,46 +6103,46 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.468841</v>
+        <v>-58.468496</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.686635</v>
+        <v>-34.591282</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6157,7 +6157,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6165,7 +6165,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -6179,14 +6179,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.375684</v>
+        <v>-58.460818</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.656092</v>
+        <v>-34.618934</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6198,27 +6198,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6255,46 +6255,46 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.468496</v>
+        <v>-58.460441</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.591282</v>
+        <v>-34.628243</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6304,12 +6304,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6322,19 +6322,15 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr"/>
       <c r="M78" t="n">
-        <v>-58.460818</v>
+        <v>-58.470919</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.618934</v>
+        <v>-34.665309</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6350,27 +6346,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6385,7 +6381,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6393,24 +6389,24 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.460441</v>
+        <v>-58.435017</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.628243</v>
+        <v>-34.622044</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -6426,27 +6422,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6456,12 +6452,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6474,19 +6470,23 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M80" t="n">
-        <v>-58.470919</v>
+        <v>-58.373428</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.665309</v>
+        <v>-34.63705</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6498,7 +6498,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6508,17 +6508,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6533,7 +6533,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6546,45 +6546,45 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.435017</v>
+        <v>-58.488424</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.622044</v>
+        <v>-34.642002</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6594,7 +6594,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6627,14 +6627,14 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.373428</v>
+        <v>-58.37456</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.63705</v>
+        <v>-34.649779</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6650,27 +6650,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6707,26 +6707,26 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.488424</v>
+        <v>-58.37805</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.642002</v>
+        <v>-34.649722</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6736,7 +6736,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6746,7 +6746,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6779,14 +6779,14 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.37456</v>
+        <v>-58.378104</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.649779</v>
+        <v>-34.649578</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -6802,17 +6802,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -6822,7 +6822,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6859,10 +6859,10 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.37805</v>
+        <v>-58.377974</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.649722</v>
+        <v>-34.641024</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -6878,7 +6878,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -6888,17 +6888,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6935,14 +6935,14 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.378104</v>
+        <v>-58.435511</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.649578</v>
+        <v>-34.644702</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6954,27 +6954,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7106</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>MARTI, JOSE 627</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809371835</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6989,7 +6989,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7011,93 +7011,17 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.377974</v>
+        <v>-58.469159</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.641024</v>
+        <v>-34.638898</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>7096</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>8/28/2025</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>809279069</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I88" t="n">
-        <v>1</v>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M88" t="n">
-        <v>-58.435511</v>
-      </c>
-      <c r="N88" t="n">
-        <v>-34.644702</v>
-      </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P88" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 08:12:48)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6346,7 +6346,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6356,17 +6356,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6381,7 +6381,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6394,23 +6394,23 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.435017</v>
+        <v>-58.373428</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.622044</v>
+        <v>-34.63705</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6422,7 +6422,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6432,17 +6432,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6457,7 +6457,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6479,46 +6479,46 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.373428</v>
+        <v>-58.488424</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.63705</v>
+        <v>-34.642002</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6533,7 +6533,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6551,40 +6551,40 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.488424</v>
+        <v>-58.37456</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.642002</v>
+        <v>-34.649779</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6594,7 +6594,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6627,14 +6627,14 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.37456</v>
+        <v>-58.37805</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.649779</v>
+        <v>-34.649722</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6650,17 +6650,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -6670,7 +6670,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6707,10 +6707,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.37805</v>
+        <v>-58.378104</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.649722</v>
+        <v>-34.649578</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6726,7 +6726,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6736,7 +6736,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6746,7 +6746,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6783,10 +6783,10 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.378104</v>
+        <v>-58.377974</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.649578</v>
+        <v>-34.641024</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -6802,7 +6802,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6812,17 +6812,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6859,14 +6859,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.377974</v>
+        <v>-58.435511</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.641024</v>
+        <v>-34.644702</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6878,17 +6878,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>7106</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>MARTI, JOSE 627</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -6898,7 +6898,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809371835</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6913,7 +6913,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6935,10 +6935,10 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.435511</v>
+        <v>-58.469159</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.644702</v>
+        <v>-34.638898</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6946,82 +6946,6 @@
         </is>
       </c>
       <c r="P86" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>7106</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>9/1/2025</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>MARTI, JOSE 627</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>809371835</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M87" t="n">
-        <v>-58.469159</v>
-      </c>
-      <c r="N87" t="n">
-        <v>-34.638898</v>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 18:47:45)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6951,6 +6951,82 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>4088</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>9/2/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>GOMEZ, VALENTIN 3648</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>809406164</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>-58.416416</v>
+      </c>
+      <c r="N87" t="n">
+        <v>-34.604812</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-03 06:47:27)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1342,7 +1342,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-193</t>
+          <t>-201</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1352,17 +1352,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>WASHINGTON /ALT/ 3251</t>
+          <t>MIGUELETES /ALT/ 1007</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>799539971</t>
+          <t>799540497</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1377,7 +1377,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Washington 3251 cambiar columna de 114 transferir tendidos. dejar pasivos en norma</t>
+          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1395,30 +1395,30 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.478272</v>
+        <v>-58.436377</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.558899</v>
+        <v>-34.565075</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-201</t>
+          <t>-202</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1007</t>
+          <t>MIGUELETES /ALT/ 1030</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>799540497</t>
+          <t>799540503</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
+          <t>Recambio de columna - alt correcta 1010</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1475,10 +1475,10 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.436377</v>
+        <v>-58.436601</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.565075</v>
+        <v>-34.565035</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1494,17 +1494,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-202</t>
+          <t>-216</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>5/2/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1030</t>
+          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>799540503</t>
+          <t>784655947</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Recambio de columna - alt correcta 1010</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1547,18 +1547,18 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.436601</v>
+        <v>-58.404652</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.565035</v>
+        <v>-34.58263</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1570,27 +1570,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>-216</t>
+          <t>-219</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5/2/2024</t>
+          <t>10/31/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
+          <t>LA PAMPA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>784655947</t>
+          <t>798953875</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1627,46 +1627,46 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.404652</v>
+        <v>-58.458282</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.58263</v>
+        <v>-34.56718</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-219</t>
+          <t>-228</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10/31/2024</t>
+          <t>11/22/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LA PAMPA /ALT/ 2836</t>
+          <t>ALVAREZ JULIAN /ALT/ 1272</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>798953875</t>
+          <t>800645527</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1703,46 +1703,46 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.458282</v>
+        <v>-58.426725</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.56718</v>
+        <v>-34.5945</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-226</t>
+          <t>-254</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/20/2024</t>
+          <t>1/7/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CUBA /ALT/ 2308</t>
+          <t>BELAUSTEGUI DR LUIS /ALT/ 1185</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>800502281</t>
+          <t>802367713</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1755,13 +1755,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1770,7 +1766,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1779,14 +1775,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.456674</v>
+        <v>-58.457158</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.558757</v>
+        <v>-34.605839</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1798,27 +1794,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-228</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/22/2024</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ALVAREZ JULIAN /ALT/ 1272</t>
+          <t>COCHABAMBA /ALT/ 1790</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>800645527</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1833,7 +1829,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>SIN RIEGO</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1846,7 +1842,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1855,14 +1851,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.426725</v>
+        <v>-58.391153</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.5945</v>
+        <v>-34.624022</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1874,27 +1870,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-254</t>
+          <t>-281</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1/7/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BELAUSTEGUI DR LUIS /ALT/ 1185</t>
+          <t>SOLER /ALT/ 4517</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>802367713</t>
+          <t>803651203</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1907,9 +1903,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>columna de 114 con nodo y redes nuestra.</t>
+        </is>
+      </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1927,46 +1927,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.457158</v>
+        <v>-58.423405</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.605839</v>
+        <v>-34.588075</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>COCHABAMBA /ALT/ 1790</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,11 +1981,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>SIN RIEGO</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1994,23 +1994,23 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.391153</v>
+        <v>-58.42486</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.624022</v>
+        <v>-34.577318</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2022,27 +2022,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-281</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>SOLER /ALT/ 4517</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803651203</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2057,11 +2057,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>columna de 114 con nodo y redes nuestra.</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2079,46 +2079,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.423405</v>
+        <v>-58.491074</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.588075</v>
+        <v>-34.575623</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2151,50 +2151,50 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.42486</v>
+        <v>-58.525125</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.577318</v>
+        <v>-34.604668</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2222,7 +2222,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2231,46 +2231,46 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.491074</v>
+        <v>-58.421964</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.575623</v>
+        <v>-34.586342</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2307,14 +2307,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.525125</v>
+        <v>-58.498493</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.604668</v>
+        <v>-34.581262</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2326,7 +2326,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-340</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2336,17 +2336,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>SUPERI /ALT/ 1445</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804838869</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2383,36 +2383,36 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.421964</v>
+        <v>-58.460666</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.586342</v>
+        <v>-34.573823</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,15 +2437,15 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2459,10 +2459,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.498493</v>
+        <v>-58.502447</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.581262</v>
+        <v>-34.561008</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2478,27 +2478,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-340</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>SUPERI /ALT/ 1445</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804838869</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,15 +2513,15 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2535,14 +2535,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.460666</v>
+        <v>-58.483947</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.573823</v>
+        <v>-34.583207</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2554,7 +2554,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2607,14 +2607,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.502447</v>
+        <v>-58.503673</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.561008</v>
+        <v>-34.586925</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2630,7 +2630,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2640,17 +2640,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2687,10 +2687,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.483947</v>
+        <v>-58.504455</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.583207</v>
+        <v>-34.579941</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2706,7 +2706,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-355</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>CUENCA /ALT/ 4480</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839675</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2749,24 +2749,24 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente TLC</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.503673</v>
+        <v>-58.504568</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.586925</v>
+        <v>-34.590534</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2839,10 +2839,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.504455</v>
+        <v>-58.503195</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.579941</v>
+        <v>-34.581735</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2858,7 +2858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-355</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 4480</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804839675</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2915,14 +2915,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.504568</v>
+        <v>-58.493164</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.590534</v>
+        <v>-34.55732</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2934,7 +2934,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2991,10 +2991,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.503195</v>
+        <v>-58.491934</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.581735</v>
+        <v>-34.569348</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3010,7 +3010,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3067,14 +3067,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.493164</v>
+        <v>-58.501418</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.55732</v>
+        <v>-34.574363</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,7 +3086,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3106,7 +3106,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3143,14 +3143,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.491934</v>
+        <v>-58.494584</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.569348</v>
+        <v>-34.554981</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3162,27 +3162,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,11 +3197,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3215,18 +3215,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.501418</v>
+        <v>-58.465608</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.574363</v>
+        <v>-34.538489</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3238,27 +3238,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,15 +3273,15 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3295,14 +3295,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.494584</v>
+        <v>-58.436788</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.554981</v>
+        <v>-34.604014</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3314,27 +3314,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3367,30 +3367,30 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.465608</v>
+        <v>-58.439461</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.538489</v>
+        <v>-34.605744</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3400,17 +3400,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3447,26 +3447,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.436788</v>
+        <v>-58.418424</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.604014</v>
+        <v>-34.604463</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>7054</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3476,17 +3476,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>HUMAHUACA 3918</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903788</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3523,10 +3523,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.439461</v>
+        <v>-58.419694</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.605744</v>
+        <v>-34.602062</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3542,27 +3542,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>-383</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>VALDERRAMA /ALT/ 4187</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>805507401</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 114 </t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3599,46 +3599,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.418424</v>
+        <v>-58.481834</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.604463</v>
+        <v>-34.560796</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>7054</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>HUMAHUACA 3918</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804903788</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3675,26 +3675,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.419694</v>
+        <v>-58.473936</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.602062</v>
+        <v>-34.577346</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-383</t>
+          <t>-386</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +3704,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>VALDERRAMA /ALT/ 4187</t>
+          <t>MOLDES /ALT/ 1943</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805507401</t>
+          <t>805507419</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114 </t>
+          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3742,7 +3742,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3751,14 +3751,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.481834</v>
+        <v>-58.458217</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.560796</v>
+        <v>-34.565043</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3770,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3827,36 +3827,36 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.473936</v>
+        <v>-58.387847</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.577346</v>
+        <v>-34.587043</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-386</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1943</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805507419</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3889,12 +3889,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.458217</v>
+        <v>-58.451835</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.565043</v>
+        <v>-34.562646</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,27 +3922,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3975,30 +3975,30 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.387847</v>
+        <v>-58.470837</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.587043</v>
+        <v>-34.545751</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,17 +4008,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4041,12 +4041,12 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4055,14 +4055,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.451835</v>
+        <v>-58.472267</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.562646</v>
+        <v>-34.551163</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4074,27 +4074,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4127,14 +4127,14 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.470837</v>
+        <v>-58.464144</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.545751</v>
+        <v>-34.541832</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4150,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4193,12 +4193,12 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4207,26 +4207,26 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.472267</v>
+        <v>-58.434761</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.551163</v>
+        <v>-34.598381</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4246,7 +4246,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4279,14 +4279,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.464144</v>
+        <v>-58.464177</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.541832</v>
+        <v>-34.558239</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4302,7 +4302,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4312,17 +4312,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,14 +4359,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.434761</v>
+        <v>-58.412302</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.598381</v>
+        <v>-34.59301</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4378,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4413,11 +4413,11 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4431,14 +4431,14 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.464177</v>
+        <v>-58.485056</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.558239</v>
+        <v>-34.555059</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4454,27 +4454,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4511,46 +4511,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.412302</v>
+        <v>-58.469783</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.59301</v>
+        <v>-34.599214</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,15 +4565,15 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4583,50 +4583,50 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.485056</v>
+        <v>-58.487144</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.555059</v>
+        <v>-34.669078</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4649,7 +4649,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4663,14 +4663,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.469783</v>
+        <v>-58.49147</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.599214</v>
+        <v>-34.55031</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4682,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4715,17 +4715,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
-        </is>
-      </c>
+      <c r="H57" t="inlineStr"/>
       <c r="I57" t="n">
         <v>1</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4735,18 +4731,18 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.487144</v>
+        <v>-58.405761</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.669078</v>
+        <v>-34.582476</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4758,27 +4754,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4793,7 +4789,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4815,36 +4811,36 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.49147</v>
+        <v>-58.432241</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.55031</v>
+        <v>-34.56642</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4854,7 +4850,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4867,7 +4863,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+        </is>
+      </c>
       <c r="I59" t="n">
         <v>1</v>
       </c>
@@ -4887,14 +4887,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.405761</v>
+        <v>-58.417348</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.582476</v>
+        <v>-34.595467</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4906,27 +4906,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4959,18 +4959,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.432241</v>
+        <v>-58.472311</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.56642</v>
+        <v>-34.654867</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4982,27 +4982,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5039,26 +5039,26 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.417348</v>
+        <v>-58.450113</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.595467</v>
+        <v>-34.574534</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5068,17 +5068,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5111,50 +5111,50 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.472311</v>
+        <v>-58.484729</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.654867</v>
+        <v>-34.574614</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>6409</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>CASTAÑARES AV. 5656</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Faltan cargar las fotos del cierre</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5187,50 +5187,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.450113</v>
+        <v>-58.479921</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.574534</v>
+        <v>-34.673021</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5253,7 +5253,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5267,14 +5267,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.484729</v>
+        <v>-58.510247</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.574614</v>
+        <v>-34.645038</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6942</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 2169</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807789702</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5343,10 +5343,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.452583</v>
+        <v>-58.483145</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.558668</v>
+        <v>-34.557043</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5362,27 +5362,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6409</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 5656</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Faltan cargar las fotos del cierre</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5415,50 +5415,50 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.479921</v>
+        <v>-58.496608</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.673021</v>
+        <v>-34.666371</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5491,50 +5491,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.510247</v>
+        <v>-58.422229</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.645038</v>
+        <v>-34.573148</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5567,50 +5567,50 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.483145</v>
+        <v>-58.494864</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.557043</v>
+        <v>-34.678826</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5647,10 +5647,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.496608</v>
+        <v>-58.473089</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.666371</v>
+        <v>-34.625478</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -5666,27 +5666,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5723,14 +5723,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.422229</v>
+        <v>-58.468841</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.573148</v>
+        <v>-34.686635</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5742,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5795,18 +5795,18 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.494864</v>
+        <v>-58.375684</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.678826</v>
+        <v>-34.656092</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5818,27 +5818,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>-549</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>14 de Julio 65</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808749189</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5875,14 +5875,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.473089</v>
+        <v>-58.468496</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.625478</v>
+        <v>-34.591282</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5894,27 +5894,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5951,10 +5951,10 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.468841</v>
+        <v>-58.460818</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.686635</v>
+        <v>-34.618934</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -5970,27 +5970,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6005,7 +6005,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6027,14 +6027,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.375684</v>
+        <v>-58.460441</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.656092</v>
+        <v>-34.628243</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6046,27 +6046,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6076,12 +6076,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6094,55 +6094,51 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr"/>
       <c r="M75" t="n">
-        <v>-58.468496</v>
+        <v>-58.470919</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.591282</v>
+        <v>-34.665309</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6179,14 +6175,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.460818</v>
+        <v>-58.373428</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.618934</v>
+        <v>-34.63705</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6198,27 +6194,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6233,7 +6229,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6241,7 +6237,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6255,46 +6251,46 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.460441</v>
+        <v>-58.488424</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.628243</v>
+        <v>-34.642002</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6304,12 +6300,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6322,19 +6318,23 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L78" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M78" t="n">
-        <v>-58.470919</v>
+        <v>-58.37456</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.665309</v>
+        <v>-34.649779</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6346,17 +6346,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6366,7 +6366,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6381,7 +6381,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6403,10 +6403,10 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.373428</v>
+        <v>-58.37805</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.63705</v>
+        <v>-34.649722</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -6422,27 +6422,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6457,7 +6457,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6479,26 +6479,26 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.488424</v>
+        <v>-58.378104</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.642002</v>
+        <v>-34.649578</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6508,7 +6508,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -6518,7 +6518,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6551,14 +6551,14 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.37456</v>
+        <v>-58.377974</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.649779</v>
+        <v>-34.641024</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6574,27 +6574,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6631,14 +6631,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.37805</v>
+        <v>-58.435511</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.649722</v>
+        <v>-34.644702</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6650,27 +6650,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7106</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>MARTI, JOSE 627</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809371835</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6707,14 +6707,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.378104</v>
+        <v>-58.469159</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.649578</v>
+        <v>-34.638898</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6726,27 +6726,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>4088</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>GOMEZ, VALENTIN 3648</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809406164</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6783,245 +6783,17 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.377974</v>
+        <v>-58.416416</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.641024</v>
+        <v>-34.604812</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>7096</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>8/28/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>809279069</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.435511</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.644702</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>7106</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>9/1/2025</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>MARTI, JOSE 627</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>809371835</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
-        </is>
-      </c>
-      <c r="I86" t="n">
-        <v>1</v>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M86" t="n">
-        <v>-58.469159</v>
-      </c>
-      <c r="N86" t="n">
-        <v>-34.638898</v>
-      </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P86" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>4088</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>9/2/2025</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>GOMEZ, VALENTIN 3648</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>809406164</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M87" t="n">
-        <v>-58.416416</v>
-      </c>
-      <c r="N87" t="n">
-        <v>-34.604812</v>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-03 22:05:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1946,27 +1946,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>7141</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>CALVO, CARLOS AV. 4007</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1999,18 +1999,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.42486</v>
+        <v>-58.422037</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.577318</v>
+        <v>-34.624729</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2022,27 +2022,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2070,35 +2070,35 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.491074</v>
+        <v>-58.42486</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.575623</v>
+        <v>-34.577318</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2108,17 +2108,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,12 +2141,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2155,14 +2155,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.525125</v>
+        <v>-58.491074</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.604668</v>
+        <v>-34.575623</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,27 +2174,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2231,26 +2231,26 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.421964</v>
+        <v>-58.525125</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.586342</v>
+        <v>-34.604668</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2260,17 +2260,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2307,26 +2307,26 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.498493</v>
+        <v>-58.421964</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.581262</v>
+        <v>-34.586342</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-340</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2336,17 +2336,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>SUPERI /ALT/ 1445</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804838869</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2383,14 +2383,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.460666</v>
+        <v>-58.498493</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.573823</v>
+        <v>-34.581262</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2706,7 +2706,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-355</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 4480</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804839675</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2763,10 +2763,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.504568</v>
+        <v>-58.503195</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.590534</v>
+        <v>-34.581735</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2839,14 +2839,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.503195</v>
+        <v>-58.493164</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.581735</v>
+        <v>-34.55732</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2915,14 +2915,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.493164</v>
+        <v>-58.491934</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.55732</v>
+        <v>-34.569348</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2934,7 +2934,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2991,10 +2991,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.491934</v>
+        <v>-58.501418</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.569348</v>
+        <v>-34.574363</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3010,7 +3010,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3067,14 +3067,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.501418</v>
+        <v>-58.494584</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.574363</v>
+        <v>-34.554981</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,27 +3086,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,11 +3121,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3139,14 +3139,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.494584</v>
+        <v>-58.465608</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.554981</v>
+        <v>-34.538489</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3162,27 +3162,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,18 +3215,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.465608</v>
+        <v>-58.436788</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.538489</v>
+        <v>-34.604014</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3238,7 +3238,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,17 +3248,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3295,26 +3295,26 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.436788</v>
+        <v>-58.439461</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.604014</v>
+        <v>-34.605744</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3324,17 +3324,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3371,10 +3371,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.439461</v>
+        <v>-58.418424</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.605744</v>
+        <v>-34.604463</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,7 +3390,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>7054</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>HUMAHUACA 3918</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>804903788</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3447,10 +3447,10 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.418424</v>
+        <v>-58.419694</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.604463</v>
+        <v>-34.602062</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3466,27 +3466,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>7054</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>HUMAHUACA 3918</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804903788</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3523,46 +3523,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.419694</v>
+        <v>-58.473936</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.602062</v>
+        <v>-34.577346</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-383</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>VALDERRAMA /ALT/ 4187</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805507401</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114 </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3599,46 +3599,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.481834</v>
+        <v>-58.387847</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.560796</v>
+        <v>-34.587043</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3675,10 +3675,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.473936</v>
+        <v>-58.451835</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.577346</v>
+        <v>-34.562646</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,27 +3694,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-386</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1943</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805507419</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3742,23 +3742,23 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.458217</v>
+        <v>-58.470837</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.565043</v>
+        <v>-34.545751</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3770,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3813,12 +3813,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3827,36 +3827,36 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.387847</v>
+        <v>-58.472267</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.587043</v>
+        <v>-34.551163</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3903,14 +3903,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.451835</v>
+        <v>-58.464144</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.562646</v>
+        <v>-34.541832</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3922,27 +3922,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3975,50 +3975,50 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.470837</v>
+        <v>-58.434761</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.545751</v>
+        <v>-34.598381</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4041,24 +4041,24 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.472267</v>
+        <v>-58.464177</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.551163</v>
+        <v>-34.558239</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4074,7 +4074,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4084,17 +4084,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4131,46 +4131,46 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.464144</v>
+        <v>-58.412302</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.541832</v>
+        <v>-34.59301</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,11 +4185,11 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4207,46 +4207,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.434761</v>
+        <v>-58.485056</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.598381</v>
+        <v>-34.555059</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4279,18 +4279,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.464177</v>
+        <v>-58.469783</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.558239</v>
+        <v>-34.599214</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4355,18 +4355,18 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.412302</v>
+        <v>-58.487144</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.59301</v>
+        <v>-34.669078</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4378,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4411,13 +4411,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Columna de retención (columna más ancha</t>
-        </is>
-      </c>
+      <c r="H53" t="inlineStr"/>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4435,46 +4431,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.485056</v>
+        <v>-58.405761</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.555059</v>
+        <v>-34.582476</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4489,7 +4485,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4497,7 +4493,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4511,46 +4507,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.469783</v>
+        <v>-58.432241</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.599214</v>
+        <v>-34.56642</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4565,7 +4561,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4573,7 +4569,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4583,18 +4579,18 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.487144</v>
+        <v>-58.417348</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.669078</v>
+        <v>-34.595467</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4606,27 +4602,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4641,7 +4637,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4659,50 +4655,50 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.49147</v>
+        <v>-58.472311</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.55031</v>
+        <v>-34.654867</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4715,7 +4711,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+        </is>
+      </c>
       <c r="I57" t="n">
         <v>1</v>
       </c>
@@ -4731,50 +4731,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.405761</v>
+        <v>-58.484729</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.582476</v>
+        <v>-34.574614</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>6409</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>CASTAÑARES AV. 5656</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Faltan cargar las fotos del cierre</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4807,18 +4807,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.432241</v>
+        <v>-58.479921</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.56642</v>
+        <v>-34.673021</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4830,27 +4830,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4883,50 +4883,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.417348</v>
+        <v>-58.510247</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.595467</v>
+        <v>-34.645038</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4959,50 +4959,50 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.472311</v>
+        <v>-58.483145</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.654867</v>
+        <v>-34.557043</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6239</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>PALPA 2964</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807763098</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5039,14 +5039,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.450113</v>
+        <v>-58.496608</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.574534</v>
+        <v>-34.666371</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5058,27 +5058,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5111,40 +5111,40 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.484729</v>
+        <v>-58.422229</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.574614</v>
+        <v>-34.573148</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6409</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 5656</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5154,7 +5154,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Faltan cargar las fotos del cierre</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5187,14 +5187,14 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.479921</v>
+        <v>-58.494864</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.673021</v>
+        <v>-34.678826</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5210,27 +5210,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5253,7 +5253,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5263,14 +5263,14 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.510247</v>
+        <v>-58.473089</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.645038</v>
+        <v>-34.625478</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5286,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5343,46 +5343,46 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.483145</v>
+        <v>-58.468841</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.557043</v>
+        <v>-34.686635</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5419,46 +5419,46 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.496608</v>
+        <v>-58.375684</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.666371</v>
+        <v>-34.656092</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5495,14 +5495,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.422229</v>
+        <v>-58.460818</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.573148</v>
+        <v>-34.618934</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5514,27 +5514,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5567,14 +5567,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.494864</v>
+        <v>-58.460441</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.678826</v>
+        <v>-34.628243</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5590,27 +5590,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5620,12 +5620,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5638,55 +5638,51 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr"/>
       <c r="M69" t="n">
-        <v>-58.473089</v>
+        <v>-58.470919</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.625478</v>
+        <v>-34.665309</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5723,14 +5719,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.468841</v>
+        <v>-58.373428</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.686635</v>
+        <v>-34.63705</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5742,27 +5738,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5773,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5785,7 +5781,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5799,46 +5795,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.375684</v>
+        <v>-58.488424</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.656092</v>
+        <v>-34.642002</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-549</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>14 de Julio 65</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808749189</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5849,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5871,50 +5867,50 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.468496</v>
+        <v>-58.37456</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.591282</v>
+        <v>-34.649779</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5929,7 +5925,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5951,14 +5947,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.460818</v>
+        <v>-58.37805</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.618934</v>
+        <v>-34.649722</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5970,27 +5966,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6005,7 +6001,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6013,7 +6009,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6027,14 +6023,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.460441</v>
+        <v>-58.378104</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.628243</v>
+        <v>-34.649578</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6046,27 +6042,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6076,12 +6072,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6094,19 +6090,23 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L75" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M75" t="n">
-        <v>-58.470919</v>
+        <v>-58.377974</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.665309</v>
+        <v>-34.641024</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6118,27 +6118,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6175,14 +6175,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.373428</v>
+        <v>-58.435511</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.63705</v>
+        <v>-34.644702</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6194,27 +6194,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>7106</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>MARTI, JOSE 627</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>809371835</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6229,7 +6229,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6251,46 +6251,46 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.488424</v>
+        <v>-58.469159</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.642002</v>
+        <v>-34.638898</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>4088</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>GOMEZ, VALENTIN 3648</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809406164</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6305,7 +6305,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6323,477 +6323,21 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.37456</v>
+        <v>-58.416416</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.649779</v>
+        <v>-34.604812</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>7089</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>8/27/2025</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>SAN ANTONIO 637</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>809270751</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M79" t="n">
-        <v>-58.37805</v>
-      </c>
-      <c r="N79" t="n">
-        <v>-34.649722</v>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P79" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>7090</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>8/28/2025</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>SAN ANTONIO 625</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>809270753</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I80" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M80" t="n">
-        <v>-58.378104</v>
-      </c>
-      <c r="N80" t="n">
-        <v>-34.649578</v>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P80" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>7091</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>8/28/2025</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>SUAREZ AV. 1966</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>809279022</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M81" t="n">
-        <v>-58.377974</v>
-      </c>
-      <c r="N81" t="n">
-        <v>-34.641024</v>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>7096</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>8/28/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>809279069</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>-58.435511</v>
-      </c>
-      <c r="N82" t="n">
-        <v>-34.644702</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>7106</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>9/1/2025</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>MARTI, JOSE 627</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>809371835</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
-        </is>
-      </c>
-      <c r="I83" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M83" t="n">
-        <v>-58.469159</v>
-      </c>
-      <c r="N83" t="n">
-        <v>-34.638898</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P83" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>4088</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>9/2/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>GOMEZ, VALENTIN 3648</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>809406164</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>-58.416416</v>
-      </c>
-      <c r="N84" t="n">
-        <v>-34.604812</v>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 07:53:20)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6343,6 +6343,78 @@
         </is>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>-581</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>9/4/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Praga 1380</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>809432814</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.481608</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.587837</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 08:03:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3542,27 +3542,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3599,14 +3599,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.387847</v>
+        <v>-58.372751</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.587043</v>
+        <v>-34.631917</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3618,27 +3618,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3675,26 +3675,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.451835</v>
+        <v>-58.387847</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.562646</v>
+        <v>-34.587043</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +3704,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3747,18 +3747,18 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.470837</v>
+        <v>-58.451835</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.545751</v>
+        <v>-34.562646</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3770,7 +3770,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3780,7 +3780,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3818,19 +3818,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.472267</v>
+        <v>-58.470837</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.551163</v>
+        <v>-34.545751</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,27 +3846,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3889,12 +3889,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.464144</v>
+        <v>-58.472267</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.541832</v>
+        <v>-34.551163</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3979,26 +3979,26 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.434761</v>
+        <v>-58.464144</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.598381</v>
+        <v>-34.541832</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,17 +4008,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4051,30 +4051,30 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.464177</v>
+        <v>-58.434761</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.558239</v>
+        <v>-34.598381</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4084,17 +4084,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4127,50 +4127,50 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.412302</v>
+        <v>-58.464177</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.59301</v>
+        <v>-34.558239</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,11 +4185,11 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4207,46 +4207,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.485056</v>
+        <v>-58.412302</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.555059</v>
+        <v>-34.59301</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,15 +4261,15 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4283,14 +4283,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.469783</v>
+        <v>-58.485056</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.599214</v>
+        <v>-34.555059</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4355,50 +4355,50 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.487144</v>
+        <v>-58.469783</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.669078</v>
+        <v>-34.599214</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4411,13 +4411,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
+        </is>
+      </c>
       <c r="I53" t="n">
         <v>1</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4427,18 +4431,18 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.405761</v>
+        <v>-58.487144</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.582476</v>
+        <v>-34.669078</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4450,17 +4454,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4470,7 +4474,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4483,11 +4487,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H54" t="inlineStr"/>
       <c r="I54" t="n">
         <v>1</v>
       </c>
@@ -4507,14 +4507,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.432241</v>
+        <v>-58.405761</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.56642</v>
+        <v>-34.582476</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4526,7 +4526,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4536,7 +4536,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4583,10 +4583,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.417348</v>
+        <v>-58.432241</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.595467</v>
+        <v>-34.56642</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4602,27 +4602,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4655,18 +4655,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.472311</v>
+        <v>-58.417348</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.654867</v>
+        <v>-34.595467</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4678,7 +4678,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4688,17 +4688,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4731,50 +4731,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.484729</v>
+        <v>-58.472311</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.574614</v>
+        <v>-34.654867</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6409</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 5656</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Faltan cargar las fotos del cierre</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4807,50 +4807,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.479921</v>
+        <v>-58.484729</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.673021</v>
+        <v>-34.574614</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6409</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>CASTAÑARES AV. 5656</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Faltan cargar las fotos del cierre</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4883,40 +4883,40 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.510247</v>
+        <v>-58.479921</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.645038</v>
+        <v>-34.673021</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4926,7 +4926,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4963,10 +4963,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.483145</v>
+        <v>-58.470347</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.557043</v>
+        <v>-34.547965</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4982,27 +4982,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6486</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>BILBAO, FRANCISCO 2442</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5039,46 +5039,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.496608</v>
+        <v>-58.460522</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.666371</v>
+        <v>-34.635514</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5111,50 +5111,50 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.422229</v>
+        <v>-58.510247</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.573148</v>
+        <v>-34.645038</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5187,40 +5187,40 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.494864</v>
+        <v>-58.478941</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.678826</v>
+        <v>-34.57242</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5230,7 +5230,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5267,14 +5267,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.473089</v>
+        <v>-58.483145</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.625478</v>
+        <v>-34.557043</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5343,36 +5343,36 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.468841</v>
+        <v>-58.496608</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.686635</v>
+        <v>-34.666371</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5382,7 +5382,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5419,10 +5419,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.375684</v>
+        <v>-58.401083</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.656092</v>
+        <v>-34.629397</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5495,14 +5495,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.460818</v>
+        <v>-58.422229</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.618934</v>
+        <v>-34.573148</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5514,27 +5514,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5567,14 +5567,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.460441</v>
+        <v>-58.494864</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.628243</v>
+        <v>-34.678826</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5590,27 +5590,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5620,12 +5620,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5638,51 +5638,55 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M69" t="n">
-        <v>-58.470919</v>
+        <v>-58.473089</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.665309</v>
+        <v>-34.625478</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5719,14 +5723,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.373428</v>
+        <v>-58.468841</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.63705</v>
+        <v>-34.686635</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5738,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5773,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5781,7 +5785,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5795,46 +5799,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.488424</v>
+        <v>-58.375684</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.642002</v>
+        <v>-34.656092</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5849,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5867,18 +5871,18 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.37456</v>
+        <v>-58.460818</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.649779</v>
+        <v>-34.618934</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5890,27 +5894,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5925,7 +5929,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5933,7 +5937,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5947,14 +5951,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.37805</v>
+        <v>-58.460441</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.649722</v>
+        <v>-34.628243</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5966,27 +5970,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5996,12 +6000,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6014,23 +6018,19 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr"/>
       <c r="M74" t="n">
-        <v>-58.378104</v>
+        <v>-58.470919</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.649578</v>
+        <v>-34.665309</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6042,17 +6042,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6062,7 +6062,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6099,10 +6099,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.377974</v>
+        <v>-58.373428</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.641024</v>
+        <v>-34.63705</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6118,27 +6118,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6175,46 +6175,46 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.435511</v>
+        <v>-58.488424</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.644702</v>
+        <v>-34.642002</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7106</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>MARTI, JOSE 627</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809371835</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6229,7 +6229,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6247,18 +6247,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.469159</v>
+        <v>-58.37456</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.638898</v>
+        <v>-34.649779</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6270,27 +6270,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>4088</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>GOMEZ, VALENTIN 3648</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809406164</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6305,7 +6305,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6327,14 +6327,14 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.416416</v>
+        <v>-58.37805</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.604812</v>
+        <v>-34.649722</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6346,70 +6346,450 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>7090</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>SAN ANTONIO 625</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>809270753</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.378104</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.649578</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>7091</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>SUAREZ AV. 1966</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>809279022</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.377974</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.641024</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>7096</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>VEDIA, AGUSTIN DE 2185</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>809279069</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.435511</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.644702</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>7106</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>9/1/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>MARTI, JOSE 627</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809371835</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.469159</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.638898</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>4088</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>9/2/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>GOMEZ, VALENTIN 3648</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>809406164</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>-58.416416</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.604812</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
           <t>-581</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B84" t="inlineStr">
         <is>
           <t>9/4/2025</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C84" t="inlineStr">
         <is>
           <t>Praga 1380</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr">
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
         <is>
           <t>809432814</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
         <is>
           <t>Cambiar</t>
         </is>
       </c>
-      <c r="I79" t="n">
+      <c r="I84" t="n">
         <v>0</v>
       </c>
-      <c r="J79" t="inlineStr">
+      <c r="J84" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M79" t="n">
+      <c r="M84" t="n">
         <v>-58.481608</v>
       </c>
-      <c r="N79" t="n">
+      <c r="N84" t="n">
         <v>-34.587837</v>
       </c>
-      <c r="O79" t="inlineStr">
+      <c r="O84" t="inlineStr">
         <is>
           <t>Paternal</t>
         </is>
       </c>
-      <c r="P79" t="inlineStr">
+      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 21:00:38)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -3390,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>7054</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>HUMAHUACA 3918</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804903788</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3447,46 +3447,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.419694</v>
+        <v>-58.473936</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.602062</v>
+        <v>-34.577346</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3523,46 +3523,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.473936</v>
+        <v>-58.372751</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.577346</v>
+        <v>-34.631917</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3599,14 +3599,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.372751</v>
+        <v>-58.387847</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.631917</v>
+        <v>-34.587043</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3618,27 +3618,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3675,26 +3675,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.387847</v>
+        <v>-58.451835</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.587043</v>
+        <v>-34.562646</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +3704,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3747,18 +3747,18 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.451835</v>
+        <v>-58.470837</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.562646</v>
+        <v>-34.545751</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3770,7 +3770,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3780,7 +3780,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3818,19 +3818,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,27 +3846,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3889,12 +3889,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3979,26 +3979,26 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,17 +4008,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4051,30 +4051,30 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4084,17 +4084,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4127,50 +4127,50 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,11 +4185,11 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4207,46 +4207,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.412302</v>
+        <v>-58.485056</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.59301</v>
+        <v>-34.555059</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/22/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Cucha Cucha 2918</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807044223</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4261,15 +4261,15 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4283,14 +4283,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.485056</v>
+        <v>-58.469783</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.555059</v>
+        <v>-34.599214</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4302,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t>807044233</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/22/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Cucha Cucha 2918</t>
+          <t>Martin Grandoli 5761</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807044223</t>
+          <t xml:space="preserve">ICD30261461 </t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4355,50 +4355,50 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.469783</v>
+        <v>-58.487144</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.599214</v>
+        <v>-34.669078</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>807044233</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Martin Grandoli 5761</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30261461 </t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4411,17 +4411,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Desmontar columna de 7 en desuso no colocar nueva queda OT 807044233 solo para el cambio ya realizado el ICD es para el desmonte</t>
-        </is>
-      </c>
+      <c r="H53" t="inlineStr"/>
       <c r="I53" t="n">
         <v>1</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4431,18 +4427,18 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.487144</v>
+        <v>-58.405761</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.669078</v>
+        <v>-34.582476</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4454,17 +4450,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4474,7 +4470,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4487,7 +4483,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr"/>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I54" t="n">
         <v>1</v>
       </c>
@@ -4507,14 +4507,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4526,7 +4526,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4536,7 +4536,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4583,10 +4583,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4602,27 +4602,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4655,18 +4655,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4678,7 +4678,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4688,17 +4688,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4731,40 +4731,40 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.472311</v>
+        <v>-58.484729</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.654867</v>
+        <v>-34.574614</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4774,7 +4774,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4807,18 +4807,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.484729</v>
+        <v>-58.470347</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.574614</v>
+        <v>-34.547965</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4830,27 +4830,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6409</t>
+          <t>6486</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 5656</t>
+          <t>BILBAO, FRANCISCO 2442</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807965768</t>
+          <t>808243829</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Faltan cargar las fotos del cierre</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4883,14 +4883,14 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.479921</v>
+        <v>-58.460522</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.673021</v>
+        <v>-34.635514</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4906,7 +4906,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4916,17 +4916,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4959,18 +4959,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.470347</v>
+        <v>-58.510247</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.547965</v>
+        <v>-34.645038</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4982,27 +4982,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6486</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2442</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808243829</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5039,46 +5039,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.460522</v>
+        <v>-58.478941</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.635514</v>
+        <v>-34.57242</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6585</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>Crisologo Larralde 4073</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373627</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Cambiar columna corroída en base</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5111,18 +5111,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.510247</v>
+        <v>-58.483145</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.645038</v>
+        <v>-34.557043</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5134,27 +5134,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5191,14 +5191,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.478941</v>
+        <v>-58.496608</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.57242</v>
+        <v>-34.666371</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5210,27 +5210,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5267,46 +5267,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.483145</v>
+        <v>-58.401083</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.557043</v>
+        <v>-34.629397</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5343,46 +5343,46 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.496608</v>
+        <v>-58.422229</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.666371</v>
+        <v>-34.573148</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5415,18 +5415,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.401083</v>
+        <v>-58.494864</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.629397</v>
+        <v>-34.678826</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5495,36 +5495,36 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.422229</v>
+        <v>-58.473089</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.573148</v>
+        <v>-34.625478</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5567,14 +5567,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.494864</v>
+        <v>-58.468841</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.678826</v>
+        <v>-34.686635</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5590,27 +5590,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5647,46 +5647,46 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.473089</v>
+        <v>-58.375684</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.625478</v>
+        <v>-34.656092</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5723,10 +5723,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.468841</v>
+        <v>-58.460818</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.686635</v>
+        <v>-34.618934</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5742,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5799,14 +5799,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.375684</v>
+        <v>-58.460441</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.656092</v>
+        <v>-34.628243</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5818,27 +5818,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5848,12 +5848,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5866,19 +5866,15 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr"/>
       <c r="M72" t="n">
-        <v>-58.460818</v>
+        <v>-58.470919</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.618934</v>
+        <v>-34.665309</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5894,27 +5890,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7060</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>PINZON 1578</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>809195671</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5929,7 +5925,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5937,7 +5933,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5951,14 +5947,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.460441</v>
+        <v>-58.373428</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.628243</v>
+        <v>-34.63705</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5970,27 +5966,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>-568</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>Ameghino 523</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6000,12 +5996,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>Picada con pelgro de caida</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6018,41 +6014,45 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M74" t="n">
-        <v>-58.470919</v>
+        <v>-58.488424</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.665309</v>
+        <v>-34.642002</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6062,7 +6062,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6095,14 +6095,14 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.373428</v>
+        <v>-58.37456</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.63705</v>
+        <v>-34.649779</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6118,27 +6118,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada con pelgro de caida</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6175,26 +6175,26 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.488424</v>
+        <v>-58.37805</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.642002</v>
+        <v>-34.649722</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6204,7 +6204,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6214,7 +6214,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6247,14 +6247,14 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.37456</v>
+        <v>-58.378104</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.649779</v>
+        <v>-34.649578</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6270,17 +6270,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6290,7 +6290,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6327,10 +6327,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.37805</v>
+        <v>-58.377974</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.649722</v>
+        <v>-34.641024</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6346,7 +6346,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6356,17 +6356,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6403,14 +6403,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.378104</v>
+        <v>-58.435511</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.649578</v>
+        <v>-34.644702</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6422,27 +6422,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7106</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>MARTI, JOSE 627</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809371835</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6457,7 +6457,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6479,14 +6479,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.377974</v>
+        <v>-58.469159</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.641024</v>
+        <v>-34.638898</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6498,27 +6498,23 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>-581</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/4/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
+          <t>Praga 1380</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809432814</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6537,7 +6533,7 @@
         </is>
       </c>
       <c r="I81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -6555,241 +6551,17 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.435511</v>
+        <v>-58.481608</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.644702</v>
+        <v>-34.587837</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>7106</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>9/1/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>MARTI, JOSE 627</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>809371835</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>-58.469159</v>
-      </c>
-      <c r="N82" t="n">
-        <v>-34.638898</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>4088</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>9/2/2025</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>GOMEZ, VALENTIN 3648</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>809406164</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I83" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M83" t="n">
-        <v>-58.416416</v>
-      </c>
-      <c r="N83" t="n">
-        <v>-34.604812</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P83" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>-581</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>9/4/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Praga 1380</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>809432814</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>0</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>-58.481608</v>
-      </c>
-      <c r="N84" t="n">
-        <v>-34.587837</v>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-08 07:30:13)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1946,27 +1946,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>7141</t>
+          <t>6066</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS AV. 4007</t>
+          <t>ALBARIÑO 1331</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>803651213</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Podrida en la base</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2003,46 +2003,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.422037</v>
+        <v>-58.496255</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.624729</v>
+        <v>-34.650599</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>7141</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>CALVO, CARLOS AV. 4007</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2075,18 +2075,18 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.42486</v>
+        <v>-58.422037</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.577318</v>
+        <v>-34.624729</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2098,27 +2098,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2146,35 +2146,35 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.491074</v>
+        <v>-58.42486</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.575623</v>
+        <v>-34.577318</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2184,17 +2184,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2217,12 +2217,12 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2231,14 +2231,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.525125</v>
+        <v>-58.491074</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.604668</v>
+        <v>-34.575623</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2250,27 +2250,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2307,26 +2307,26 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.421964</v>
+        <v>-58.525125</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.586342</v>
+        <v>-34.604668</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2336,17 +2336,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2383,36 +2383,36 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.498493</v>
+        <v>-58.421964</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.581262</v>
+        <v>-34.586342</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,15 +2437,15 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2459,10 +2459,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.502447</v>
+        <v>-58.498493</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.561008</v>
+        <v>-34.581262</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,17 +2488,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2535,10 +2535,10 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.483947</v>
+        <v>-58.502447</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.583207</v>
+        <v>-34.561008</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2554,7 +2554,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2564,17 +2564,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2607,14 +2607,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.503673</v>
+        <v>-58.483947</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.586925</v>
+        <v>-34.583207</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2630,7 +2630,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2683,14 +2683,14 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.504455</v>
+        <v>-58.503673</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579941</v>
+        <v>-34.586925</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2706,7 +2706,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2763,10 +2763,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.503195</v>
+        <v>-58.504455</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.581735</v>
+        <v>-34.579941</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2782,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2839,14 +2839,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.493164</v>
+        <v>-58.503195</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.55732</v>
+        <v>-34.581735</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2915,14 +2915,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.491934</v>
+        <v>-58.493164</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.569348</v>
+        <v>-34.55732</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2934,7 +2934,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2991,10 +2991,10 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.501418</v>
+        <v>-58.491934</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.574363</v>
+        <v>-34.569348</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3010,7 +3010,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3020,7 +3020,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -3030,7 +3030,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3067,14 +3067,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.494584</v>
+        <v>-58.501418</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.554981</v>
+        <v>-34.574363</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3086,27 +3086,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,11 +3121,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3139,14 +3139,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.465608</v>
+        <v>-58.494584</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.538489</v>
+        <v>-34.554981</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3162,27 +3162,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,18 +3215,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.436788</v>
+        <v>-58.465608</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.604014</v>
+        <v>-34.538489</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3238,7 +3238,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,17 +3248,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3295,26 +3295,26 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.439461</v>
+        <v>-58.436788</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.605744</v>
+        <v>-34.604014</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3324,17 +3324,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3371,10 +3371,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.418424</v>
+        <v>-58.439461</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.604463</v>
+        <v>-34.605744</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3390,27 +3390,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3447,46 +3447,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.473936</v>
+        <v>-58.418424</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.577346</v>
+        <v>-34.604463</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3523,46 +3523,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.372751</v>
+        <v>-58.473936</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.631917</v>
+        <v>-34.577346</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3599,14 +3599,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.387847</v>
+        <v>-58.372751</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.587043</v>
+        <v>-34.631917</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3618,27 +3618,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3675,26 +3675,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.451835</v>
+        <v>-58.387847</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.562646</v>
+        <v>-34.587043</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +3704,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3747,18 +3747,18 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.470837</v>
+        <v>-58.451835</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.545751</v>
+        <v>-34.562646</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3770,7 +3770,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3780,7 +3780,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3818,19 +3818,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.472267</v>
+        <v>-58.470837</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.551163</v>
+        <v>-34.545751</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,27 +3846,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3889,12 +3889,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3903,10 +3903,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.464144</v>
+        <v>-58.472267</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.541832</v>
+        <v>-34.551163</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3922,7 +3922,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3979,26 +3979,26 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.434761</v>
+        <v>-58.464144</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.598381</v>
+        <v>-34.541832</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,17 +4008,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4051,30 +4051,30 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.464177</v>
+        <v>-58.434761</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.558239</v>
+        <v>-34.598381</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4084,17 +4084,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4109,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4127,50 +4127,50 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.412302</v>
+        <v>-58.464177</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.59301</v>
+        <v>-34.558239</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4185,11 +4185,11 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -4207,19 +4207,19 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.485056</v>
+        <v>-58.412302</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.555059</v>
+        <v>-34.59301</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -5058,27 +5058,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6585</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Crisologo Larralde 4073</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808373627</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Cambiar columna corroída en base</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5115,14 +5115,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.483145</v>
+        <v>-58.496608</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.557043</v>
+        <v>-34.666371</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5134,27 +5134,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5191,46 +5191,46 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.496608</v>
+        <v>-58.401083</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.666371</v>
+        <v>-34.629397</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5253,7 +5253,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5267,14 +5267,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.401083</v>
+        <v>-58.422229</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.629397</v>
+        <v>-34.573148</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5339,18 +5339,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.422229</v>
+        <v>-58.494864</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.573148</v>
+        <v>-34.678826</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5362,27 +5362,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5415,50 +5415,50 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.494864</v>
+        <v>-58.473089</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.678826</v>
+        <v>-34.625478</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5495,26 +5495,26 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.473089</v>
+        <v>-58.468841</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.625478</v>
+        <v>-34.686635</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5524,17 +5524,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5571,14 +5571,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.468841</v>
+        <v>-58.375684</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.686635</v>
+        <v>-34.656092</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5590,27 +5590,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5647,14 +5647,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.375684</v>
+        <v>-58.460818</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.656092</v>
+        <v>-34.618934</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5666,17 +5666,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5686,7 +5686,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5723,10 +5723,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.460818</v>
+        <v>-58.460441</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.618934</v>
+        <v>-34.628243</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5742,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7072</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>CASTAÑARES AV. 4611</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>ICD30519785</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t xml:space="preserve">Ya se traspaso nodo retirar columna ICD30462144 fue la cocacion </t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5785,24 +5785,20 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr"/>
       <c r="M71" t="n">
-        <v>-58.460441</v>
+        <v>-58.470919</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.628243</v>
+        <v>-34.665309</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -5818,27 +5814,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7072</t>
+          <t>7149</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>CASTAÑARES AV. 4611</t>
+          <t>QUITO 3666</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>ICD30519785</t>
+          <t>809168441</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5848,12 +5844,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>ICD30462144 fue la colocacion se genera otro para desmonte qap traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5866,19 +5862,23 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L72" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M72" t="n">
-        <v>-58.470919</v>
+        <v>-58.41791</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.665309</v>
+        <v>-34.616706</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5966,7 +5966,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-568</t>
+          <t>7162</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5976,7 +5976,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Ameghino 523</t>
+          <t>AMEGHINO, FLORENTINO, DR. 525</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -6042,27 +6042,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7157</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>CALVO, CARLOS 1750</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809257762</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6095,14 +6095,14 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.37456</v>
+        <v>-58.390806</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.649779</v>
+        <v>-34.620213</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6118,17 +6118,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6171,14 +6171,14 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.37805</v>
+        <v>-58.37456</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.649722</v>
+        <v>-34.649779</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6194,17 +6194,17 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6214,7 +6214,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6251,10 +6251,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.378104</v>
+        <v>-58.37805</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.649578</v>
+        <v>-34.649722</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6270,7 +6270,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6280,7 +6280,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6290,7 +6290,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6327,10 +6327,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.377974</v>
+        <v>-58.378104</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.641024</v>
+        <v>-34.649578</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6346,7 +6346,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6356,17 +6356,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6403,14 +6403,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.435511</v>
+        <v>-58.377974</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.644702</v>
+        <v>-34.641024</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6422,17 +6422,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7106</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>MARTI, JOSE 627</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6442,7 +6442,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809371835</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6457,7 +6457,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Poste quebrado cambiar por prfv es un poste viejo ExCV</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6479,10 +6479,10 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.469159</v>
+        <v>-58.435511</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.638898</v>
+        <v>-34.644702</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -6562,6 +6562,158 @@
         </is>
       </c>
       <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>7166</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>9/5/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>BRIN, MINISTRO 1259</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809492876</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.355919</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.634597</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>7169</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>9/5/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>SAN NICOLAS 5045</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>809492980</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Poste quebrado</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>-58.515637</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.589993</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-08 10:59:13)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6719,6 +6719,158 @@
         </is>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>-583</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Av Eva Perón 1145</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809504290</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.441547</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.630481</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>-584</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>General Gregorio Aráoz de Lamadrid 865</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>809504300</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Columna colgando</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.364566</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.639404</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-09 14:46:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1870,27 +1870,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6066</t>
+          <t>7141</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ALBARIÑO 1331</t>
+          <t>CALVO, CARLOS AV. 4007</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>803651213</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Podrida en la base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1927,46 +1927,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.496255</v>
+        <v>-58.422037</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.650599</v>
+        <v>-34.624729</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>7141</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS AV. 4007</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1999,18 +1999,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.422037</v>
+        <v>-58.42486</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.624729</v>
+        <v>-34.577318</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2022,27 +2022,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2070,35 +2070,35 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.42486</v>
+        <v>-58.491074</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.577318</v>
+        <v>-34.575623</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2108,17 +2108,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,12 +2141,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2155,14 +2155,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.491074</v>
+        <v>-58.525125</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.575623</v>
+        <v>-34.604668</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,27 +2174,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2231,26 +2231,26 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.525125</v>
+        <v>-58.421964</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.604668</v>
+        <v>-34.586342</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2260,17 +2260,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2307,36 +2307,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.421964</v>
+        <v>-58.498493</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.586342</v>
+        <v>-34.581262</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,15 +2361,15 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2383,10 +2383,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.498493</v>
+        <v>-58.502447</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.581262</v>
+        <v>-34.561008</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2402,7 +2402,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2412,17 +2412,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2459,10 +2459,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.502447</v>
+        <v>-58.483947</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.561008</v>
+        <v>-34.583207</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,17 +2488,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2531,14 +2531,14 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.483947</v>
+        <v>-58.503673</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.583207</v>
+        <v>-34.586925</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2554,7 +2554,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2607,14 +2607,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.503673</v>
+        <v>-58.504455</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.586925</v>
+        <v>-34.579941</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2630,7 +2630,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2687,10 +2687,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.504455</v>
+        <v>-58.503195</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579941</v>
+        <v>-34.581735</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2706,7 +2706,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2763,14 +2763,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.503195</v>
+        <v>-58.493164</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.581735</v>
+        <v>-34.55732</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2782,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2839,14 +2839,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.493164</v>
+        <v>-58.491934</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.55732</v>
+        <v>-34.569348</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2915,10 +2915,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.491934</v>
+        <v>-58.501418</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.569348</v>
+        <v>-34.574363</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2934,7 +2934,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2991,14 +2991,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.501418</v>
+        <v>-58.494584</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.574363</v>
+        <v>-34.554981</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,11 +3045,11 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3063,14 +3063,14 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.494584</v>
+        <v>-58.465608</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.554981</v>
+        <v>-34.538489</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3086,27 +3086,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,18 +3139,18 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.465608</v>
+        <v>-58.436788</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.538489</v>
+        <v>-34.604014</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3162,7 +3162,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3172,17 +3172,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3219,26 +3219,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.436788</v>
+        <v>-58.439461</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.604014</v>
+        <v>-34.605744</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3248,17 +3248,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3295,10 +3295,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.439461</v>
+        <v>-58.418424</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.605744</v>
+        <v>-34.604463</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3314,27 +3314,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3371,46 +3371,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.418424</v>
+        <v>-58.473936</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.604463</v>
+        <v>-34.577346</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3433,7 +3433,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3447,46 +3447,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.473936</v>
+        <v>-58.372751</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.577346</v>
+        <v>-34.631917</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3523,14 +3523,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.372751</v>
+        <v>-58.387847</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.631917</v>
+        <v>-34.587043</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3542,27 +3542,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3572,12 +3572,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3590,7 +3590,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3599,26 +3599,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.387847</v>
+        <v>-58.451835</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.587043</v>
+        <v>-34.562646</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,17 +3628,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3648,12 +3648,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3661,28 +3661,28 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.451835</v>
+        <v>-58.470837</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.562646</v>
+        <v>-34.545751</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3694,7 +3694,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3742,19 +3742,19 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,27 +3770,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3813,12 +3813,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3827,10 +3827,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3846,7 +3846,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,17 +3856,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3903,26 +3903,26 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3975,30 +3975,30 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4008,17 +4008,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4051,50 +4051,50 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4107,11 +4107,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
-        </is>
-      </c>
+      <c r="H49" t="inlineStr"/>
       <c r="I49" t="n">
         <v>1</v>
       </c>
@@ -4131,14 +4127,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.412302</v>
+        <v>-58.405761</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.59301</v>
+        <v>-34.582476</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4150,17 +4146,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4170,7 +4166,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4183,7 +4179,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I50" t="n">
         <v>1</v>
       </c>
@@ -4203,14 +4203,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4232,7 +4232,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4242,7 +4242,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4279,10 +4279,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4298,27 +4298,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4333,7 +4333,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4351,18 +4351,18 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4374,7 +4374,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4384,17 +4384,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4409,7 +4409,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4427,50 +4427,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.472311</v>
+        <v>-58.484729</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.654867</v>
+        <v>-34.574614</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>7200</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4485,7 +4485,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4503,23 +4503,23 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.484729</v>
+        <v>-58.403422</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.574614</v>
+        <v>-34.609195</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -5590,27 +5590,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7157</t>
+          <t>7162</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1750</t>
+          <t>AMEGHINO, FLORENTINO, DR. 525</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809257762</t>
+          <t>809208239</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5623,11 +5623,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H69" t="inlineStr"/>
       <c r="I69" t="n">
         <v>1</v>
       </c>
@@ -5647,46 +5643,46 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.390806</v>
+        <v>-58.488424</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.620213</v>
+        <v>-34.642002</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7157</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>CALVO, CARLOS 1750</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809257762</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5701,7 +5697,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5719,14 +5715,14 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.37456</v>
+        <v>-58.390806</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.649779</v>
+        <v>-34.620213</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5742,7 +5738,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7171</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5752,17 +5748,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 5531</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809268253</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5773,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5795,50 +5791,50 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.491028</v>
+        <v>-58.37456</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.579381</v>
+        <v>-34.649779</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7171</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>OLAZABAL AV. 5531</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809268253</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5849,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5875,36 +5871,36 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.37805</v>
+        <v>-58.491028</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.649722</v>
+        <v>-34.579381</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -5914,7 +5910,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5951,10 +5947,10 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.378104</v>
+        <v>-58.37805</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.649578</v>
+        <v>-34.649722</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -5970,7 +5966,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5980,7 +5976,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -5990,7 +5986,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6027,10 +6023,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.377974</v>
+        <v>-58.378104</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.641024</v>
+        <v>-34.649578</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6046,7 +6042,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6056,17 +6052,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6103,14 +6099,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.435511</v>
+        <v>-58.377974</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.644702</v>
+        <v>-34.641024</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6122,23 +6118,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-581</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>9/4/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Praga 1380</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr"/>
+          <t>VEDIA, AGUSTIN DE 2185</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809432814</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6157,7 +6157,7 @@
         </is>
       </c>
       <c r="I76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
@@ -6175,46 +6175,42 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.481608</v>
+        <v>-58.435511</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.587837</v>
+        <v>-34.644702</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7166</t>
+          <t>-581</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/4/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1259</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t>Praga 1380</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809492876</t>
+          <t>809432814</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6229,11 +6225,11 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -6251,19 +6247,19 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.355919</v>
+        <v>-58.481608</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.634597</v>
+        <v>-34.587837</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -6422,7 +6418,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-584</t>
+          <t>7174</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6432,17 +6428,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>General Gregorio Aráoz de Lamadrid 865</t>
+          <t>FERNANDEZ BLANCO 2320</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809504300</t>
+          <t>809526154</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6457,7 +6453,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Columna colgando</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6479,26 +6475,26 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.364566</v>
+        <v>-58.481983</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.639404</v>
+        <v>-34.573931</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7174</t>
+          <t>7177</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6508,7 +6504,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>FERNANDEZ BLANCO 2320</t>
+          <t>LUGONES 2830</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -6518,7 +6514,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809526154</t>
+          <t>809526156</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6555,10 +6551,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.481983</v>
+        <v>-58.482786</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.573931</v>
+        <v>-34.56748</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6574,7 +6570,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7177</t>
+          <t>7184</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6584,7 +6580,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>LUGONES 2830</t>
+          <t>VALLEJOS 2221</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6594,7 +6590,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809526156</t>
+          <t>809526160</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6631,93 +6627,17 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.482786</v>
+        <v>-58.493225</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.56748</v>
+        <v>-34.583095</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>7184</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>VALLEJOS 2221</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>809526160</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I83" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M83" t="n">
-        <v>-58.493225</v>
-      </c>
-      <c r="N83" t="n">
-        <v>-34.583095</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P83" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-10 08:36:35)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3238,27 +3238,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3295,46 +3295,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.418424</v>
+        <v>-58.473936</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.604463</v>
+        <v>-34.577346</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3371,46 +3371,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.473936</v>
+        <v>-58.372751</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.577346</v>
+        <v>-34.631917</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3447,14 +3447,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.372751</v>
+        <v>-58.387847</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.631917</v>
+        <v>-34.587043</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3466,27 +3466,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3496,12 +3496,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3514,7 +3514,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3523,26 +3523,26 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.387847</v>
+        <v>-58.451835</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.587043</v>
+        <v>-34.562646</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3552,17 +3552,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3572,12 +3572,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3585,28 +3585,28 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.451835</v>
+        <v>-58.470837</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.562646</v>
+        <v>-34.545751</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3618,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,7 +3628,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3666,19 +3666,19 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.470837</v>
+        <v>-58.472267</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.545751</v>
+        <v>-34.551163</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,27 +3694,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3737,12 +3737,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3751,10 +3751,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.472267</v>
+        <v>-58.464144</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.551163</v>
+        <v>-34.541832</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,7 +3770,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3780,17 +3780,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3827,26 +3827,26 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.464144</v>
+        <v>-58.434761</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.541832</v>
+        <v>-34.598381</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,17 +3856,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3899,30 +3899,30 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.434761</v>
+        <v>-58.464177</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.598381</v>
+        <v>-34.558239</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3975,50 +3975,50 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.464177</v>
+        <v>-58.412302</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.558239</v>
+        <v>-34.59301</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4031,11 +4031,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
-        </is>
-      </c>
+      <c r="H48" t="inlineStr"/>
       <c r="I48" t="n">
         <v>1</v>
       </c>
@@ -4055,14 +4051,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.412302</v>
+        <v>-58.405761</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.59301</v>
+        <v>-34.582476</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4074,17 +4070,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4094,7 +4090,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4107,7 +4103,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I49" t="n">
         <v>1</v>
       </c>
@@ -4127,14 +4127,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4166,7 +4166,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4203,10 +4203,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4222,27 +4222,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4275,18 +4275,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4308,17 +4308,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4333,7 +4333,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4351,50 +4351,50 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.472311</v>
+        <v>-58.484729</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.654867</v>
+        <v>-34.574614</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>7200</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4409,7 +4409,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4427,50 +4427,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.484729</v>
+        <v>-58.403422</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.574614</v>
+        <v>-34.609195</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>7200</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4507,26 +4507,26 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.403422</v>
+        <v>-58.470347</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.609195</v>
+        <v>-34.547965</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4536,17 +4536,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4579,18 +4579,18 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.470347</v>
+        <v>-58.510247</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.547965</v>
+        <v>-34.645038</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4602,27 +4602,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4655,18 +4655,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.510247</v>
+        <v>-58.478941</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.645038</v>
+        <v>-34.57242</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4678,27 +4678,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>-521</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>Laferrere 6572</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808430950</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4735,14 +4735,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.478941</v>
+        <v>-58.496608</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.57242</v>
+        <v>-34.666371</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4754,27 +4754,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6478</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/24/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>JUJUY AV. 1647</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808509387</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4811,46 +4811,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.496608</v>
+        <v>-58.401083</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.666371</v>
+        <v>-34.629397</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6478</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/24/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>JUJUY AV. 1647</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808509387</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4887,14 +4887,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.401083</v>
+        <v>-58.422229</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.629397</v>
+        <v>-34.573148</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4906,27 +4906,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4959,18 +4959,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.422229</v>
+        <v>-58.494864</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.573148</v>
+        <v>-34.678826</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4982,27 +4982,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6274</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/5/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>ARANGUREN, JUAN F., Dr. 2964</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808720858</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>chocada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5035,50 +5035,50 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.494864</v>
+        <v>-58.473089</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.678826</v>
+        <v>-34.625478</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5115,26 +5115,26 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.473089</v>
+        <v>-58.468841</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.625478</v>
+        <v>-34.686635</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5144,17 +5144,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5191,14 +5191,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.468841</v>
+        <v>-58.375684</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.686635</v>
+        <v>-34.656092</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5210,27 +5210,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6960</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>VALLESE, FELIPE 1940</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808972988</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5253,7 +5253,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5267,14 +5267,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.375684</v>
+        <v>-58.460818</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.656092</v>
+        <v>-34.618934</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,17 +5286,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5343,10 +5343,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.460818</v>
+        <v>-58.460441</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.618934</v>
+        <v>-34.628243</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5362,27 +5362,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7149</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>QUITO 3666</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>809168441</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5419,14 +5419,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.460441</v>
+        <v>-58.41791</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.628243</v>
+        <v>-34.616706</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7149</t>
+          <t>7157</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>QUITO 3666</t>
+          <t>CALVO, CARLOS 1750</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809168441</t>
+          <t>809257762</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5495,14 +5495,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.41791</v>
+        <v>-58.390806</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.616706</v>
+        <v>-34.620213</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5514,17 +5514,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7060</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>PINZON 1578</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809195671</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5567,14 +5567,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.373428</v>
+        <v>-58.37456</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.63705</v>
+        <v>-34.649779</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5590,27 +5590,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7162</t>
+          <t>7171</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>AMEGHINO, FLORENTINO, DR. 525</t>
+          <t>OLAZABAL AV. 5531</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809208239</t>
+          <t>809268253</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5623,7 +5623,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I69" t="n">
         <v>1</v>
       </c>
@@ -5643,14 +5647,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.488424</v>
+        <v>-58.491028</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.642002</v>
+        <v>-34.579381</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5662,7 +5666,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7157</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5672,17 +5676,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1750</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809257762</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5697,7 +5701,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5719,10 +5723,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.390806</v>
+        <v>-58.37805</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.620213</v>
+        <v>-34.649722</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5738,7 +5742,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5748,7 +5752,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5758,7 +5762,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5791,14 +5795,14 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.37456</v>
+        <v>-58.378104</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.649779</v>
+        <v>-34.649578</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -5814,7 +5818,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7171</t>
+          <t>7091</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5824,17 +5828,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 5531</t>
+          <t>SUAREZ AV. 1966</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809268253</t>
+          <t>809279022</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5849,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5871,46 +5875,46 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.491028</v>
+        <v>-58.377974</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.579381</v>
+        <v>-34.641024</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5947,14 +5951,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.37805</v>
+        <v>-58.435511</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.649722</v>
+        <v>-34.644702</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5966,27 +5970,23 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>-581</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/4/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t>Praga 1380</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809432814</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6005,7 +6005,7 @@
         </is>
       </c>
       <c r="I74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -6023,46 +6023,46 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.378104</v>
+        <v>-58.481608</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.649578</v>
+        <v>-34.587837</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7169</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/5/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>SAN NICOLAS 5045</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809492980</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste quebrado</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6095,40 +6095,40 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.377974</v>
+        <v>-58.515637</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.641024</v>
+        <v>-34.589993</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>-583</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>Av Eva Perón 1145</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6138,7 +6138,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809504290</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6175,10 +6175,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.435511</v>
+        <v>-58.441547</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.644702</v>
+        <v>-34.630481</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6194,23 +6194,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-581</t>
+          <t>7174</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/4/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Praga 1380</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr"/>
+          <t>FERNANDEZ BLANCO 2320</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809432814</t>
+          <t>809526154</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6225,11 +6229,11 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
@@ -6247,14 +6251,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.481608</v>
+        <v>-58.481983</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.587837</v>
+        <v>-34.573931</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6266,27 +6270,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>7177</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>LUGONES 2830</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809526156</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6301,7 +6305,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6319,18 +6323,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.515637</v>
+        <v>-58.482786</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.589993</v>
+        <v>-34.56748</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6342,7 +6346,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-583</t>
+          <t>7184</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6352,17 +6356,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Av Eva Perón 1145</t>
+          <t>VALLEJOS 2221</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809504290</t>
+          <t>809526160</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6399,36 +6403,36 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.441547</v>
+        <v>-58.493225</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.630481</v>
+        <v>-34.583095</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7174</t>
+          <t>-589</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>9/8/2025</t>
+          <t>9/9/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>FERNANDEZ BLANCO 2320</t>
+          <t>Balbin 4059</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6438,7 +6442,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809526154</t>
+          <t>809575056</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6453,7 +6457,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corrimiento ver con Pablo</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6471,18 +6475,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.481983</v>
+        <v>-58.48797</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.573931</v>
+        <v>-34.554733</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6494,17 +6498,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7177</t>
+          <t>-590</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>9/8/2025</t>
+          <t>9/9/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>LUGONES 2830</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -6514,7 +6518,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809526156</t>
+          <t>809575080</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6529,7 +6533,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corrimiento ver con Pablo</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6551,93 +6555,17 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.482786</v>
+        <v>-58.487821</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.56748</v>
+        <v>-34.554603</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>7184</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>VALLEJOS 2221</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>809526160</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>-58.493225</v>
-      </c>
-      <c r="N82" t="n">
-        <v>-34.583095</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-11 07:49:33)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1718,27 +1718,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>4768</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>COCHABAMBA /ALT/ 1790</t>
+          <t>VALLESE, FELIPE 684</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>802988221</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1748,16 +1748,16 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>SIN RIEGO</t>
+          <t>Picada info para cierre tambien entro como caso 6909</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1775,14 +1775,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.391153</v>
+        <v>-58.443039</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.624022</v>
+        <v>-34.612262</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1794,27 +1794,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-281</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>2/24/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SOLER /ALT/ 4517</t>
+          <t>COCHABAMBA /ALT/ 1790</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>803651203</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1824,12 +1824,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>columna de 114 con nodo y redes nuestra.</t>
+          <t>SIN RIEGO</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1851,14 +1851,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.423405</v>
+        <v>-58.391153</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.588075</v>
+        <v>-34.624022</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1870,27 +1870,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>7141</t>
+          <t>-281</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS AV. 4007</t>
+          <t>SOLER /ALT/ 4517</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804161220</t>
+          <t>803651203</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1905,11 +1905,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>columna de 114 con nodo y redes nuestra.</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1927,14 +1927,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.422037</v>
+        <v>-58.423405</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.624729</v>
+        <v>-34.588075</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1946,27 +1946,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>7141</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>CALVO, CARLOS AV. 4007</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804161220</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1999,18 +1999,18 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.42486</v>
+        <v>-58.422037</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.577318</v>
+        <v>-34.624729</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2022,27 +2022,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2070,35 +2070,35 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.491074</v>
+        <v>-58.42486</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.575623</v>
+        <v>-34.577318</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2108,17 +2108,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2141,12 +2141,12 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2155,14 +2155,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.525125</v>
+        <v>-58.491074</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.604668</v>
+        <v>-34.575623</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,27 +2174,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2231,26 +2231,26 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.421964</v>
+        <v>-58.525125</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.586342</v>
+        <v>-34.604668</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2260,17 +2260,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2307,36 +2307,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.498493</v>
+        <v>-58.421964</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.581262</v>
+        <v>-34.586342</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2361,15 +2361,15 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2383,10 +2383,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.502447</v>
+        <v>-58.498493</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.561008</v>
+        <v>-34.581262</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2402,7 +2402,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2412,17 +2412,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2459,10 +2459,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.483947</v>
+        <v>-58.502447</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.583207</v>
+        <v>-34.561008</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2478,7 +2478,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2488,17 +2488,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2531,14 +2531,14 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.503673</v>
+        <v>-58.483947</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.586925</v>
+        <v>-34.583207</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2554,7 +2554,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2574,7 +2574,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2607,14 +2607,14 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.504455</v>
+        <v>-58.503673</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.579941</v>
+        <v>-34.586925</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2630,7 +2630,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2687,10 +2687,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.503195</v>
+        <v>-58.504455</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.581735</v>
+        <v>-34.579941</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2706,7 +2706,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2763,14 +2763,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.493164</v>
+        <v>-58.503195</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.55732</v>
+        <v>-34.581735</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2782,7 +2782,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2839,14 +2839,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.491934</v>
+        <v>-58.493164</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.569348</v>
+        <v>-34.55732</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2915,10 +2915,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.501418</v>
+        <v>-58.491934</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.574363</v>
+        <v>-34.569348</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2934,7 +2934,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2991,14 +2991,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.494584</v>
+        <v>-58.501418</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.554981</v>
+        <v>-34.574363</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3010,27 +3010,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3045,11 +3045,11 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3063,14 +3063,14 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.465608</v>
+        <v>-58.494584</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.538489</v>
+        <v>-34.554981</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3086,27 +3086,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3139,18 +3139,18 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.436788</v>
+        <v>-58.465608</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.604014</v>
+        <v>-34.538489</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3162,7 +3162,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3172,17 +3172,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3219,46 +3219,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.439461</v>
+        <v>-58.436788</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.605744</v>
+        <v>-34.604014</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3295,46 +3295,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.473936</v>
+        <v>-58.439461</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.577346</v>
+        <v>-34.605744</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3349,7 +3349,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3371,46 +3371,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.372751</v>
+        <v>-58.473936</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.631917</v>
+        <v>-34.577346</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3447,14 +3447,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.387847</v>
+        <v>-58.372751</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.587043</v>
+        <v>-34.631917</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3466,27 +3466,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3496,12 +3496,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3514,7 +3514,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3523,26 +3523,26 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.451835</v>
+        <v>-58.387847</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.562646</v>
+        <v>-34.587043</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3552,17 +3552,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3572,12 +3572,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3585,28 +3585,28 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.470837</v>
+        <v>-58.451835</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.545751</v>
+        <v>-34.562646</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3618,7 +3618,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3628,7 +3628,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3666,19 +3666,19 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.472267</v>
+        <v>-58.470837</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.551163</v>
+        <v>-34.545751</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3694,27 +3694,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3737,12 +3737,12 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3751,10 +3751,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.464144</v>
+        <v>-58.472267</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.541832</v>
+        <v>-34.551163</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3770,7 +3770,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3780,17 +3780,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3827,26 +3827,26 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.434761</v>
+        <v>-58.464144</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.598381</v>
+        <v>-34.541832</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3856,17 +3856,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3899,30 +3899,30 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.464177</v>
+        <v>-58.434761</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.558239</v>
+        <v>-34.598381</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3932,17 +3932,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3975,50 +3975,50 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.412302</v>
+        <v>-58.464177</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.59301</v>
+        <v>-34.558239</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4031,7 +4031,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+        </is>
+      </c>
       <c r="I48" t="n">
         <v>1</v>
       </c>
@@ -4051,14 +4055,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.405761</v>
+        <v>-58.412302</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.582476</v>
+        <v>-34.59301</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4070,17 +4074,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4090,7 +4094,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4103,11 +4107,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H49" t="inlineStr"/>
       <c r="I49" t="n">
         <v>1</v>
       </c>
@@ -4127,14 +4127,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.432241</v>
+        <v>-58.405761</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.56642</v>
+        <v>-34.582476</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4146,7 +4146,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4166,7 +4166,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4203,10 +4203,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.417348</v>
+        <v>-58.432241</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.595467</v>
+        <v>-34.56642</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4222,27 +4222,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4275,18 +4275,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.472311</v>
+        <v>-58.417348</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.654867</v>
+        <v>-34.595467</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4298,7 +4298,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4308,17 +4308,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4333,7 +4333,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4351,50 +4351,50 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.484729</v>
+        <v>-58.472311</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.574614</v>
+        <v>-34.654867</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>7200</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4409,7 +4409,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4427,50 +4427,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.403422</v>
+        <v>-58.484729</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.609195</v>
+        <v>-34.574614</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>7200</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4507,26 +4507,26 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.470347</v>
+        <v>-58.403422</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.547965</v>
+        <v>-34.609195</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4536,17 +4536,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4579,18 +4579,18 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.510247</v>
+        <v>-58.470347</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.645038</v>
+        <v>-34.547965</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4602,27 +4602,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6695</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 4417</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808373646</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4655,18 +4655,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.478941</v>
+        <v>-58.510247</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.57242</v>
+        <v>-34.645038</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4678,27 +4678,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-521</t>
+          <t>6695</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Laferrere 6572</t>
+          <t>OLAZABAL AV. 4417</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808430950</t>
+          <t>808373646</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4713,7 +4713,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Entre edificio 12 y edificio 13 columna corroida en base tambalea</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4735,14 +4735,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.496608</v>
+        <v>-58.478941</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.666371</v>
+        <v>-34.57242</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4982,27 +4982,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6274</t>
+          <t>6561</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ARANGUREN, JUAN F., Dr. 2964</t>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808720858</t>
+          <t>808733912</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5039,26 +5039,26 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.473089</v>
+        <v>-58.468841</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.625478</v>
+        <v>-34.686635</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5068,17 +5068,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5115,14 +5115,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.468841</v>
+        <v>-58.375684</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.686635</v>
+        <v>-34.656092</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5134,27 +5134,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6979</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/18/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>RIVADAVIA AV. 6740</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>809006419</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5191,14 +5191,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.375684</v>
+        <v>-58.460441</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.656092</v>
+        <v>-34.628243</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5210,27 +5210,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6960</t>
+          <t>7149</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 1940</t>
+          <t>QUITO 3666</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808972988</t>
+          <t>809168441</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5267,14 +5267,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.460818</v>
+        <v>-58.41791</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.618934</v>
+        <v>-34.616706</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>7157</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>CALVO, CARLOS 1750</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>809257762</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5343,14 +5343,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.460441</v>
+        <v>-58.390806</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.628243</v>
+        <v>-34.620213</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5362,27 +5362,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7149</t>
+          <t>7088</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>QUITO 3666</t>
+          <t>HERRERA 1998</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809168441</t>
+          <t>809268244</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5415,18 +5415,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.41791</v>
+        <v>-58.37456</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.616706</v>
+        <v>-34.649779</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7157</t>
+          <t>7171</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1750</t>
+          <t>OLAZABAL AV. 5531</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809257762</t>
+          <t>809268253</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5495,36 +5495,36 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.390806</v>
+        <v>-58.491028</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.620213</v>
+        <v>-34.579381</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>7089</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/27/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>SAN ANTONIO 637</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>809270751</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5567,14 +5567,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.37456</v>
+        <v>-58.37805</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.649779</v>
+        <v>-34.649722</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5590,7 +5590,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7171</t>
+          <t>7090</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5600,17 +5600,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>OLAZABAL AV. 5531</t>
+          <t>SAN ANTONIO 625</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809268253</t>
+          <t>809270753</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5647,46 +5647,46 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.491028</v>
+        <v>-58.378104</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.579381</v>
+        <v>-34.649578</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>7096</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>VEDIA, AGUSTIN DE 2185</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>809279069</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5723,14 +5723,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.37805</v>
+        <v>-58.435511</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.649722</v>
+        <v>-34.644702</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5742,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>7169</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/5/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>SAN NICOLAS 5045</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>809492980</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste quebrado</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5795,50 +5795,50 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.378104</v>
+        <v>-58.515637</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.649578</v>
+        <v>-34.589993</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7091</t>
+          <t>7203</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SUAREZ AV. 1966</t>
+          <t>PERON, EVA AV. 1145</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809279022</t>
+          <t>809504290</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5875,14 +5875,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.377974</v>
+        <v>-58.441547</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.641024</v>
+        <v>-34.630481</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5894,27 +5894,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>7184</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>VALLEJOS 2221</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>809526160</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5929,7 +5929,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5951,42 +5951,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.435511</v>
+        <v>-58.493225</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.644702</v>
+        <v>-34.583095</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-581</t>
+          <t>-589</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9/4/2025</t>
+          <t>9/9/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Praga 1380</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr"/>
+          <t>Balbin 4059</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809432814</t>
+          <t>809575056</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6001,11 +6005,11 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Corrimiento ver con Pablo</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
@@ -6019,18 +6023,18 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.481608</v>
+        <v>-58.48797</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.587837</v>
+        <v>-34.554733</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6042,27 +6046,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>-590</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/9/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809575080</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6081,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Corrimiento ver con Pablo</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6095,18 +6099,18 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.515637</v>
+        <v>-58.487821</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.589993</v>
+        <v>-34.554603</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6118,27 +6122,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-583</t>
+          <t>7206</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>9/8/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Av Eva Perón 1145</t>
+          <t>VERACRUZ 3453</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809504290</t>
+          <t>809601009</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6175,14 +6179,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.441547</v>
+        <v>-58.445784</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.630481</v>
+        <v>-34.664364</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6194,27 +6198,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7174</t>
+          <t>-592</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/8/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>FERNANDEZ BLANCO 2320</t>
+          <t>VARELA 3018</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809526154</t>
+          <t>809642176</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6229,7 +6233,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Corrimiento columna evaluar con Pablo la posicion</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6251,323 +6255,19 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.481983</v>
+        <v>-58.435989</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.573931</v>
+        <v>-34.657716</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>7177</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>LUGONES 2830</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>809526156</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I78" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M78" t="n">
-        <v>-58.482786</v>
-      </c>
-      <c r="N78" t="n">
-        <v>-34.56748</v>
-      </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P78" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>7184</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>VALLEJOS 2221</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>809526160</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M79" t="n">
-        <v>-58.493225</v>
-      </c>
-      <c r="N79" t="n">
-        <v>-34.583095</v>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P79" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>-589</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>9/9/2025</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Balbin 4059</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>809575056</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Corrimiento ver con Pablo</t>
-        </is>
-      </c>
-      <c r="I80" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M80" t="n">
-        <v>-58.48797</v>
-      </c>
-      <c r="N80" t="n">
-        <v>-34.554733</v>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P80" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>-590</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>9/9/2025</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Holmberg 4002</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>809575080</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Corrimiento ver con Pablo</t>
-        </is>
-      </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M81" t="n">
-        <v>-58.487821</v>
-      </c>
-      <c r="N81" t="n">
-        <v>-34.554603</v>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-11 11:57:00)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -518,27 +518,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-3</t>
+          <t>1497</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1/5/2024</t>
+          <t>4/4/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FIGUEROA ALCORTA PTE ,AV. /ALT/ 5600</t>
+          <t>SANCHEZ DE BUSTAMANTE 2064</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>777580740</t>
+          <t>784804268</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Es F. ALCORTA 5600 (pasando Av de los ombues 100mts aprox.) Para cambiar es un poste con muchas rajaduras, en Figueroa Alcorta esq. Av de los Ombues</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -566,23 +566,23 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.425911</v>
+        <v>-58.406882</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.56033</v>
+        <v>-34.588287</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>6968</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1/13/2024</t>
+          <t>1/5/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SANTA FE AV. 5154</t>
+          <t>FIGUEROA ALCORTA PTE ,AV. /ALT/ 5600</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>777843837</t>
+          <t>777580740</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,11 +629,11 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Es F. ALCORTA 5600 (pasando Av de los ombues 100mts aprox.) Para cambiar es un poste con muchas rajaduras, en Figueroa Alcorta esq. Av de los Ombues</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -647,14 +647,14 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.432658</v>
+        <v>-58.425911</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.576446</v>
+        <v>-34.56033</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -670,27 +670,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-10</t>
+          <t>6968</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1/15/2024</t>
+          <t>1/13/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DARWIN /ALT/ 651</t>
+          <t>SANTA FE AV. 5154</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>777863458</t>
+          <t>777843837</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -703,9 +703,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -723,46 +727,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.44467</v>
+        <v>-58.432658</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.593784</v>
+        <v>-34.576446</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-30</t>
+          <t>-10</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2/21/2024</t>
+          <t>1/15/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>VEGA CNEL NICETO /ALT/ 4984</t>
+          <t>DARWIN /ALT/ 651</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>780352873</t>
+          <t>777863458</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -775,11 +779,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Recambio de columna</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>0</v>
       </c>
@@ -799,36 +799,36 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.433253</v>
+        <v>-58.44467</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.591026</v>
+        <v>-34.593784</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-103</t>
+          <t>-30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6/12/2024</t>
+          <t>2/21/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SALGUERO JERONIMO /ALT/ 2533</t>
+          <t>VEGA CNEL NICETO /ALT/ 4984</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -838,7 +838,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>788206681</t>
+          <t>780352873</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Altura correcta 2549</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -875,10 +875,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.409971</v>
+        <v>-58.433253</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.58175</v>
+        <v>-34.591026</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -894,27 +894,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-118</t>
+          <t>-103</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>8/15/2024</t>
+          <t>6/12/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SUCRE MRCAL A J DE /ALT/ 1437</t>
+          <t>SALGUERO JERONIMO /ALT/ 2533</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>793333193</t>
+          <t>788206681</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Retirar columna vieja, nodo ya traspasado</t>
+          <t>Altura correcta 2549</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -942,7 +942,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -951,36 +951,36 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.445523</v>
+        <v>-58.409971</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.558237</v>
+        <v>-34.58175</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-143</t>
+          <t>-118</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10/7/2024</t>
+          <t>8/15/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
+          <t>SUCRE MRCAL A J DE /ALT/ 1437</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>797752816</t>
+          <t>793333193</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1000,10 +1000,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Retirar columna vieja, nodo ya traspasado</t>
+        </is>
+      </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
@@ -1023,10 +1027,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.458864</v>
+        <v>-58.445523</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.561167</v>
+        <v>-34.558237</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1042,27 +1046,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-152</t>
+          <t>-143</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11/1/2024</t>
+          <t>10/7/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FERNANDEZ DE ENCISO /ALT/ 3610</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>798984311</t>
+          <t>797752816</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1072,14 +1076,10 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>El poste esta pegado al arbol ver la foto adjunta</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>0</v>
       </c>
@@ -1090,23 +1090,23 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.513363</v>
+        <v>-58.458864</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.605473</v>
+        <v>-34.561167</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1118,7 +1118,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-160</t>
+          <t>-152</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1128,17 +1128,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MORAN PEDRO /ALT/ 3100</t>
+          <t>FERNANDEZ DE ENCISO /ALT/ 3610</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>798984905</t>
+          <t>798984311</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1151,7 +1151,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>El poste esta pegado al arbol ver la foto adjunta</t>
+        </is>
+      </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
@@ -1171,14 +1175,14 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.498724</v>
+        <v>-58.513363</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.594329</v>
+        <v>-34.605473</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1190,27 +1194,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-201</t>
+          <t>-160</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>11/1/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1007</t>
+          <t>MORAN PEDRO /ALT/ 3100</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>799540497</t>
+          <t>798984905</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1223,11 +1227,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
-        </is>
-      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>0</v>
       </c>
@@ -1243,30 +1243,30 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.436377</v>
+        <v>-58.498724</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.565075</v>
+        <v>-34.594329</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-202</t>
+          <t>-201</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1030</t>
+          <t>MIGUELETES /ALT/ 1007</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>799540503</t>
+          <t>799540497</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Recambio de columna - alt correcta 1010</t>
+          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1323,10 +1323,10 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.436601</v>
+        <v>-58.436377</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.565035</v>
+        <v>-34.565075</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1342,17 +1342,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-216</t>
+          <t>-202</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/2/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
+          <t>MIGUELETES /ALT/ 1030</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>784655947</t>
+          <t>799540503</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1377,7 +1377,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Recambio de columna - alt correcta 1010</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1395,18 +1395,18 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.404652</v>
+        <v>-58.436601</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.58263</v>
+        <v>-34.565035</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1418,27 +1418,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-219</t>
+          <t>-216</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10/31/2024</t>
+          <t>5/2/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LA PAMPA /ALT/ 2836</t>
+          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>798953875</t>
+          <t>784655947</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1475,46 +1475,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.458282</v>
+        <v>-58.404652</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.56718</v>
+        <v>-34.58263</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-228</t>
+          <t>-219</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11/22/2024</t>
+          <t>10/31/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ALVAREZ JULIAN /ALT/ 1272</t>
+          <t>LA PAMPA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>800645527</t>
+          <t>798953875</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1551,46 +1551,46 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.426725</v>
+        <v>-58.458282</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.5945</v>
+        <v>-34.56718</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4082</t>
+          <t>-228</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>12/21/2024</t>
+          <t>11/22/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MERCEDES 254</t>
+          <t>ALVAREZ JULIAN /ALT/ 1272</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>801901755</t>
+          <t>800645527</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1600,16 +1600,16 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Colocar R200 para pedir traspaso de equipo</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1627,46 +1627,46 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.484232</v>
+        <v>-58.426725</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.631431</v>
+        <v>-34.5945</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-254</t>
+          <t>4082</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1/7/2025</t>
+          <t>12/21/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>BELAUSTEGUI DR LUIS /ALT/ 1185</t>
+          <t>MERCEDES 254</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>802367713</t>
+          <t>801901755</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1676,10 +1676,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Colocar R200 para pedir traspaso de equipo</t>
+        </is>
+      </c>
       <c r="I17" t="n">
         <v>1</v>
       </c>
@@ -1699,14 +1703,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.457158</v>
+        <v>-58.484232</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.605839</v>
+        <v>-34.631431</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1718,17 +1722,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4768</t>
+          <t>-254</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>1/7/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 684</t>
+          <t>BELAUSTEGUI DR LUIS /ALT/ 1185</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1738,7 +1742,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>802988221</t>
+          <t>802367713</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1751,11 +1755,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Picada info para cierre tambien entro como caso 6909</t>
-        </is>
-      </c>
+      <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
         <v>1</v>
       </c>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1775,19 +1775,19 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.443039</v>
+        <v>-58.457158</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.612262</v>
+        <v>-34.605839</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -1824,12 +1824,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>SIN RIEGO</t>
+          <t>Nodo transferido ya se puede retirar columna</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-15 12:07:33)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3998,27 +3998,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>5947</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>CAFAYATE 5007</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807129336</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4031,7 +4031,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Columna inclinada Columna con base corroída oxidada</t>
+        </is>
+      </c>
       <c r="I48" t="n">
         <v>1</v>
       </c>
@@ -4051,14 +4055,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.405761</v>
+        <v>-58.468182</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.582476</v>
+        <v>-34.685231</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4070,27 +4074,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>5948</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>MURGUIONDO 3990</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807129347</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4105,7 +4109,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4123,18 +4127,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.432241</v>
+        <v>-58.477944</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.56642</v>
+        <v>-34.675149</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4146,27 +4150,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>5954</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>YAPEYU 938</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807129372</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4181,7 +4185,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4203,14 +4207,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.417348</v>
+        <v>-58.4212</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.595467</v>
+        <v>-34.623575</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4222,27 +4226,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>5973</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>PALOS 432</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807168105</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4257,7 +4261,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4275,18 +4279,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.472311</v>
+        <v>-58.362579</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.654867</v>
+        <v>-34.635096</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4298,27 +4302,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>3715</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>EL SERENO 358</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807168098</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4333,7 +4337,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4341,7 +4345,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4355,14 +4359,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.484729</v>
+        <v>-58.487371</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.574614</v>
+        <v>-34.640099</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4374,27 +4378,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>7200</t>
+          <t>5997</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Paso 58</t>
+          <t>MARMOL, JOSE 256</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808194240</t>
+          <t>807187768</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4431,10 +4435,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.403422</v>
+        <v>-58.425845</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.609195</v>
+        <v>-34.616562</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4450,27 +4454,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6580</t>
+          <t>6004</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Ciudad de la Paz 3742</t>
+          <t>MAZA 181</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808240230</t>
+          <t>807215439</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4507,46 +4511,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.470347</v>
+        <v>-58.416477</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.547965</v>
+        <v>-34.61303</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6007</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>HUMAHUACA 4435</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>807215448</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4561,7 +4565,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4569,7 +4573,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4579,50 +4583,50 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.510247</v>
+        <v>-58.427424</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.645038</v>
+        <v>-34.601217</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6008</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>ESTADO DE ISRAEL AV. 4306</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>807215455</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4637,7 +4641,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4645,7 +4649,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4659,14 +4663,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.422229</v>
+        <v>-58.426665</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.573148</v>
+        <v>-34.598019</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4678,27 +4682,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4713,7 +4717,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Picada y mal ubicada ver con Pedro</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4721,7 +4725,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4731,18 +4735,18 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.494864</v>
+        <v>-58.425478</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.678826</v>
+        <v>-34.601865</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4754,27 +4758,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6561</t>
+          <t>6214</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+          <t>GONZALEZ, JOAQUIN V. 2308</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808733912</t>
+          <t>807605710</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4797,7 +4801,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4807,50 +4811,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.468841</v>
+        <v>-58.497698</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.686635</v>
+        <v>-34.612038</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4863,17 +4867,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Aplomar</t>
-        </is>
-      </c>
+      <c r="H59" t="inlineStr"/>
       <c r="I59" t="n">
         <v>1</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4887,14 +4887,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.375684</v>
+        <v>-58.405761</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.656092</v>
+        <v>-34.582476</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4906,27 +4906,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4959,50 +4959,50 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.461024</v>
+        <v>-58.432241</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.539409</v>
+        <v>-34.56642</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 6740</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>809006419</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5039,14 +5039,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.460441</v>
+        <v>-58.417348</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.628243</v>
+        <v>-34.595467</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5058,27 +5058,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7088</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>HERRERA 1998</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809268244</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5115,14 +5115,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.37456</v>
+        <v>-58.472311</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.649779</v>
+        <v>-34.654867</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5134,27 +5134,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7089</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/27/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 637</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809270751</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5187,50 +5187,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.37805</v>
+        <v>-58.484729</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.649722</v>
+        <v>-34.574614</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7090</t>
+          <t>6249</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 625</t>
+          <t>GODOY CRUZ 2696</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809270753</t>
+          <t>807789682</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Inclinada posible cambio</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5267,14 +5267,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.378104</v>
+        <v>-58.425296</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.649578</v>
+        <v>-34.578706</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,17 +5286,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7096</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2185</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809279069</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5343,46 +5343,46 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.435511</v>
+        <v>-58.474467</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.644702</v>
+        <v>-34.624161</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Colocar columna para pedir traspaso</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5410,55 +5410,55 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.515637</v>
+        <v>-58.401827</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.589993</v>
+        <v>-34.617667</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-589</t>
+          <t>6298</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>9/9/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Balbin 4059</t>
+          <t>RIVERA INDARTE AV. 1406</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809575056</t>
+          <t>807877127</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5473,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Corrimiento ver con Pablo</t>
+          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5491,50 +5491,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.48797</v>
+        <v>-58.450359</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.554733</v>
+        <v>-34.643582</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-590</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>9/9/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809575080</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Corrimiento ver con Pablo</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5571,46 +5571,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.487821</v>
+        <v>-58.413941</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.554603</v>
+        <v>-34.57698</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-592</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>VARELA 3018</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809642176</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Corrimiento columna evaluar con Pablo la posicion</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5643,50 +5643,50 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.435989</v>
+        <v>-58.473179</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.657716</v>
+        <v>-34.629138</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-595</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9/11/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Araujo 3433</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809687268</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5723,14 +5723,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.469721</v>
+        <v>-58.426322</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.668753</v>
+        <v>-34.600097</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5742,27 +5742,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7200</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>Paso 58</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>808194240</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5777,7 +5777,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5795,50 +5795,50 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.516218</v>
+        <v>-58.403422</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.589343</v>
+        <v>-34.609195</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>6580</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>Ciudad de la Paz 3742</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>808240230</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5871,21 +5871,1541 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M72" t="n">
+        <v>-58.470347</v>
+      </c>
+      <c r="N72" t="n">
+        <v>-34.547965</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>6398</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>7/15/2025</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>LARRAZABAL AV. 579</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>808373655</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Poste inclinado</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
+        <v>-58.510247</v>
+      </c>
+      <c r="N73" t="n">
+        <v>-34.645038</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>6497</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>7/25/2025</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>808533127</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Inclinada</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
+        <v>1</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
+        <v>-58.422229</v>
+      </c>
+      <c r="N74" t="n">
+        <v>-34.573148</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>6558</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>8/4/2025</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>NAZCA 5168</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>808703877</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>-58.505593</v>
+      </c>
+      <c r="N75" t="n">
+        <v>-34.582601</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>6556</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>8/4/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2 DE ABRIL DE 1982 6982</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>ICD30334420</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>-58.494864</v>
+      </c>
+      <c r="N76" t="n">
+        <v>-34.678826</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>6561</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GOLETA SARANDI 6050 </t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>808733912</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>-58.468841</v>
+      </c>
+      <c r="N77" t="n">
+        <v>-34.686635</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>6567</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>SAN ANTONIO 1221</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>808733914</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Aplomar</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>1</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>-58.375684</v>
+      </c>
+      <c r="N78" t="n">
+        <v>-34.656092</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>6579</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>8/7/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>808749184</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Poste inclinado ingreso tambien como 7201</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.461024</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.539409</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>6917</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>8/12/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>BRIN, MINISTRO 1375</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>808918700</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>PIcada</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.355342</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.63565</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>6979</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>8/18/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>RIVADAVIA AV. 6740</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>809006419</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Reclaman fuera de plomo ver si es necesario cambio</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.460441</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.628243</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>7088</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>HERRERA 1998</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809268244</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M72" t="n">
+      <c r="M82" t="n">
+        <v>-58.37456</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.649779</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>7089</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>8/27/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>SAN ANTONIO 637</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>809270751</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>-58.37805</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.649722</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>7090</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>SAN ANTONIO 625</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809270753</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.378104</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.649578</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>7096</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>VEDIA, AGUSTIN DE 2185</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>809279069</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.435511</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.644702</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>7169</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>9/5/2025</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>SAN NICOLAS 5045</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>809492980</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Poste quebrado</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>-58.515637</v>
+      </c>
+      <c r="N86" t="n">
+        <v>-34.589993</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>-589</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>9/9/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Balbin 4059</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>809575056</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Corrimiento ver con Pablo</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>-58.48797</v>
+      </c>
+      <c r="N87" t="n">
+        <v>-34.554733</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>-590</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>9/9/2025</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Holmberg 4002</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>809575080</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Corrimiento ver con Pablo</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M88" t="n">
+        <v>-58.487821</v>
+      </c>
+      <c r="N88" t="n">
+        <v>-34.554603</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>-592</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>9/10/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>VARELA 3018</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>809642176</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Corrimiento columna evaluar con Pablo la posicion</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.435989</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.657716</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>-595</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>9/11/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Araujo 3433</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>809687268</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>-58.469721</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.668753</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>7218</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>9/15/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>SAN NICOLAS 5123</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>809758863</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>-58.516218</v>
+      </c>
+      <c r="N91" t="n">
+        <v>-34.589343</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2005</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>9/15/2025</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>SANABRIA 4817</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>809758873</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
         <v>-58.520505</v>
       </c>
-      <c r="N72" t="n">
+      <c r="N92" t="n">
         <v>-34.596045</v>
       </c>
-      <c r="O72" t="inlineStr">
+      <c r="O92" t="inlineStr">
         <is>
           <t>Paternal</t>
         </is>
       </c>
-      <c r="P72" t="inlineStr">
+      <c r="P92" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-16 09:03:34)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6882,27 +6882,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>7237</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>NAZCA 3985</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809409491</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6917,7 +6917,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6935,14 +6935,14 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.515637</v>
+        <v>-58.497366</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.589993</v>
+        <v>-34.591544</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6958,27 +6958,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-589</t>
+          <t>7169</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>9/9/2025</t>
+          <t>9/5/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Balbin 4059</t>
+          <t>SAN NICOLAS 5045</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>809575056</t>
+          <t>809492980</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Corrimiento ver con Pablo</t>
+          <t>Poste quebrado</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7011,18 +7011,18 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.48797</v>
+        <v>-58.515637</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.554733</v>
+        <v>-34.589993</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -7034,7 +7034,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-590</t>
+          <t>-589</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7044,7 +7044,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Holmberg 4002</t>
+          <t>Balbin 4059</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -7054,7 +7054,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>809575080</t>
+          <t>809575056</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7087,14 +7087,14 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.487821</v>
+        <v>-58.48797</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.554603</v>
+        <v>-34.554733</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -7110,27 +7110,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>-592</t>
+          <t>-590</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/9/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>VARELA 3018</t>
+          <t>Holmberg 4002</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>809642176</t>
+          <t>809575080</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7145,7 +7145,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Corrimiento columna evaluar con Pablo la posicion</t>
+          <t>Corrimiento ver con Pablo</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7167,36 +7167,36 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.435989</v>
+        <v>-58.487821</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.657716</v>
+        <v>-34.554603</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>-595</t>
+          <t>-592</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>9/11/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Araujo 3433</t>
+          <t>VARELA 3018</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -7206,7 +7206,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>809687268</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -7221,7 +7221,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de columna</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -7243,14 +7243,14 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.469721</v>
+        <v>-58.435989</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.668753</v>
+        <v>-34.657716</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -7262,27 +7262,27 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7247</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/11/2025</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>ARAUJO 3430</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809687268</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -7297,7 +7297,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -7315,30 +7315,30 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M91" t="n">
-        <v>-58.516218</v>
+        <v>-58.46866</v>
       </c>
       <c r="N91" t="n">
-        <v>-34.589343</v>
+        <v>-34.669465</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -7348,7 +7348,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -7373,7 +7373,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -7391,23 +7391,251 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>-58.516218</v>
+      </c>
+      <c r="N92" t="n">
+        <v>-34.589343</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2005</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>9/15/2025</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>SANABRIA 4817</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>809758873</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+        </is>
+      </c>
+      <c r="I93" t="n">
+        <v>1</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M92" t="n">
+      <c r="M93" t="n">
         <v>-58.520505</v>
       </c>
-      <c r="N92" t="n">
+      <c r="N93" t="n">
         <v>-34.596045</v>
       </c>
-      <c r="O92" t="inlineStr">
+      <c r="O93" t="inlineStr">
         <is>
           <t>Paternal</t>
         </is>
       </c>
-      <c r="P92" t="inlineStr">
+      <c r="P93" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>7240</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>809784524</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>1</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
+        <v>-58.481316</v>
+      </c>
+      <c r="N94" t="n">
+        <v>-34.556157</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>7248</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>FERNANDEZ DE LA CRUZ, F., GRAL. AV. 4065</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>809784526</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Columna chocada </t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>1</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>-58.455155</v>
+      </c>
+      <c r="N95" t="n">
+        <v>-34.669378</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-17 14:56:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7278,7 +7278,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30830056</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -7334,27 +7334,27 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>7247</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>9/11/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>ARAUJO 3430</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>809687268</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -7391,46 +7391,46 @@
         </is>
       </c>
       <c r="M92" t="n">
-        <v>-58.46866</v>
+        <v>-58.458298</v>
       </c>
       <c r="N92" t="n">
-        <v>-34.669465</v>
+        <v>-34.566511</v>
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7247</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/11/2025</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>ARAUJO 3430</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809687268</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -7445,7 +7445,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I93" t="n">
@@ -7463,30 +7463,30 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M93" t="n">
-        <v>-58.516218</v>
+        <v>-58.46866</v>
       </c>
       <c r="N93" t="n">
-        <v>-34.589343</v>
+        <v>-34.669465</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -7496,7 +7496,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -7506,7 +7506,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -7521,7 +7521,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I94" t="n">
@@ -7539,14 +7539,14 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M94" t="n">
-        <v>-58.520505</v>
+        <v>-58.516218</v>
       </c>
       <c r="N94" t="n">
-        <v>-34.596045</v>
+        <v>-34.589343</v>
       </c>
       <c r="O94" t="inlineStr">
         <is>
@@ -7562,27 +7562,27 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -7597,7 +7597,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I95" t="n">
@@ -7619,14 +7619,14 @@
         </is>
       </c>
       <c r="M95" t="n">
-        <v>-58.481316</v>
+        <v>-58.520505</v>
       </c>
       <c r="N95" t="n">
-        <v>-34.556157</v>
+        <v>-34.596045</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P95" t="inlineStr">
@@ -7638,7 +7638,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>7248</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -7648,17 +7648,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>FERNANDEZ DE LA CRUZ, F., GRAL. AV. 4065</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>809784526</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -7673,7 +7673,7 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna chocada </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I96" t="n">
@@ -7691,50 +7691,50 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M96" t="n">
-        <v>-58.455155</v>
+        <v>-58.481316</v>
       </c>
       <c r="N96" t="n">
-        <v>-34.669378</v>
+        <v>-34.556157</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>7248</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>FERNANDEZ DE LA CRUZ, F., GRAL. AV. 4065</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809784526</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -7749,7 +7749,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t xml:space="preserve">Columna chocada </t>
         </is>
       </c>
       <c r="I97" t="n">
@@ -7757,7 +7757,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -7767,18 +7767,18 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M97" t="n">
-        <v>-58.409278</v>
+        <v>-58.455155</v>
       </c>
       <c r="N97" t="n">
-        <v>-34.653566</v>
+        <v>-34.669378</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P97" t="inlineStr">
@@ -7790,7 +7790,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>-599</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -7800,17 +7800,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Lavalleja 816</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>809800218</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -7825,7 +7825,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Picada sin riesgo de caida pedido por corporativos esta frenando un alta</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I98" t="n">
@@ -7833,31 +7833,183 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M98" t="n">
+        <v>-58.409278</v>
+      </c>
+      <c r="N98" t="n">
+        <v>-34.653566</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P98" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>-599</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>9/17/2025</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Lavalleja 816</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>809800218</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Picada sin riesgo de caida pedido por corporativos esta frenando un alta</t>
+        </is>
+      </c>
+      <c r="I99" t="n">
+        <v>1</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L98" t="inlineStr">
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M98" t="n">
+      <c r="M99" t="n">
         <v>-58.430997</v>
       </c>
-      <c r="N98" t="n">
+      <c r="N99" t="n">
         <v>-34.598654</v>
       </c>
-      <c r="O98" t="inlineStr">
+      <c r="O99" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P98" t="inlineStr">
+      <c r="P99" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>6182</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>9/17/2025</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Los Patos 2702</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>809818308</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+        </is>
+      </c>
+      <c r="I100" t="n">
+        <v>1</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M100" t="n">
+        <v>-58.399262</v>
+      </c>
+      <c r="N100" t="n">
+        <v>-34.639685</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-25 12:08:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:R78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>Zona</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>PD</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>N2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -588,6 +598,16 @@
       <c r="P2" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>AGU-E</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -662,6 +682,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>PUE-B</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -738,6 +768,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>BLO-?</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -812,6 +852,16 @@
       <c r="P5" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>ATH-?</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -886,6 +936,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>VCR-I</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -962,6 +1022,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>VCR-F</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1038,6 +1108,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>AGU-O</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1112,6 +1192,16 @@
       <c r="P9" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>BLO-A</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -1186,6 +1276,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>COG-H</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1260,6 +1360,16 @@
       <c r="P11" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>DEV-F</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1DEV</t>
         </is>
       </c>
     </row>
@@ -1334,6 +1444,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>PUE-G</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1410,6 +1530,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>BLO-J</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1486,6 +1616,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>BLO-J</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1562,6 +1702,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>AGU-N</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1638,6 +1788,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>COG-F</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1714,6 +1874,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>DEV-L</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2DEV</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1790,6 +1960,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>VCR-N</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1866,6 +2046,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>DEV-F</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1DEV</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1942,6 +2132,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>VCR-O</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2018,6 +2218,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>PUE-M</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2094,6 +2304,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>PUE-H</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2170,6 +2390,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>ATH-S</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2246,6 +2476,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>PUE-M</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2322,6 +2562,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2398,6 +2648,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>PUE-M</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2474,6 +2734,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>COG-A</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2550,6 +2820,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>PUE-F</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2626,6 +2906,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>PUE-I</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2702,6 +2992,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>BLO-?</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2778,6 +3078,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>ALM-N</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2854,6 +3164,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>ALM-O</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2930,6 +3250,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>ATH-J</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3006,6 +3336,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>CON-B</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3082,6 +3422,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>RET-A</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3158,6 +3508,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>BLO-N</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3234,6 +3594,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>COG-?</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3310,6 +3680,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>BLO-F</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3386,6 +3766,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>CLI-O</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3462,6 +3852,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>COG-K</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3538,6 +3938,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>AGU-C</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3614,6 +4024,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>PAV-V</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3690,6 +4110,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>ALM-A</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3766,6 +4196,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>CON-G</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3842,6 +4282,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>PCH-S</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2PCH</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3918,6 +4368,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>CLI-I</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3994,6 +4454,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>CLI-M</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4070,6 +4540,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>CLI-N</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4144,6 +4624,16 @@
       <c r="P49" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>DEV-D</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -4218,6 +4708,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>AGU-N</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4294,6 +4794,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>BLO-I</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4370,6 +4880,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>VCR-B</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4446,6 +4966,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>PAV-O</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4522,6 +5052,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>ATH-C</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4598,6 +5138,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>VCR-N</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4672,6 +5222,16 @@
       <c r="P56" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>NRA-R</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
@@ -4746,6 +5306,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>CEN-M</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4822,6 +5392,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>AGU-P</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4898,6 +5478,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>NRA-R</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2NRA</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4974,6 +5564,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>CLI-M</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -5050,6 +5650,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>PAV-E</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5126,6 +5736,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>VCR-M</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -5202,6 +5822,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>PAV-M</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -5278,6 +5908,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>CON-I</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5354,6 +5994,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>BLO-F</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -5430,6 +6080,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>CON-G</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5506,6 +6166,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>CLI-H</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5582,6 +6252,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5658,6 +6338,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>COG-F</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5734,6 +6424,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5810,6 +6510,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>PUE-O</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -5886,6 +6596,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>COG-O</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5962,6 +6682,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>PPT-H</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -6038,6 +6768,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>CLI-N</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -6114,6 +6854,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>PPT-K</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -6190,6 +6940,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>VCR-O</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -6266,6 +7026,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>COG-C</t>
+        </is>
+      </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -6340,6 +7110,16 @@
       <c r="P78" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>NRA-H</t>
+        </is>
+      </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-27 09:16:12)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -4468,7 +4468,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6008</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4306</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807215455</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4503,7 +4503,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada y mal ubicada ver con Pedro</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4525,10 +4525,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.426665</v>
+        <v>-58.425478</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.598019</v>
+        <v>-34.601865</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>CLI-M</t>
+          <t>CLI-N</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -4554,27 +4554,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>6214</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>GONZALEZ, JOAQUIN V. 2308</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>807605710</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4589,7 +4589,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada ver con Pedro</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4597,7 +4597,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4607,28 +4607,28 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.425478</v>
+        <v>-58.497698</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.601865</v>
+        <v>-34.612038</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>DEV-D</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -4640,7 +4640,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6214</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4650,17 +4650,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807605710</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4673,17 +4673,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H50" t="inlineStr"/>
       <c r="I50" t="n">
         <v>1</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4693,28 +4689,28 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.497698</v>
+        <v>-58.405761</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.612038</v>
+        <v>-34.582476</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>DEV-D</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -4726,17 +4722,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4746,7 +4742,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4759,7 +4755,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I51" t="n">
         <v>1</v>
       </c>
@@ -4779,14 +4779,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4796,7 +4796,7 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -4808,7 +4808,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4818,7 +4818,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4828,7 +4828,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4843,7 +4843,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4865,10 +4865,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4882,7 +4882,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>VCR-B</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -4894,27 +4894,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4947,18 +4947,18 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.417348</v>
+        <v>-58.472311</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.595467</v>
+        <v>-34.654867</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4968,7 +4968,7 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>VCR-B</t>
+          <t>PAV-O</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -4980,7 +4980,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4990,17 +4990,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5015,7 +5015,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -5033,28 +5033,28 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.472311</v>
+        <v>-58.484729</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.654867</v>
+        <v>-34.574614</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>PAV-O</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5066,27 +5066,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6249</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>GODOY CRUZ 2696</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807789682</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Inclinada posible cambio</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -5119,28 +5119,28 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.484729</v>
+        <v>-58.425296</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.574614</v>
+        <v>-34.578706</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>ATH-C</t>
+          <t>VCR-N</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5152,27 +5152,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6249</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2696</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807789682</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Inclinada posible cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5209,56 +5209,56 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.425296</v>
+        <v>-58.474467</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.578706</v>
+        <v>-34.624161</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>VCR-N</t>
+          <t>NRA-R</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ARGERICH 740</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807789686</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5268,14 +5268,10 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr"/>
       <c r="I57" t="n">
         <v>1</v>
       </c>
@@ -5286,7 +5282,7 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
@@ -5295,56 +5291,56 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.474467</v>
+        <v>-58.401827</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.624161</v>
+        <v>-34.617667</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>NRA-R</t>
+          <t>CEN-M</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2NRA</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5354,10 +5350,14 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Picada e inclinada</t>
+        </is>
+      </c>
       <c r="I58" t="n">
         <v>1</v>
       </c>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
@@ -5377,14 +5377,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.401827</v>
+        <v>-58.413941</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.617667</v>
+        <v>-34.57698</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>CEN-M</t>
+          <t>AGU-P</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
@@ -5406,27 +5406,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5441,7 +5441,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -5449,7 +5449,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -5459,60 +5459,60 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.413941</v>
+        <v>-58.473179</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.57698</v>
+        <v>-34.629138</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>AGU-P</t>
+          <t>NRA-R</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>6398</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>LARRAZABAL AV. 579</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>808373655</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5527,7 +5527,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -5535,7 +5535,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -5545,14 +5545,14 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.473179</v>
+        <v>-58.510247</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.629138</v>
+        <v>-34.645038</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -5566,39 +5566,39 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>NRA-R</t>
+          <t>PAV-E</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2NRA</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5635,14 +5635,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.426322</v>
+        <v>-58.422229</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.600097</v>
+        <v>-34.573148</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5652,7 +5652,7 @@
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>CLI-M</t>
+          <t>VCR-M</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5664,27 +5664,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>7336</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>CRAMER AV. 2141</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5699,7 +5699,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5707,7 +5707,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5717,18 +5717,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.510247</v>
+        <v>-58.461582</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.645038</v>
+        <v>-34.564296</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5738,7 +5738,7 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>PAV-E</t>
+          <t>COG-H</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -5750,27 +5750,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5793,7 +5793,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5803,18 +5803,18 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.422229</v>
+        <v>-58.494864</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.573148</v>
+        <v>-34.678826</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5824,7 +5824,7 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>VCR-M</t>
+          <t>PAV-M</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -5836,27 +5836,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5871,7 +5871,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5879,7 +5879,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5889,18 +5889,18 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.494864</v>
+        <v>-58.375684</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.678826</v>
+        <v>-34.656092</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5910,7 +5910,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>PAV-M</t>
+          <t>CON-I</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -5922,27 +5922,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5957,7 +5957,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste inclinado ingreso tambien como 7201</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5975,28 +5975,28 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.375684</v>
+        <v>-58.461024</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.656092</v>
+        <v>-34.539409</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>CON-I</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -6008,27 +6008,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6043,7 +6043,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -6051,7 +6051,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -6061,28 +6061,28 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.461024</v>
+        <v>-58.355342</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.539409</v>
+        <v>-34.63565</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>CON-G</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -6094,27 +6094,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6917</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1375</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808918700</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6129,7 +6129,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -6151,24 +6151,24 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.355342</v>
+        <v>-58.472869</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.63565</v>
+        <v>-34.562</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>CON-G</t>
+          <t>COG-I</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6180,27 +6180,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>7169</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/5/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
+          <t>SAN NICOLAS 5045</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>809492980</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6215,7 +6215,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste quebrado</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -6233,28 +6233,28 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.410025</v>
+        <v>-58.515637</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.609184</v>
+        <v>-34.589993</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>CLI-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6266,27 +6266,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -6319,18 +6319,18 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.515637</v>
+        <v>-58.458298</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.589993</v>
+        <v>-34.566511</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -6340,7 +6340,7 @@
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6352,27 +6352,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6387,7 +6387,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -6405,18 +6405,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.458298</v>
+        <v>-58.516218</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.566511</v>
+        <v>-34.589343</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -6426,7 +6426,7 @@
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -6438,7 +6438,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -6448,7 +6448,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -6458,7 +6458,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6473,7 +6473,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -6491,14 +6491,14 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.516218</v>
+        <v>-58.520505</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.589343</v>
+        <v>-34.596045</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -6512,39 +6512,39 @@
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6559,7 +6559,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -6581,14 +6581,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.520505</v>
+        <v>-58.481316</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.596045</v>
+        <v>-34.556157</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -6598,39 +6598,39 @@
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6645,7 +6645,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -6653,7 +6653,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -6667,24 +6667,24 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.481316</v>
+        <v>-58.409278</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.556157</v>
+        <v>-34.653566</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
@@ -6696,7 +6696,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>-599</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -6706,17 +6706,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>Lavalleja 816</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809800218</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6731,7 +6731,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada sin riesgo de caida pedido por corporativos esta frenando un alta</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6739,7 +6739,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6749,18 +6749,18 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.409278</v>
+        <v>-58.430997</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.653566</v>
+        <v>-34.598654</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6770,7 +6770,7 @@
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>CLI-N</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -6782,7 +6782,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-599</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6792,17 +6792,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Lavalleja 816</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809800218</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6817,7 +6817,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada sin riesgo de caida pedido por corporativos esta frenando un alta</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6839,14 +6839,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.430997</v>
+        <v>-58.399262</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.598654</v>
+        <v>-34.639685</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6856,7 +6856,7 @@
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -6868,27 +6868,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>-602</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/18/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>Agustin de vedia 2111</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809837501</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6903,7 +6903,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6925,14 +6925,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.399262</v>
+        <v>-58.435637</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.639685</v>
+        <v>-34.64435</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6942,7 +6942,7 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PPT-O</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
@@ -6954,27 +6954,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-602</t>
+          <t>-604</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/18/2025</t>
+          <t>9/22/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Agustin de vedia 2111</t>
+          <t>Gurruchaga 2126</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809837501</t>
+          <t>809929884</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6989,7 +6989,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna cortada sostenida por la red</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -7011,14 +7011,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.435637</v>
+        <v>-58.424217</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.64435</v>
+        <v>-34.586032</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>PPT-O</t>
+          <t>VCR-O</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
@@ -7040,27 +7040,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-604</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/22/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Gurruchaga 2126</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809929884</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7075,7 +7075,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Columna cortada sostenida por la red</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -7088,7 +7088,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
@@ -7097,24 +7097,24 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.424217</v>
+        <v>-58.447743</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.586032</v>
+        <v>-34.570457</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>VCR-O</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -7126,27 +7126,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7161,7 +7161,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -7174,7 +7174,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
@@ -7183,14 +7183,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.447743</v>
+        <v>-58.452532</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.570457</v>
+        <v>-34.609005</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -7200,7 +7200,7 @@
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>NRA-H</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -7212,7 +7212,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>7296</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -7222,17 +7222,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>VEDIA, AGUSTIN DE 2130</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>809979719</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -7247,7 +7247,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t xml:space="preserve">3 columnas picadas ver en calle cuales son necesarias cambiar con Pablo </t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -7269,24 +7269,24 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.452532</v>
+        <v>-58.435634</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.609005</v>
+        <v>-34.64412</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>NRA-H</t>
+          <t>PPT-O</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
@@ -7298,27 +7298,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7296</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2130</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809979719</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -7333,7 +7333,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 columnas picadas ver en calle cuales son necesarias cambiar con Pablo </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -7355,24 +7355,24 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.435634</v>
+        <v>-58.485454</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.64412</v>
+        <v>-34.555745</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>PPT-O</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -7384,7 +7384,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -7394,17 +7394,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -7419,7 +7419,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -7437,18 +7437,18 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.485454</v>
+        <v>-58.509324</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.555745</v>
+        <v>-34.635335</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -7458,19 +7458,19 @@
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -7480,17 +7480,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -7505,7 +7505,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -7523,14 +7523,14 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.509324</v>
+        <v>-58.501431</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.635335</v>
+        <v>-34.647791</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -7544,39 +7544,39 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7321</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>9/26/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>BOYACA 1108</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>810015417</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -7591,7 +7591,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar terminal</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -7609,18 +7609,18 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.501431</v>
+        <v>-58.464691</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.647791</v>
+        <v>-34.615559</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -7630,7 +7630,7 @@
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>NRA-J</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-07 09:01:18)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,16 +514,6 @@
           <t>Zona</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>PD</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>N2</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -598,16 +588,6 @@
       <c r="P2" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>AGU-E</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -682,16 +662,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>PUE-B</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -766,16 +736,6 @@
       <c r="P4" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>BLO-?</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -850,16 +810,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>VCR-I</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -936,16 +886,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>AGU-O</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1020,16 +960,6 @@
       <c r="P7" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>BLO-A</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -1104,16 +1034,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>COG-H</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1188,16 +1108,6 @@
       <c r="P9" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>DEV-F</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1DEV</t>
         </is>
       </c>
     </row>
@@ -1272,16 +1182,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>PUE-G</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1358,16 +1258,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>BLO-J</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1444,16 +1334,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>BLO-J</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1530,16 +1410,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>AGU-N</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1616,16 +1486,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>COG-F</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1702,16 +1562,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>DEV-L</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.2DEV</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1788,16 +1638,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>DEV-F</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1DEV</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1874,16 +1714,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>VCR-O</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1960,16 +1790,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>PUE-M</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PUE</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2046,16 +1866,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>PUE-H</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2132,16 +1942,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>ATH-S</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2218,16 +2018,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>PUE-M</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PUE</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2304,16 +2094,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>PUE-J</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2390,16 +2170,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>PUE-M</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PUE</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2476,16 +2246,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>COG-A</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2562,16 +2322,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>PUE-F</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2648,16 +2398,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>PUE-I</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2734,16 +2474,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>BLO-?</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2820,16 +2550,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>ALM-N</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2906,16 +2626,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>ALM-O</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2992,16 +2702,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>ATH-J</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3078,16 +2778,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>CON-B</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3164,16 +2854,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>RET-A</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3250,16 +2930,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>BLO-N</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3336,16 +3006,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>COG-?</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3422,16 +3082,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>BLO-F</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3508,16 +3158,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>COG-K</t>
-        </is>
-      </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3594,16 +3234,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>AGU-C</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3680,16 +3310,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>PAV-V</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3766,16 +3386,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>ALM-A</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3852,16 +3462,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>CON-G</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3938,16 +3538,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>PCH-S</t>
-        </is>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.2PCH</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4024,16 +3614,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>CLI-I</t>
-        </is>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4110,16 +3690,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>CLI-N</t>
-        </is>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4194,16 +3764,6 @@
       <c r="P44" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>DEV-D</t>
-        </is>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -4278,16 +3838,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>AGU-N</t>
-        </is>
-      </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4364,16 +3914,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>BLO-I</t>
-        </is>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4450,16 +3990,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>VCR-B</t>
-        </is>
-      </c>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4536,16 +4066,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>PAV-O</t>
-        </is>
-      </c>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4622,16 +4142,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>ATH-C</t>
-        </is>
-      </c>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4706,16 +4216,6 @@
       <c r="P50" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>NRA-R</t>
-        </is>
-      </c>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
@@ -4790,16 +4290,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>CEN-M</t>
-        </is>
-      </c>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4876,16 +4366,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>AGU-P</t>
-        </is>
-      </c>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4962,41 +4442,31 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>NRA-R</t>
-        </is>
-      </c>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.2NRA</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6398</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>LARRAZABAL AV. 579</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808373655</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5011,7 +4481,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -5029,60 +4499,50 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.510247</v>
+        <v>-58.422229</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.645038</v>
+        <v>-34.573148</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>PAV-E</t>
-        </is>
-      </c>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>7336</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>CRAMER AV. 2141</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5097,7 +4557,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -5105,7 +4565,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -5119,56 +4579,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.422229</v>
+        <v>-58.461582</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.573148</v>
+        <v>-34.564296</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>VCR-M</t>
-        </is>
-      </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>7336</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CRAMER AV. 2141</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5183,7 +4633,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5191,7 +4641,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -5201,60 +4651,50 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.461582</v>
+        <v>-58.494864</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.564296</v>
+        <v>-34.678826</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>COG-H</t>
-        </is>
-      </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5269,7 +4709,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -5277,7 +4717,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -5287,60 +4727,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.494864</v>
+        <v>-58.375684</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.678826</v>
+        <v>-34.656092</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>PAV-M</t>
-        </is>
-      </c>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5355,7 +4785,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste inclinado ingreso tambien como 7201</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -5373,60 +4803,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.375684</v>
+        <v>-58.461024</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.656092</v>
+        <v>-34.539409</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>CON-I</t>
-        </is>
-      </c>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5441,7 +4861,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -5449,7 +4869,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -5459,60 +4879,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.461024</v>
+        <v>-58.355342</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.539409</v>
+        <v>-34.63565</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>BLO-F</t>
-        </is>
-      </c>
-      <c r="R59" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6917</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1375</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808918700</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5527,7 +4937,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -5549,56 +4959,46 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.355342</v>
+        <v>-58.472869</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.63565</v>
+        <v>-34.562</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>CON-G</t>
-        </is>
-      </c>
-      <c r="R60" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5635,56 +5035,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.472869</v>
+        <v>-58.434651</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.562</v>
+        <v>-34.598814</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>COG-I</t>
-        </is>
-      </c>
-      <c r="R61" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7169</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/5/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>SAN NICOLAS 5045</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809492980</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5699,7 +5089,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste quebrado</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5717,60 +5107,50 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.434651</v>
+        <v>-58.515637</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.598814</v>
+        <v>-34.589993</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>CLI-O</t>
-        </is>
-      </c>
-      <c r="R62" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5785,7 +5165,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5803,60 +5183,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.515637</v>
+        <v>-58.458298</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.589993</v>
+        <v>-34.566511</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>PUE-J</t>
-        </is>
-      </c>
-      <c r="R63" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5871,7 +5241,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5889,40 +5259,30 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.458298</v>
+        <v>-58.516218</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.566511</v>
+        <v>-34.589343</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>COG-F</t>
-        </is>
-      </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5932,7 +5292,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5942,7 +5302,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5957,7 +5317,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5975,14 +5335,14 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.516218</v>
+        <v>-58.520505</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.589343</v>
+        <v>-34.596045</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5992,43 +5352,33 @@
       <c r="P65" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q65" t="inlineStr">
-        <is>
-          <t>PUE-J</t>
-        </is>
-      </c>
-      <c r="R65" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6043,7 +5393,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -6065,56 +5415,46 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.520505</v>
+        <v>-58.481316</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.596045</v>
+        <v>-34.556157</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>PUE-O</t>
-        </is>
-      </c>
-      <c r="R66" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6129,7 +5469,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -6137,7 +5477,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -6151,36 +5491,26 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.481316</v>
+        <v>-58.409278</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.556157</v>
+        <v>-34.653566</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>COG-O</t>
-        </is>
-      </c>
-      <c r="R67" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -6190,7 +5520,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -6200,7 +5530,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6215,7 +5545,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -6223,7 +5553,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -6233,14 +5563,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.409278</v>
+        <v>-58.399262</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.653566</v>
+        <v>-34.639685</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -6250,43 +5580,33 @@
       <c r="P68" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>PPT-H</t>
-        </is>
-      </c>
-      <c r="R68" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>-602</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/18/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>Agustin de vedia 2111</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809837501</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6301,7 +5621,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -6323,56 +5643,46 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.399262</v>
+        <v>-58.435637</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.639685</v>
+        <v>-34.64435</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>PPT-K</t>
-        </is>
-      </c>
-      <c r="R69" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-602</t>
+          <t>-604</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9/18/2025</t>
+          <t>9/22/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Agustin de vedia 2111</t>
+          <t>Gurruchaga 2126</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809837501</t>
+          <t>809929884</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6387,7 +5697,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna cortada sostenida por la red</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -6409,56 +5719,46 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.435637</v>
+        <v>-58.424217</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.64435</v>
+        <v>-34.586032</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>PPT-O</t>
-        </is>
-      </c>
-      <c r="R70" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-604</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>9/22/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Gurruchaga 2126</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809929884</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6473,7 +5773,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Columna cortada sostenida por la red</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -6486,7 +5786,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -6495,56 +5795,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.424217</v>
+        <v>-58.447743</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.586032</v>
+        <v>-34.570457</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>VCR-O</t>
-        </is>
-      </c>
-      <c r="R71" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6559,7 +5849,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -6572,7 +5862,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -6581,36 +5871,26 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.447743</v>
+        <v>-58.452532</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.570457</v>
+        <v>-34.609005</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>COG-C</t>
-        </is>
-      </c>
-      <c r="R72" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>7296</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -6620,17 +5900,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>VEDIA, AGUSTIN DE 2130</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>809979719</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6645,7 +5925,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t xml:space="preserve">3 columnas picadas ver en calle cuales son necesarias cambiar con Pablo </t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -6667,56 +5947,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.452532</v>
+        <v>-58.435634</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.609005</v>
+        <v>-34.64412</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>NRA-H</t>
-        </is>
-      </c>
-      <c r="R73" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7296</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2130</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809979719</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6731,7 +6001,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 columnas picadas ver en calle cuales son necesarias cambiar con Pablo </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6753,36 +6023,26 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.435634</v>
+        <v>-58.485454</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.64412</v>
+        <v>-34.555745</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>PPT-O</t>
-        </is>
-      </c>
-      <c r="R74" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6792,17 +6052,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6817,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6835,40 +6095,30 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.485454</v>
+        <v>-58.509324</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.555745</v>
+        <v>-34.635335</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q75" t="inlineStr">
-        <is>
-          <t>COG-O</t>
-        </is>
-      </c>
-      <c r="R75" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6878,17 +6128,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6903,7 +6153,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6921,14 +6171,14 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.509324</v>
+        <v>-58.501431</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.635335</v>
+        <v>-34.647791</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6938,43 +6188,33 @@
       <c r="P76" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>DEV-M</t>
-        </is>
-      </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7359</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>9/29/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>VEGA, NICETO, CNEL. 4678</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>810056579</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6989,7 +6229,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada con base corroida</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -7011,56 +6251,46 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.501431</v>
+        <v>-58.430056</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.647791</v>
+        <v>-34.593188</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>PAV-?</t>
-        </is>
-      </c>
-      <c r="R77" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-617</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/29/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Soler 3815</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD31437343</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7075,15 +6305,15 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Desmonte de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -7097,56 +6327,46 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.416328</v>
+        <v>-58.384406</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.592509</v>
+        <v>-34.622932</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>VCR-C</t>
-        </is>
-      </c>
-      <c r="R78" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7359</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>9/29/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>VEGA, NICETO, CNEL. 4678</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>810056579</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7161,7 +6381,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroida</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -7183,36 +6403,26 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.430056</v>
+        <v>-58.521719</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.593188</v>
+        <v>-34.647467</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>VCR-F</t>
-        </is>
-      </c>
-      <c r="R79" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -7222,17 +6432,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -7269,36 +6479,26 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.384406</v>
+        <v>-58.461482</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.622932</v>
+        <v>-34.632432</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q80" t="inlineStr">
-        <is>
-          <t>CON-M</t>
-        </is>
-      </c>
-      <c r="R80" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7402</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -7308,17 +6508,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>RIVADAVIA AV. 2479</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132836</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -7333,7 +6533,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -7355,36 +6555,26 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.521719</v>
+        <v>-58.401428</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.647467</v>
+        <v>-34.609797</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q81" t="inlineStr">
-        <is>
-          <t>PAV-C</t>
-        </is>
-      </c>
-      <c r="R81" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7405</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -7394,17 +6584,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>CHILE 2115</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132907</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -7441,46 +6631,36 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.461482</v>
+        <v>-58.396368</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.632432</v>
+        <v>-34.61718</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>PCH-F</t>
-        </is>
-      </c>
-      <c r="R82" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7402</t>
+          <t>7410</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 2479</t>
+          <t>CHILE 2163</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -7490,7 +6670,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>810132836</t>
+          <t>810132956</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -7505,7 +6685,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -7527,10 +6707,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.401428</v>
+        <v>-58.397024</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.609797</v>
+        <v>-34.617234</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -7540,188 +6720,6 @@
       <c r="P83" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>CLI-D</t>
-        </is>
-      </c>
-      <c r="R83" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>7405</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>10/2/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>CHILE 2115</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>810132907</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>-58.396368</v>
-      </c>
-      <c r="N84" t="n">
-        <v>-34.61718</v>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q84" t="inlineStr">
-        <is>
-          <t>CEN-C</t>
-        </is>
-      </c>
-      <c r="R84" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>7410</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>10/1/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>CHILE 2163</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>810132956</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.397024</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.617234</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q85" t="inlineStr">
-        <is>
-          <t>CEN-C</t>
-        </is>
-      </c>
-      <c r="R85" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-08 08:23:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:R80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>Zona</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>PD</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>N2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -588,6 +598,16 @@
       <c r="P2" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>AGU-E</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -662,6 +682,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>PUE-B</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -736,6 +766,16 @@
       <c r="P4" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>BLO-?</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -810,6 +850,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>VCR-I</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -886,6 +936,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>AGU-O</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -960,6 +1020,16 @@
       <c r="P7" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>BLO-A</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -1034,6 +1104,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>COG-H</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1108,6 +1188,16 @@
       <c r="P9" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>DEV-F</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1DEV</t>
         </is>
       </c>
     </row>
@@ -1182,6 +1272,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>PUE-G</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1258,6 +1358,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>BLO-J</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1334,6 +1444,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>BLO-J</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1410,6 +1530,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>AGU-N</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1486,6 +1616,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>COG-F</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1562,6 +1702,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>DEV-L</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2DEV</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1638,6 +1788,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>DEV-F</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1DEV</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1714,6 +1874,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>VCR-O</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1790,6 +1960,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>PUE-M</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1866,6 +2046,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>PUE-H</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1942,6 +2132,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>ATH-S</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2018,6 +2218,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>PUE-M</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2094,6 +2304,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2170,6 +2390,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>PUE-M</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2246,6 +2476,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>COG-A</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2322,6 +2562,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>PUE-F</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2398,6 +2648,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>PUE-I</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2474,6 +2734,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>BLO-?</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2550,6 +2820,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>ALM-N</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2626,6 +2906,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>ALM-O</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2702,6 +2992,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>ATH-J</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2778,6 +3078,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>CON-B</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2854,6 +3164,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>RET-A</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2930,6 +3250,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>BLO-N</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3006,6 +3336,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>COG-?</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3082,6 +3422,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>BLO-F</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3158,6 +3508,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>COG-K</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3234,6 +3594,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>AGU-C</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3310,6 +3680,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>PAV-V</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3386,6 +3766,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>ALM-A</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3462,6 +3852,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>CON-G</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3538,6 +3938,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>PCH-S</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2PCH</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3614,6 +4024,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>CLI-I</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3690,11 +4110,21 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>CLI-N</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6214</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3704,17 +4134,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807605710</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3727,17 +4157,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H44" t="inlineStr"/>
       <c r="I44" t="n">
         <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3747,40 +4173,50 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.497698</v>
+        <v>-58.405761</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.612038</v>
+        <v>-34.582476</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>AGU-N</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3790,7 +4226,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3803,7 +4239,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I45" t="n">
         <v>1</v>
       </c>
@@ -3823,26 +4263,36 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.405761</v>
+        <v>-58.432241</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.582476</v>
+        <v>-34.56642</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>BLO-I</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3852,7 +4302,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3862,7 +4312,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3877,7 +4327,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3899,10 +4349,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.432241</v>
+        <v>-58.417348</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.56642</v>
+        <v>-34.595467</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3912,33 +4362,43 @@
       <c r="P46" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>VCR-B</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3953,7 +4413,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3971,50 +4431,60 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.417348</v>
+        <v>-58.484729</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.595467</v>
+        <v>-34.574614</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>ATH-C</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6223</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ECHEANDIA 4200</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807762996</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4029,7 +4499,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna inclinada con base  corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4047,50 +4517,60 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.472311</v>
+        <v>-58.474467</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.654867</v>
+        <v>-34.624161</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>NRA-R</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4100,14 +4580,10 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr"/>
       <c r="I49" t="n">
         <v>1</v>
       </c>
@@ -4118,45 +4594,55 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.484729</v>
+        <v>-58.401827</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.574614</v>
+        <v>-34.617667</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>CEN-M</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ARGERICH 740</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4166,7 +4652,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807789686</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4181,7 +4667,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4189,7 +4675,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4199,14 +4685,14 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.474467</v>
+        <v>-58.473179</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.624161</v>
+        <v>-34.629138</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4216,33 +4702,43 @@
       <c r="P50" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>NRA-R</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4252,21 +4748,25 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Inclinada</t>
+        </is>
+      </c>
       <c r="I51" t="n">
         <v>1</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4275,46 +4775,56 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.401827</v>
+        <v>-58.422229</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.617667</v>
+        <v>-34.573148</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>VCR-M</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>7336</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>CRAMER AV. 2141</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4329,7 +4839,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4351,46 +4861,56 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.413941</v>
+        <v>-58.461582</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.57698</v>
+        <v>-34.564296</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>COG-H</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4405,7 +4925,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4413,7 +4933,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4423,50 +4943,60 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.473179</v>
+        <v>-58.494864</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.629138</v>
+        <v>-34.678826</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>PAV-M</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4481,7 +5011,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4503,36 +5033,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.422229</v>
+        <v>-58.375684</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.573148</v>
+        <v>-34.656092</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>CON-I</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>7336</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CRAMER AV. 2141</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4542,7 +5082,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4557,7 +5097,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Poste inclinado ingreso tambien como 7201</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4565,7 +5105,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4575,14 +5115,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.461582</v>
+        <v>-58.461024</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.564296</v>
+        <v>-34.539409</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4592,33 +5132,43 @@
       <c r="P55" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>BLO-F</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4633,7 +5183,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4641,7 +5191,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4651,50 +5201,60 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.494864</v>
+        <v>-58.355342</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.678826</v>
+        <v>-34.63565</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>CON-G</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4709,7 +5269,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4717,7 +5277,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4731,46 +5291,56 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.375684</v>
+        <v>-58.472869</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.656092</v>
+        <v>-34.562</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>COG-I</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4785,7 +5355,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4793,7 +5363,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4803,50 +5373,60 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.461024</v>
+        <v>-58.434651</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.539409</v>
+        <v>-34.598814</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>CLI-O</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6917</t>
+          <t>7169</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>9/5/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1375</t>
+          <t>SAN NICOLAS 5045</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808918700</t>
+          <t>809492980</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4861,7 +5441,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Poste quebrado</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4879,50 +5459,60 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.355342</v>
+        <v>-58.515637</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.63565</v>
+        <v>-34.589993</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4959,10 +5549,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.472869</v>
+        <v>-58.458298</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.562</v>
+        <v>-34.566511</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4972,33 +5562,43 @@
       <c r="P60" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>COG-F</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5013,7 +5613,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5031,40 +5631,50 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.434651</v>
+        <v>-58.516218</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.598814</v>
+        <v>-34.589343</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>PUE-J</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5074,7 +5684,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5089,7 +5699,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5107,14 +5717,14 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.515637</v>
+        <v>-58.520505</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.589993</v>
+        <v>-34.596045</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5124,33 +5734,43 @@
       <c r="P62" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>PUE-O</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5183,50 +5803,60 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.458298</v>
+        <v>-58.481316</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.566511</v>
+        <v>-34.556157</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>COG-O</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5241,7 +5871,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5249,7 +5879,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5259,50 +5889,60 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.516218</v>
+        <v>-58.409278</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.589343</v>
+        <v>-34.653566</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>PPT-H</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5317,7 +5957,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5335,50 +5975,60 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.520505</v>
+        <v>-58.399262</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.596045</v>
+        <v>-34.639685</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>PPT-K</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>-602</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/18/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>Agustin de vedia 2111</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809837501</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5411,50 +6061,60 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.481316</v>
+        <v>-58.435637</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.556157</v>
+        <v>-34.64435</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>PPT-O</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>-604</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/22/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>Gurruchaga 2126</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809929884</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5469,7 +6129,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Columna cortada sostenida por la red</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5477,7 +6137,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5487,50 +6147,60 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.409278</v>
+        <v>-58.424217</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.653566</v>
+        <v>-34.586032</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>VCR-O</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5545,7 +6215,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5558,7 +6228,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -5567,46 +6237,56 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.399262</v>
+        <v>-58.447743</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.639685</v>
+        <v>-34.570457</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>COG-C</t>
+        </is>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-602</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>9/18/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Agustin de vedia 2111</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809837501</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5621,7 +6301,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5643,46 +6323,56 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.435637</v>
+        <v>-58.452532</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.64435</v>
+        <v>-34.609005</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>NRA-H</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-604</t>
+          <t>7296</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9/22/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Gurruchaga 2126</t>
+          <t>VEDIA, AGUSTIN DE 2130</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809929884</t>
+          <t>809979719</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5697,7 +6387,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Columna cortada sostenida por la red</t>
+          <t xml:space="preserve">3 columnas picadas ver en calle cuales son necesarias cambiar con Pablo </t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5719,46 +6409,56 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.424217</v>
+        <v>-58.435634</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.586032</v>
+        <v>-34.64412</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>PPT-O</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5773,7 +6473,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5786,7 +6486,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5795,46 +6495,56 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.447743</v>
+        <v>-58.485454</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.570457</v>
+        <v>-34.555745</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>COG-O</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5849,7 +6559,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5867,50 +6577,60 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.452532</v>
+        <v>-58.509324</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.609005</v>
+        <v>-34.635335</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>DEV-M</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7296</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2130</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809979719</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5925,7 +6645,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 columnas picadas ver en calle cuales son necesarias cambiar con Pablo </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5947,46 +6667,56 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.435634</v>
+        <v>-58.501431</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.64412</v>
+        <v>-34.647791</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>PAV-?</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>7359</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>9/29/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>VEGA, NICETO, CNEL. 4678</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>810056579</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6001,7 +6731,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada con base corroida</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6023,46 +6753,56 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.485454</v>
+        <v>-58.430056</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.555745</v>
+        <v>-34.593188</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>VCR-F</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6817,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6095,40 +6835,50 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.509324</v>
+        <v>-58.384406</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.635335</v>
+        <v>-34.622932</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>CON-M</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6138,7 +6888,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6153,7 +6903,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6175,10 +6925,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.501431</v>
+        <v>-58.521719</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.647791</v>
+        <v>-34.647467</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6188,33 +6938,43 @@
       <c r="P76" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>PAV-C</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7359</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/29/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>VEGA, NICETO, CNEL. 4678</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>810056579</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6229,7 +6989,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6251,26 +7011,36 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.430056</v>
+        <v>-58.461482</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.593188</v>
+        <v>-34.632432</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>PCH-F</t>
+        </is>
+      </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7402</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6280,17 +7050,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>RIVADAVIA AV. 2479</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>810132836</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6305,7 +7075,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6327,26 +7097,36 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.384406</v>
+        <v>-58.401428</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.622932</v>
+        <v>-34.609797</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>CLI-D</t>
+        </is>
+      </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7405</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6356,17 +7136,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>CHILE 2115</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132907</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6381,7 +7161,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6403,46 +7183,56 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.521719</v>
+        <v>-58.396368</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.647467</v>
+        <v>-34.61718</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>CEN-C</t>
+        </is>
+      </c>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7410</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>CHILE 2163</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132956</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6479,14 +7269,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.461482</v>
+        <v>-58.397024</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.632432</v>
+        <v>-34.617234</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6494,232 +7284,14 @@
           <t>Capital Sur</t>
         </is>
       </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>7402</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>10/2/2025</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>RIVADAVIA AV. 2479</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>810132836</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>picada</t>
-        </is>
-      </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M81" t="n">
-        <v>-58.401428</v>
-      </c>
-      <c r="N81" t="n">
-        <v>-34.609797</v>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>7405</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>10/2/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>CHILE 2115</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>810132907</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>-58.396368</v>
-      </c>
-      <c r="N82" t="n">
-        <v>-34.61718</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>7410</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>10/1/2025</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>CHILE 2163</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>810132956</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I83" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M83" t="n">
-        <v>-58.397024</v>
-      </c>
-      <c r="N83" t="n">
-        <v>-34.617234</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P83" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>CEN-C</t>
+        </is>
+      </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-13 07:27:20)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R79"/>
+  <dimension ref="A1:R76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5750,7 +5750,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5760,7 +5760,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5770,7 +5770,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5793,7 +5793,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5803,14 +5803,14 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.409278</v>
+        <v>-58.399262</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.653566</v>
+        <v>-34.639685</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5824,7 +5824,7 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -5836,27 +5836,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>-604</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/22/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>Gurruchaga 2126</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809929884</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5871,7 +5871,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>Columna cortada sostenida por la red</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5893,14 +5893,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.399262</v>
+        <v>-58.424217</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.639685</v>
+        <v>-34.586032</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5910,7 +5910,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>VCR-O</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -5922,27 +5922,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-602</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>9/18/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Agustin de vedia 2111</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809837501</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5957,7 +5957,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L65" t="inlineStr">
@@ -5979,24 +5979,24 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.435637</v>
+        <v>-58.447743</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.64435</v>
+        <v>-34.570457</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>PPT-O</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -6008,27 +6008,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-604</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>9/22/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Gurruchaga 2126</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809929884</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6043,7 +6043,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Columna cortada sostenida por la red</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -6065,24 +6065,24 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.424217</v>
+        <v>-58.452532</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.586032</v>
+        <v>-34.609005</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>VCR-O</t>
+          <t>NRA-H</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -6094,27 +6094,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6129,7 +6129,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -6142,7 +6142,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -6151,14 +6151,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.447743</v>
+        <v>-58.485454</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.570457</v>
+        <v>-34.555745</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -6168,7 +6168,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6180,27 +6180,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6215,7 +6215,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -6233,18 +6233,18 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.452532</v>
+        <v>-58.509324</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.609005</v>
+        <v>-34.635335</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -6254,39 +6254,39 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>NRA-H</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7296</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>VEDIA, AGUSTIN DE 2130</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809979719</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 columnas picadas ver en calle cuales son necesarias cambiar con Pablo </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -6323,24 +6323,24 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.435634</v>
+        <v>-58.501431</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.64412</v>
+        <v>-34.647791</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>PPT-O</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6352,27 +6352,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>7359</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>9/29/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>VEGA, NICETO, CNEL. 4678</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>810056579</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6387,7 +6387,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada con base corroida</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -6409,24 +6409,24 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.485454</v>
+        <v>-58.430056</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.555745</v>
+        <v>-34.593188</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>VCR-F</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -6438,27 +6438,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6473,7 +6473,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -6491,50 +6491,50 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.509324</v>
+        <v>-58.384406</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.635335</v>
+        <v>-34.622932</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -6544,7 +6544,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6559,7 +6559,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -6581,10 +6581,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.501431</v>
+        <v>-58.521719</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.647791</v>
+        <v>-34.647467</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -6598,7 +6598,7 @@
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -6610,27 +6610,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7359</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9/29/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>VEGA, NICETO, CNEL. 4678</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>810056579</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6645,7 +6645,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -6667,14 +6667,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.430056</v>
+        <v>-58.461482</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.593188</v>
+        <v>-34.632432</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -6684,7 +6684,7 @@
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>VCR-F</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
@@ -6696,7 +6696,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7402</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -6706,17 +6706,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>RIVADAVIA AV. 2479</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>810132836</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6731,7 +6731,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6753,14 +6753,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.384406</v>
+        <v>-58.401428</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.622932</v>
+        <v>-34.609797</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6770,7 +6770,7 @@
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>CLI-D</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -6782,7 +6782,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7405</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6792,17 +6792,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>CHILE 2115</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132907</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6817,7 +6817,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6839,24 +6839,24 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.521719</v>
+        <v>-58.396368</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.647467</v>
+        <v>-34.61718</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>CEN-C</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -6868,27 +6868,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7410</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>CHILE 2163</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132956</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6925,14 +6925,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.461482</v>
+        <v>-58.397024</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.632432</v>
+        <v>-34.617234</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6942,268 +6942,10 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>CEN-C</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>7402</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>10/2/2025</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>RIVADAVIA AV. 2479</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>810132836</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>picada</t>
-        </is>
-      </c>
-      <c r="I77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M77" t="n">
-        <v>-58.401428</v>
-      </c>
-      <c r="N77" t="n">
-        <v>-34.609797</v>
-      </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P77" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>CLI-D</t>
-        </is>
-      </c>
-      <c r="R77" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>7405</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>10/2/2025</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>CHILE 2115</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>810132907</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I78" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M78" t="n">
-        <v>-58.396368</v>
-      </c>
-      <c r="N78" t="n">
-        <v>-34.61718</v>
-      </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P78" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>CEN-C</t>
-        </is>
-      </c>
-      <c r="R78" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>7410</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>10/1/2025</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>CHILE 2163</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>810132956</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M79" t="n">
-        <v>-58.397024</v>
-      </c>
-      <c r="N79" t="n">
-        <v>-34.617234</v>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P79" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>CEN-C</t>
-        </is>
-      </c>
-      <c r="R79" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-17 20:17:21)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AYKO" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AYKO" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-20 07:30:34)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3522,27 +3522,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-604</t>
+          <t>6465</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>9/22/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Gurruchaga 2126</t>
+          <t>AGUIRRE 368</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>809929884</t>
+          <t>809268249</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3557,7 +3557,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna cortada sostenida por la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3579,27 +3579,199 @@
         </is>
       </c>
       <c r="M37" t="n">
+        <v>-58.434651</v>
+      </c>
+      <c r="N37" t="n">
+        <v>-34.598814</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>CLI-O</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>-604</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>9/22/2025</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Gurruchaga 2126</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>809929884</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Columna cortada sostenida por la red</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
         <v>-58.424217</v>
       </c>
-      <c r="N37" t="n">
+      <c r="N38" t="n">
         <v>-34.586032</v>
       </c>
-      <c r="O37" t="inlineStr">
+      <c r="O38" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr">
+      <c r="P38" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q37" t="inlineStr">
+      <c r="Q38" t="inlineStr">
         <is>
           <t>VCR-O</t>
         </is>
       </c>
-      <c r="R37" t="inlineStr">
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>7359</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>9/29/2025</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>VEGA, NICETO, CNEL. 4678</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>810056579</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>AYKO</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Columna inclinada con base corroida</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>-58.430056</v>
+      </c>
+      <c r="N39" t="n">
+        <v>-34.593188</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>VCR-F</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-20 14:47:05)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3350,27 +3350,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3403,375 +3403,31 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.417348</v>
+        <v>-58.484729</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.595467</v>
+        <v>-34.574614</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>VCR-B</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>-488</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Blanco Encalada 4896</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>807763099</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
-        </is>
-      </c>
-      <c r="I36" t="n">
-        <v>1</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M36" t="n">
-        <v>-58.484729</v>
-      </c>
-      <c r="N36" t="n">
-        <v>-34.574614</v>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P36" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>ATH-C</t>
-        </is>
-      </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>6465</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>8/28/2025</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>AGUIRRE 368</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>809268249</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I37" t="n">
-        <v>1</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L37" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M37" t="n">
-        <v>-58.434651</v>
-      </c>
-      <c r="N37" t="n">
-        <v>-34.598814</v>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>CLI-O</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>-604</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>9/22/2025</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Gurruchaga 2126</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>809929884</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Columna cortada sostenida por la red</t>
-        </is>
-      </c>
-      <c r="I38" t="n">
-        <v>1</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M38" t="n">
-        <v>-58.424217</v>
-      </c>
-      <c r="N38" t="n">
-        <v>-34.586032</v>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P38" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>VCR-O</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>7359</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>9/29/2025</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>VEGA, NICETO, CNEL. 4678</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>810056579</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Columna inclinada con base corroida</t>
-        </is>
-      </c>
-      <c r="I39" t="n">
-        <v>1</v>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M39" t="n">
-        <v>-58.430056</v>
-      </c>
-      <c r="N39" t="n">
-        <v>-34.593188</v>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P39" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>VCR-F</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-23 08:09:41)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-3</t>
+          <t>-152</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1/5/2024</t>
+          <t>11/1/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FIGUEROA ALCORTA PTE ,AV. /ALT/ 5600</t>
+          <t>FERNANDEZ DE ENCISO /ALT/ 3610</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>777580740</t>
+          <t>798984311</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Es F. ALCORTA 5600 (pasando Av de los ombues 100mts aprox.) Para cambiar es un poste con muchas rajaduras, en Figueroa Alcorta esq. Av de los Ombues</t>
+          <t>El poste esta pegado al arbol ver la foto adjunta</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -585,56 +585,56 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.425911</v>
+        <v>-58.513363</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.56033</v>
+        <v>-34.605473</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>BLO-?</t>
+          <t>DEV-F</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1DEV</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-10</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1/15/2024</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DARWIN /ALT/ 651</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>777863458</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,13 +647,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aplomar columna 114  </t>
+        </is>
+      </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -667,10 +671,10 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.44467</v>
+        <v>-58.498493</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.593784</v>
+        <v>-34.581262</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -684,39 +688,39 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>VCR-I</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-103</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6/12/2024</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SALGUERO JERONIMO /ALT/ 2533</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>788206681</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -731,7 +735,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Altura correcta 2549</t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -753,24 +757,24 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.409971</v>
+        <v>-58.502447</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.58175</v>
+        <v>-34.561008</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>AGU-O</t>
+          <t>PUE-H</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -782,27 +786,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-118</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/15/2024</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SUCRE MRCAL A J DE /ALT/ 1437</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>793333193</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,7 +821,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Retirar columna vieja, nodo ya traspasado</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -830,23 +834,23 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.445523</v>
+        <v>-58.503673</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.558237</v>
+        <v>-34.586925</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -856,39 +860,39 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>BLO-A</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-143</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/7/2024</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>797752816</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -898,21 +902,25 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
+        </is>
+      </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -921,14 +929,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.458864</v>
+        <v>-58.504455</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.561167</v>
+        <v>-34.579941</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -938,7 +946,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-152</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11/1/2024</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>FERNANDEZ DE ENCISO /ALT/ 3610</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>798984311</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,7 +993,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>El poste esta pegado al arbol ver la foto adjunta</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -993,7 +1001,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1003,18 +1011,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.513363</v>
+        <v>-58.503195</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.605473</v>
+        <v>-34.581735</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1024,39 +1032,39 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>DEV-F</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1DEV</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-160</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11/1/2024</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MORAN PEDRO /ALT/ 3100</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>798984905</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1069,13 +1077,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Aplomar columna de 114 - VIRARDI</t>
+        </is>
+      </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1085,18 +1097,18 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.498724</v>
+        <v>-58.493164</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.594329</v>
+        <v>-34.55732</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1106,7 +1118,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PUE-G</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1118,27 +1130,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-201</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1007</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>799540497</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1153,7 +1165,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1171,28 +1183,28 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.436377</v>
+        <v>-58.491934</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.565075</v>
+        <v>-34.569348</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>PUE-F</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1204,27 +1216,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-202</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1030</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>799540503</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1239,7 +1251,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Recambio de columna - alt correcta 1010</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1247,7 +1259,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1257,28 +1269,28 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.436601</v>
+        <v>-58.501418</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.565035</v>
+        <v>-34.574363</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>PUE-I</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1290,27 +1302,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-216</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5/2/2024</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>784655947</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1325,15 +1337,15 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1343,28 +1355,28 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.404652</v>
+        <v>-58.470837</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.58263</v>
+        <v>-34.545751</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>COG-?</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1376,27 +1388,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-219</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10/31/2024</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LA PAMPA /ALT/ 2836</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>798953875</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1411,11 +1423,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1429,18 +1441,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.458282</v>
+        <v>-58.484729</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.56718</v>
+        <v>-34.574614</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1450,7 +1462,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1462,27 +1474,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-118</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>8/15/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>SUCRE MRCAL A J DE /ALT/ 1437</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>793333193</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1497,11 +1509,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna vieja, nodo ya traspasado</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1510,7 +1522,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1519,24 +1531,24 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.421964</v>
+        <v>-58.445523</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.586342</v>
+        <v>-34.558237</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>VCR-O</t>
+          <t>BLO-A</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1548,27 +1560,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-143</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>10/7/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>797752816</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1578,25 +1590,21 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1605,14 +1613,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.498493</v>
+        <v>-58.458864</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.581262</v>
+        <v>-34.561167</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1622,39 +1630,39 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>COG-H</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-219</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>10/31/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>LA PAMPA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>798953875</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1669,7 +1677,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1691,14 +1699,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.502447</v>
+        <v>-58.458282</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.561008</v>
+        <v>-34.56718</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1708,7 +1716,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-H</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1720,27 +1728,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1755,11 +1763,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1773,18 +1781,18 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.483947</v>
+        <v>-58.465608</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.583207</v>
+        <v>-34.538489</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1794,7 +1802,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ATH-S</t>
+          <t>BLO-?</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1806,27 +1814,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1836,16 +1844,16 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1854,23 +1862,23 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.503673</v>
+        <v>-58.451835</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.586925</v>
+        <v>-34.562646</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1880,39 +1888,39 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>BLO-N</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1927,15 +1935,15 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1949,14 +1957,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.504455</v>
+        <v>-58.464144</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.579941</v>
+        <v>-34.541832</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1966,7 +1974,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1978,27 +1986,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2013,15 +2021,15 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2031,18 +2039,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.503195</v>
+        <v>-58.464177</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.581735</v>
+        <v>-34.558239</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2052,39 +2060,39 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>COG-K</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>1/5/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>FIGUEROA ALCORTA PTE ,AV. /ALT/ 5600</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>777580740</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2099,7 +2107,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Es F. ALCORTA 5600 (pasando Av de los ombues 100mts aprox.) Para cambiar es un poste con muchas rajaduras, en Figueroa Alcorta esq. Av de los Ombues</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2107,7 +2115,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2117,28 +2125,28 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.493164</v>
+        <v>-58.425911</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.55732</v>
+        <v>-34.56033</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>BLO-?</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2150,27 +2158,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-103</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>6/12/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>SALGUERO JERONIMO /ALT/ 2533</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>788206681</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2185,7 +2193,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Altura correcta 2549</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2207,24 +2215,24 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.491934</v>
+        <v>-58.409971</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.569348</v>
+        <v>-34.58175</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PUE-F</t>
+          <t>AGU-O</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2236,27 +2244,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-201</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>MIGUELETES /ALT/ 1007</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>799540497</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2271,7 +2279,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2279,7 +2287,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2289,28 +2297,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.501418</v>
+        <v>-58.436377</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.574363</v>
+        <v>-34.565075</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PUE-I</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2322,27 +2330,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-202</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>MIGUELETES /ALT/ 1030</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>799540503</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2357,15 +2365,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Recambio de columna - alt correcta 1010</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2379,24 +2387,24 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.465608</v>
+        <v>-58.436601</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.538489</v>
+        <v>-34.565035</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>BLO-?</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2408,27 +2416,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-216</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>5/2/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>784655947</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2443,11 +2451,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2465,24 +2473,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.436788</v>
+        <v>-58.404652</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.604014</v>
+        <v>-34.58263</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>ALM-N</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2494,27 +2502,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2529,7 +2537,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2537,7 +2545,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2551,14 +2559,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.439461</v>
+        <v>-58.421964</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.605744</v>
+        <v>-34.586342</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2568,7 +2576,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>ALM-O</t>
+          <t>VCR-O</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2580,27 +2588,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2613,17 +2621,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
-        </is>
-      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="n">
         <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2637,24 +2641,24 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.473936</v>
+        <v>-58.405761</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.577346</v>
+        <v>-34.582476</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>ATH-J</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2666,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2723,14 +2727,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.387847</v>
+        <v>-58.432241</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.587043</v>
+        <v>-34.56642</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2740,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>RET-A</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2752,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-10</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>1/15/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>DARWIN /ALT/ 651</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>777863458</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2782,16 +2786,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
-        </is>
-      </c>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2800,7 +2800,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2809,14 +2809,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.451835</v>
+        <v>-58.44467</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.562646</v>
+        <v>-34.593784</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>BLO-N</t>
+          <t>VCR-I</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2838,27 +2838,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-160</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>11/1/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>MORAN PEDRO /ALT/ 3100</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>798984905</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2871,17 +2871,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
-        </is>
-      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2891,18 +2887,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.470837</v>
+        <v>-58.498724</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.545751</v>
+        <v>-34.594329</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2912,7 +2908,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>COG-?</t>
+          <t>PUE-G</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2924,27 +2920,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2959,15 +2955,15 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2981,14 +2977,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.464144</v>
+        <v>-58.483947</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.541832</v>
+        <v>-34.583207</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2998,7 +2994,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>ATH-S</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3010,27 +3006,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3045,7 +3041,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3063,18 +3059,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.464177</v>
+        <v>-58.436788</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.558239</v>
+        <v>-34.604014</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3084,7 +3080,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>COG-K</t>
+          <t>ALM-N</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3096,27 +3092,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3131,7 +3127,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3139,7 +3135,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3153,24 +3149,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.412302</v>
+        <v>-58.473936</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.59301</v>
+        <v>-34.577346</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>AGU-C</t>
+          <t>ATH-J</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3182,27 +3178,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3215,7 +3211,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I33" t="n">
         <v>1</v>
       </c>
@@ -3235,10 +3235,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.405761</v>
+        <v>-58.387847</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.582476</v>
+        <v>-34.587043</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>RET-A</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3264,27 +3264,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3321,14 +3321,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.432241</v>
+        <v>-58.412302</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.56642</v>
+        <v>-34.59301</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>AGU-C</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3350,27 +3350,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3403,28 +3403,28 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.484729</v>
+        <v>-58.439461</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.574614</v>
+        <v>-34.605744</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>ATH-C</t>
+          <t>ALM-O</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-24 15:35:12)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-152</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11/1/2024</t>
+          <t>1/5/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FERNANDEZ DE ENCISO /ALT/ 3610</t>
+          <t>FIGUEROA ALCORTA PTE ,AV. /ALT/ 5600</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>798984311</t>
+          <t>777580740</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>El poste esta pegado al arbol ver la foto adjunta</t>
+          <t>Es F. ALCORTA 5600 (pasando Av de los ombues 100mts aprox.) Para cambiar es un poste con muchas rajaduras, en Figueroa Alcorta esq. Av de los Ombues</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -585,56 +585,56 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.513363</v>
+        <v>-58.425911</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.605473</v>
+        <v>-34.56033</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>DEV-F</t>
+          <t>BLO-?</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>1/15/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>DARWIN /ALT/ 651</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>777863458</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,17 +647,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -671,10 +667,10 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.498493</v>
+        <v>-58.44467</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.581262</v>
+        <v>-34.593784</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -688,39 +684,39 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>VCR-I</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-103</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>6/12/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>SALGUERO JERONIMO /ALT/ 2533</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>788206681</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -735,7 +731,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t>Altura correcta 2549</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -757,24 +753,24 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.502447</v>
+        <v>-58.409971</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.561008</v>
+        <v>-34.58175</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>PUE-H</t>
+          <t>AGU-O</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -786,27 +782,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-118</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>8/15/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>SUCRE MRCAL A J DE /ALT/ 1437</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>793333193</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -821,7 +817,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Retirar columna vieja, nodo ya traspasado</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -834,23 +830,23 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.503673</v>
+        <v>-58.445523</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.586925</v>
+        <v>-34.558237</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -860,39 +856,39 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>BLO-A</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-143</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>10/7/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>797752816</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -902,25 +898,21 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -929,14 +921,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.504455</v>
+        <v>-58.458864</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.579941</v>
+        <v>-34.561167</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -946,7 +938,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-H</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +950,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-152</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>11/1/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>FERNANDEZ DE ENCISO /ALT/ 3610</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>798984311</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -993,7 +985,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>El poste esta pegado al arbol ver la foto adjunta</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -1001,7 +993,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1011,18 +1003,18 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.503195</v>
+        <v>-58.513363</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.581735</v>
+        <v>-34.605473</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1032,39 +1024,39 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>DEV-F</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>ARATO-25058.PO.1DEV</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-160</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>11/1/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>MORAN PEDRO /ALT/ 3100</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>798984905</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1077,17 +1069,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
-        </is>
-      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1097,18 +1085,18 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.493164</v>
+        <v>-58.498724</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.55732</v>
+        <v>-34.594329</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1118,7 +1106,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>PUE-G</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1130,27 +1118,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-201</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>MIGUELETES /ALT/ 1007</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>799540497</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1165,7 +1153,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1183,28 +1171,28 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.491934</v>
+        <v>-58.436377</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.569348</v>
+        <v>-34.565075</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>PUE-F</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1216,27 +1204,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-202</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>MIGUELETES /ALT/ 1030</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>799540503</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1251,7 +1239,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Recambio de columna - alt correcta 1010</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1259,7 +1247,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1269,28 +1257,28 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.501418</v>
+        <v>-58.436601</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.574363</v>
+        <v>-34.565035</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>PUE-I</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1302,27 +1290,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-216</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/2/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>784655947</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1337,15 +1325,15 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1355,28 +1343,28 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.470837</v>
+        <v>-58.404652</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.545751</v>
+        <v>-34.58263</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>COG-?</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1388,27 +1376,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-488</t>
+          <t>-219</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>10/31/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Blanco Encalada 4896</t>
+          <t>LA PAMPA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>807763099</t>
+          <t>798953875</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1423,11 +1411,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
+          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1441,18 +1429,18 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.484729</v>
+        <v>-58.458282</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.574614</v>
+        <v>-34.56718</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1462,7 +1450,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>ATH-C</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1474,27 +1462,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-118</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8/15/2024</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SUCRE MRCAL A J DE /ALT/ 1437</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>793333193</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1509,11 +1497,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Retirar columna vieja, nodo ya traspasado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1522,7 +1510,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1531,24 +1519,24 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.445523</v>
+        <v>-58.421964</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.558237</v>
+        <v>-34.586342</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-A</t>
+          <t>VCR-O</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1560,27 +1548,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-143</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10/7/2024</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>797752816</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1590,21 +1578,25 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aplomar columna 114  </t>
+        </is>
+      </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1613,14 +1605,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.458864</v>
+        <v>-58.498493</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.561167</v>
+        <v>-34.581262</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1630,39 +1622,39 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-219</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10/31/2024</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LA PAMPA /ALT/ 2836</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>798953875</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1677,7 +1669,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1699,14 +1691,14 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.458282</v>
+        <v>-58.502447</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.56718</v>
+        <v>-34.561008</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -1716,7 +1708,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>PUE-H</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1728,27 +1720,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,11 +1755,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1781,18 +1773,18 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.465608</v>
+        <v>-58.483947</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.538489</v>
+        <v>-34.583207</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1802,7 +1794,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>BLO-?</t>
+          <t>ATH-S</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1814,27 +1806,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1844,16 +1836,16 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1862,23 +1854,23 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.451835</v>
+        <v>-58.503673</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.562646</v>
+        <v>-34.586925</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1888,39 +1880,39 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>BLO-N</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,15 +1927,15 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1957,14 +1949,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.464144</v>
+        <v>-58.504455</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.541832</v>
+        <v>-34.579941</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1974,7 +1966,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1986,27 +1978,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2021,15 +2013,15 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2039,18 +2031,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.464177</v>
+        <v>-58.503195</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.558239</v>
+        <v>-34.581735</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2060,39 +2052,39 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>COG-K</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-3</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1/5/2024</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>FIGUEROA ALCORTA PTE ,AV. /ALT/ 5600</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>777580740</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2107,7 +2099,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Es F. ALCORTA 5600 (pasando Av de los ombues 100mts aprox.) Para cambiar es un poste con muchas rajaduras, en Figueroa Alcorta esq. Av de los Ombues</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2115,7 +2107,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2125,28 +2117,28 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.425911</v>
+        <v>-58.493164</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.56033</v>
+        <v>-34.55732</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>BLO-?</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2158,27 +2150,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-103</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6/12/2024</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SALGUERO JERONIMO /ALT/ 2533</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>788206681</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2193,7 +2185,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Altura correcta 2549</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2215,24 +2207,24 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.409971</v>
+        <v>-58.491934</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.58175</v>
+        <v>-34.569348</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>AGU-O</t>
+          <t>PUE-F</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2244,27 +2236,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-201</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1007</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>799540497</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2279,7 +2271,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2287,7 +2279,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2297,28 +2289,28 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.436377</v>
+        <v>-58.501418</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.565075</v>
+        <v>-34.574363</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>PUE-I</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2330,27 +2322,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-202</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1030</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>799540503</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2365,15 +2357,15 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Recambio de columna - alt correcta 1010</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2387,24 +2379,24 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.436601</v>
+        <v>-58.465608</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.565035</v>
+        <v>-34.538489</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>BLO-?</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2416,27 +2408,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-216</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5/2/2024</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>784655947</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2451,11 +2443,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2473,24 +2465,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.404652</v>
+        <v>-58.436788</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.58263</v>
+        <v>-34.604014</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>ALM-N</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2502,27 +2494,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2537,7 +2529,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2545,7 +2537,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2559,14 +2551,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.421964</v>
+        <v>-58.439461</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.586342</v>
+        <v>-34.605744</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2576,7 +2568,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>VCR-O</t>
+          <t>ALM-O</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2588,27 +2580,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2621,13 +2613,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+        </is>
+      </c>
       <c r="I26" t="n">
         <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2641,24 +2637,24 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.405761</v>
+        <v>-58.473936</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.582476</v>
+        <v>-34.577346</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>ATH-J</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2666,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2727,14 +2723,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.432241</v>
+        <v>-58.387847</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.56642</v>
+        <v>-34.587043</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2740,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>BLO-I</t>
+          <t>RET-A</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2752,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-10</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1/15/2024</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>DARWIN /ALT/ 651</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>777863458</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2786,12 +2782,16 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+        </is>
+      </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2800,7 +2800,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2809,14 +2809,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.44467</v>
+        <v>-58.451835</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.593784</v>
+        <v>-34.562646</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>VCR-I</t>
+          <t>BLO-N</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2838,27 +2838,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-160</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11/1/2024</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MORAN PEDRO /ALT/ 3100</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>798984905</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2871,13 +2871,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+        </is>
+      </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2887,18 +2891,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.498724</v>
+        <v>-58.470837</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.594329</v>
+        <v>-34.545751</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2908,7 +2912,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PUE-G</t>
+          <t>COG-?</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2920,27 +2924,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2955,15 +2959,15 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2977,14 +2981,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.483947</v>
+        <v>-58.464144</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.583207</v>
+        <v>-34.541832</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2994,7 +2998,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>ATH-S</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3006,27 +3010,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3041,7 +3045,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3059,18 +3063,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.436788</v>
+        <v>-58.464177</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.604014</v>
+        <v>-34.558239</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3080,7 +3084,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>ALM-N</t>
+          <t>COG-K</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3092,27 +3096,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3127,7 +3131,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3135,7 +3139,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3149,24 +3153,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.473936</v>
+        <v>-58.412302</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.577346</v>
+        <v>-34.59301</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>ATH-J</t>
+          <t>AGU-C</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3178,27 +3182,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3211,11 +3215,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
         <v>1</v>
       </c>
@@ -3235,10 +3235,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.387847</v>
+        <v>-58.405761</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.587043</v>
+        <v>-34.582476</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -3252,7 +3252,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>RET-A</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3264,27 +3264,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3321,14 +3321,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.412302</v>
+        <v>-58.432241</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.59301</v>
+        <v>-34.56642</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>AGU-C</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3350,27 +3350,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3403,28 +3403,28 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.439461</v>
+        <v>-58.484729</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.605744</v>
+        <v>-34.574614</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>ALM-O</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-06 10:01:34)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AYKO" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AYKO" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-06 10:38:17)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>-3</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1/5/2024</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FIGUEROA ALCORTA PTE ,AV. /ALT/ 5600</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>777580740</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -563,11 +563,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Es F. ALCORTA 5600 (pasando Av de los ombues 100mts aprox.) Para cambiar es un poste con muchas rajaduras, en Figueroa Alcorta esq. Av de los Ombues</t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -585,24 +585,24 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.425911</v>
+        <v>-58.484729</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.56033</v>
+        <v>-34.574614</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>BLO-?</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>-10</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1/15/2024</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DARWIN /ALT/ 651</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>777863458</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -647,9 +647,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -667,24 +671,24 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.44467</v>
+        <v>-58.432241</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.593784</v>
+        <v>-34.56642</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>VCR-I</t>
+          <t>BLO-I</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -696,17 +700,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-103</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6/12/2024</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SALGUERO JERONIMO /ALT/ 2533</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -716,7 +720,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>788206681</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -729,13 +733,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Altura correcta 2549</t>
-        </is>
-      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -753,14 +753,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.409971</v>
+        <v>-58.405761</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.58175</v>
+        <v>-34.582476</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>AGU-O</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -782,17 +782,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>-118</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/15/2024</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SUCRE MRCAL A J DE /ALT/ 1437</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>793333193</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,11 +817,11 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Retirar columna vieja, nodo ya traspasado</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -830,7 +830,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -839,10 +839,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.445523</v>
+        <v>-58.464144</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.558237</v>
+        <v>-34.541832</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -856,7 +856,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>BLO-A</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -868,17 +868,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-143</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/7/2024</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 2261</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>797752816</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -898,12 +898,16 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+        </is>
+      </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -912,19 +916,19 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.458864</v>
+        <v>-58.464177</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.561167</v>
+        <v>-34.558239</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -938,7 +942,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>COG-K</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -950,27 +954,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>-152</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11/1/2024</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>FERNANDEZ DE ENCISO /ALT/ 3610</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>798984311</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -985,11 +989,11 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>El poste esta pegado al arbol ver la foto adjunta</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -1003,60 +1007,60 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.513363</v>
+        <v>-58.412302</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.605473</v>
+        <v>-34.59301</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>DEV-F</t>
+          <t>AGU-C</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-160</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11/1/2024</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MORAN PEDRO /ALT/ 3100</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>798984905</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1069,13 +1073,17 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+        </is>
+      </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1085,18 +1093,18 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.498724</v>
+        <v>-58.470837</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.594329</v>
+        <v>-34.545751</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1106,7 +1114,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PUE-G</t>
+          <t>COG-?</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1118,27 +1126,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-201</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1007</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>799540497</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1153,11 +1161,11 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -1171,18 +1179,18 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.436377</v>
+        <v>-58.387847</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.565075</v>
+        <v>-34.587043</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1192,7 +1200,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>RET-A</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1204,27 +1212,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-202</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MIGUELETES /ALT/ 1030</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>799540503</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1239,15 +1247,15 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Recambio de columna - alt correcta 1010</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1257,28 +1265,28 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.436601</v>
+        <v>-58.473936</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.565035</v>
+        <v>-34.577346</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>BLO-J</t>
+          <t>ATH-J</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1290,27 +1298,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-216</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5/2/2024</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>784655947</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1325,11 +1333,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1347,24 +1355,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.404652</v>
+        <v>-58.436788</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.58263</v>
+        <v>-34.604014</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>ALM-N</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1376,27 +1384,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-219</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10/31/2024</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LA PAMPA /ALT/ 2836</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>798953875</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1411,15 +1419,15 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1433,24 +1441,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.458282</v>
+        <v>-58.439461</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.56718</v>
+        <v>-34.605744</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>ALM-O</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1462,27 +1470,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1497,7 +1505,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1505,7 +1513,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1515,28 +1523,28 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.421964</v>
+        <v>-58.465608</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.586342</v>
+        <v>-34.538489</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>VCR-O</t>
+          <t>BLO-?</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1548,7 +1556,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1558,17 +1566,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1583,7 +1591,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1591,7 +1599,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1605,46 +1613,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.498493</v>
+        <v>-58.421964</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.581262</v>
+        <v>-34.586342</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>VCR-O</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1654,7 +1662,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1669,15 +1677,15 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1691,10 +1699,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.502447</v>
+        <v>-58.498493</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.561008</v>
+        <v>-34.581262</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1708,19 +1716,19 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-H</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1730,17 +1738,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1755,7 +1763,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1763,7 +1771,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1777,10 +1785,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.483947</v>
+        <v>-58.502447</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.583207</v>
+        <v>-34.561008</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1794,7 +1802,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ATH-S</t>
+          <t>PUE-H</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1806,7 +1814,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1816,17 +1824,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1841,7 +1849,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1849,7 +1857,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1859,14 +1867,14 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.503673</v>
+        <v>-58.483947</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.586925</v>
+        <v>-34.583207</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1880,19 +1888,19 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>ATH-S</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1902,7 +1910,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1912,7 +1920,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1927,7 +1935,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1935,7 +1943,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1945,14 +1953,14 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.504455</v>
+        <v>-58.503673</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.579941</v>
+        <v>-34.586925</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1966,19 +1974,19 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1988,7 +1996,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1998,7 +2006,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2013,7 +2021,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -2035,10 +2043,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.503195</v>
+        <v>-58.504455</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.581735</v>
+        <v>-34.579941</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -2052,19 +2060,19 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2074,7 +2082,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2084,7 +2092,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2099,7 +2107,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2121,14 +2129,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.493164</v>
+        <v>-58.503195</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.55732</v>
+        <v>-34.581735</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2138,19 +2146,19 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>COG-A</t>
+          <t>PUE-M</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2160,7 +2168,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2170,7 +2178,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2185,7 +2193,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2193,7 +2201,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2207,14 +2215,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.491934</v>
+        <v>-58.493164</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.569348</v>
+        <v>-34.55732</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2224,7 +2232,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PUE-F</t>
+          <t>COG-A</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2236,7 +2244,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2246,7 +2254,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2256,7 +2264,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2271,7 +2279,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2279,7 +2287,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2293,10 +2301,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.501418</v>
+        <v>-58.491934</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.574363</v>
+        <v>-34.569348</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2310,7 +2318,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PUE-I</t>
+          <t>PUE-F</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2322,27 +2330,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2357,11 +2365,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2375,18 +2383,18 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.465608</v>
+        <v>-58.501418</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.538489</v>
+        <v>-34.574363</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2396,7 +2404,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>BLO-?</t>
+          <t>PUE-I</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2408,27 +2416,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-152</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>11/1/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>FERNANDEZ DE ENCISO /ALT/ 3610</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>798984311</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2443,11 +2451,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t>El poste esta pegado al arbol ver la foto adjunta</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2461,18 +2469,18 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.436788</v>
+        <v>-58.513363</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.604014</v>
+        <v>-34.605473</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2482,39 +2490,39 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>ALM-N</t>
+          <t>DEV-F</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1DEV</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-160</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>11/1/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>MORAN PEDRO /ALT/ 3100</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>798984905</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2527,17 +2535,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
-        </is>
-      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2547,28 +2551,28 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.439461</v>
+        <v>-58.498724</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.605744</v>
+        <v>-34.594329</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>ALM-O</t>
+          <t>PUE-G</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2580,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-219</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>10/31/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>LA PAMPA /ALT/ 2836</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>798953875</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2615,15 +2619,15 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Colocar Columna entre 2836/2838 ver con inspector la viabilidad</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2637,10 +2641,10 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.473936</v>
+        <v>-58.458282</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.577346</v>
+        <v>-34.56718</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -2654,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>ATH-J</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2666,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-118</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>8/15/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>SUCRE MRCAL A J DE /ALT/ 1437</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>793333193</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2701,11 +2705,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna vieja, nodo ya traspasado</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2714,7 +2718,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2723,24 +2727,24 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.387847</v>
+        <v>-58.445523</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.587043</v>
+        <v>-34.558237</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>RET-A</t>
+          <t>BLO-A</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2752,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-103</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>6/12/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>SALGUERO JERONIMO /ALT/ 2533</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>788206681</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2782,16 +2786,16 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Altura correcta 2549</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2800,7 +2804,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2809,24 +2813,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.451835</v>
+        <v>-58.409971</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.562646</v>
+        <v>-34.58175</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>BLO-N</t>
+          <t>AGU-O</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2838,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-216</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/2/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>ORTIZ DE OCAMPO ,AV. /ALT/ 2635</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>784655947</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2873,15 +2877,15 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2891,28 +2895,28 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.470837</v>
+        <v>-58.404652</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.545751</v>
+        <v>-34.58263</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>COG-?</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2924,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-10</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>1/15/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>DARWIN /ALT/ 651</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>777863458</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2957,13 +2961,9 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
-        </is>
-      </c>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2981,14 +2981,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.464144</v>
+        <v>-58.44467</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.541832</v>
+        <v>-34.593784</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2998,7 +2998,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>VCR-I</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3010,27 +3010,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>1/5/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>FIGUEROA ALCORTA PTE ,AV. /ALT/ 5600</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>777580740</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3045,11 +3045,11 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>Es F. ALCORTA 5600 (pasando Av de los ombues 100mts aprox.) Para cambiar es un poste con muchas rajaduras, en Figueroa Alcorta esq. Av de los Ombues</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3067,24 +3067,24 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.464177</v>
+        <v>-58.425911</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.558239</v>
+        <v>-34.56033</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>COG-K</t>
+          <t>BLO-?</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3096,27 +3096,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>-201</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>MIGUELETES /ALT/ 1007</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>799540497</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3131,11 +3131,11 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>reemplazo de columnas en mal estado Migueletes 1007 reemplazar columna 114 y colocar rienda a pique</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -3149,18 +3149,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.412302</v>
+        <v>-58.436377</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.59301</v>
+        <v>-34.565075</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>AGU-C</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3182,17 +3182,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>-202</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>MIGUELETES /ALT/ 1030</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -3202,7 +3202,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>799540503</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3215,9 +3215,13 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Recambio de columna - alt correcta 1010</t>
+        </is>
+      </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3231,18 +3235,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.405761</v>
+        <v>-58.436601</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.582476</v>
+        <v>-34.565035</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3252,182 +3256,10 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>BLO-J</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>-486</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>6/23/2025</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Del Libertador 4596</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>807762871</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
-        <v>1</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M34" t="n">
-        <v>-58.432241</v>
-      </c>
-      <c r="N34" t="n">
-        <v>-34.56642</v>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P34" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>BLO-I</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>-488</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Blanco Encalada 4896</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>807763099</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
-        </is>
-      </c>
-      <c r="I35" t="n">
-        <v>1</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M35" t="n">
-        <v>-58.484729</v>
-      </c>
-      <c r="N35" t="n">
-        <v>-34.574614</v>
-      </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P35" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>ATH-C</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-06 10:47:08)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1040,7 +1040,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1050,17 +1050,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1070,12 +1070,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1083,28 +1083,28 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.470837</v>
+        <v>-58.451835</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.545751</v>
+        <v>-34.562646</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>COG-?</t>
+          <t>BLO-N</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1126,27 +1126,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1179,28 +1179,28 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.387847</v>
+        <v>-58.470837</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.587043</v>
+        <v>-34.545751</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>RET-A</t>
+          <t>COG-?</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1212,27 +1212,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1269,24 +1269,24 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.473936</v>
+        <v>-58.387847</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.577346</v>
+        <v>-34.587043</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>ATH-J</t>
+          <t>RET-A</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1298,17 +1298,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1355,14 +1355,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.436788</v>
+        <v>-58.473936</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.604014</v>
+        <v>-34.577346</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>ALM-N</t>
+          <t>ATH-J</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1384,7 +1384,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1394,17 +1394,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1441,24 +1441,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.439461</v>
+        <v>-58.436788</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.605744</v>
+        <v>-34.604014</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>ALM-O</t>
+          <t>ALM-N</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1470,27 +1470,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1523,28 +1523,28 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.465608</v>
+        <v>-58.439461</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.538489</v>
+        <v>-34.605744</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>BLO-?</t>
+          <t>ALM-O</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1556,27 +1556,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1609,28 +1609,28 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.421964</v>
+        <v>-58.465608</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.586342</v>
+        <v>-34.538489</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>VCR-O</t>
+          <t>BLO-?</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1642,7 +1642,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1652,17 +1652,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1699,46 +1699,46 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.498493</v>
+        <v>-58.421964</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.581262</v>
+        <v>-34.586342</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-M</t>
+          <t>VCR-O</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
